<commit_message>
win10 rev0.2(release for preview at IMC)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46A51C7-D793-44A8-875C-8C05151A96D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BFEDB6-4D03-4CEF-A41C-CF3CD4FD4CF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40680" yWindow="90" windowWidth="13575" windowHeight="9645" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40680" yWindow="90" windowWidth="13575" windowHeight="9645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="237">
   <si>
     <t>header1</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>win10-0-01.svg</t>
-  </si>
-  <si>
-    <t>win10-0-02.svg</t>
   </si>
   <si>
     <t>win10-0-03.svg</t>
@@ -736,17 +733,6 @@
  広島大学 情報メディア教育研究センター&lt;br&gt;
  広島大学 消費生活協同組合 
  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">必携PC初期講習会では、みなさんのパソコンを広島大学のキャンパスで使用するための準備をおこないます。本日おこなうことを以下にあげます。おおむね90分くらいかかると思います。頑張ってください。
-  </t>
-    <rPh sb="73" eb="74">
-      <t>フンクライ</t>
-    </rPh>
-    <rPh sb="86" eb="88">
-      <t>ガンバッテ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1121,6 +1107,11 @@
   </si>
   <si>
     <t>win10-5-04a.jpg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">必携PC初期講習会では、みなさんのパソコンを広島大学のキャンパスで使用するための準備をおこないます。本日おこなうことを以下にあげます。おおむね90分くらいかかると思います。頑張ってください。
+  </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1548,7 +1539,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1580,7 +1571,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -1588,7 +1579,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1602,7 +1593,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>174</v>
+        <v>236</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1614,6 +1605,7 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1621,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="19.5" x14ac:dyDescent="0.2"/>
@@ -1663,7 +1655,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
@@ -1671,7 +1663,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>5</v>
@@ -1699,35 +1691,32 @@
         <v>5</v>
       </c>
       <c r="B8" t="s" ph="1">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>11</v>
       </c>
-      <c r="D8" t="s" ph="1">
-        <v>13</v>
-      </c>
     </row>
     <row r="9" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="B9" t="s" ph="1">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" t="s" ph="1">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1735,13 +1724,13 @@
         <v>5</v>
       </c>
       <c r="B11" t="s" ph="1">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1749,21 +1738,21 @@
         <v>5</v>
       </c>
       <c r="B12" t="s" ph="1">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" t="s" ph="1">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1771,13 +1760,13 @@
         <v>5</v>
       </c>
       <c r="B14" t="s" ph="1">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1785,13 +1774,13 @@
         <v>5</v>
       </c>
       <c r="B15" t="s" ph="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1799,21 +1788,21 @@
         <v>5</v>
       </c>
       <c r="B16" t="s" ph="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" t="s" ph="1">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1821,13 +1810,13 @@
         <v>5</v>
       </c>
       <c r="B18" t="s" ph="1">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1835,21 +1824,21 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s" ph="1">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" t="s" ph="1">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1857,13 +1846,13 @@
         <v>5</v>
       </c>
       <c r="B21" t="s" ph="1">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1871,13 +1860,13 @@
         <v>5</v>
       </c>
       <c r="B22" t="s" ph="1">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1885,13 +1874,13 @@
         <v>5</v>
       </c>
       <c r="B23" t="s" ph="1">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -1922,7 +1911,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1930,7 +1919,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1946,7 +1935,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -1954,7 +1943,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1968,13 +1957,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
         <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="195" x14ac:dyDescent="0.2">
@@ -1982,13 +1971,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -1996,13 +1985,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -2010,21 +1999,21 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -2038,13 +2027,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2052,13 +2041,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2066,13 +2055,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2080,13 +2069,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
         <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2099,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2116,7 +2105,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2124,7 +2113,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2140,7 +2129,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2148,7 +2137,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2162,13 +2151,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2176,13 +2165,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>69</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2190,13 +2179,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>71</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2204,13 +2193,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>73</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2218,13 +2207,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>75</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2232,21 +2221,21 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2254,21 +2243,21 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -2282,13 +2271,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2319,7 +2308,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2327,7 +2316,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2343,7 +2332,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="130" x14ac:dyDescent="0.2">
@@ -2351,7 +2340,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2362,7 +2351,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="182" x14ac:dyDescent="0.2">
@@ -2370,7 +2359,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -2381,7 +2370,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2389,13 +2378,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2403,13 +2392,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>47</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2417,13 +2406,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>49</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2431,13 +2420,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2445,18 +2434,18 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
         <v>52</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2464,13 +2453,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2478,13 +2467,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2492,13 +2481,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2506,18 +2495,18 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2525,13 +2514,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2539,13 +2528,13 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2559,8 +2548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="B1" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2576,7 +2565,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2584,7 +2573,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2600,7 +2589,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -2608,7 +2597,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2619,7 +2608,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2627,13 +2616,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>87</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2641,13 +2630,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>89</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2655,13 +2644,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2669,13 +2658,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2683,18 +2672,18 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>92</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2702,13 +2691,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2716,13 +2705,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2730,13 +2719,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
         <v>96</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2744,13 +2733,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2758,13 +2747,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2772,18 +2761,18 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2791,13 +2780,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
         <v>100</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2805,13 +2794,13 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2819,13 +2808,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2833,7 +2822,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -2844,13 +2833,13 @@
         <v>5</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2858,13 +2847,13 @@
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2894,7 +2883,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2902,7 +2891,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2918,7 +2907,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -2926,7 +2915,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2937,7 +2926,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2959,13 +2948,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>107</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2973,18 +2962,18 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>109</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3006,13 +2995,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>112</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3020,13 +3009,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
         <v>114</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3034,7 +3023,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -3048,13 +3037,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" t="s">
         <v>117</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>118</v>
-      </c>
-      <c r="D16" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3062,13 +3051,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" t="s">
         <v>120</v>
-      </c>
-      <c r="C17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3076,13 +3065,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
         <v>122</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3090,13 +3079,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
         <v>124</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3104,18 +3093,18 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
         <v>126</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -3137,13 +3126,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
         <v>129</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3151,13 +3140,13 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
         <v>131</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3165,18 +3154,18 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
         <v>133</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -3198,13 +3187,13 @@
         <v>5</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
         <v>136</v>
-      </c>
-      <c r="C28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3212,13 +3201,13 @@
         <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
         <v>138</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3226,13 +3215,13 @@
         <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
         <v>140</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3240,13 +3229,13 @@
         <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
         <v>142</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -3254,13 +3243,13 @@
         <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
         <v>144</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3268,13 +3257,13 @@
         <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3282,13 +3271,13 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
         <v>147</v>
-      </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3296,13 +3285,13 @@
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
         <v>149</v>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3310,13 +3299,13 @@
         <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
         <v>151</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3324,13 +3313,13 @@
         <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
         <v>153</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="169" x14ac:dyDescent="0.2">
@@ -3338,18 +3327,18 @@
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
         <v>155</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3357,7 +3346,7 @@
         <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -3371,13 +3360,13 @@
         <v>5</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C41" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3385,13 +3374,13 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C42" t="s">
         <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3399,13 +3388,13 @@
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3413,13 +3402,13 @@
         <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C44" t="s">
         <v>11</v>
       </c>
       <c r="D44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -3449,7 +3438,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3465,7 +3454,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3473,7 +3462,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -3484,12 +3473,12 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="208" x14ac:dyDescent="0.2">
@@ -3497,7 +3486,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
rev.1.21 win10 Office offline install fixed
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BFEDB6-4D03-4CEF-A41C-CF3CD4FD4CF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB7E04D-4089-475D-A615-C07F89064C28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40680" yWindow="90" windowWidth="13575" windowHeight="9645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26880" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
     <sheet name="ch0" sheetId="2" r:id="rId2"/>
     <sheet name="ch1" sheetId="3" r:id="rId3"/>
-    <sheet name="ch2" sheetId="5" r:id="rId4"/>
-    <sheet name="ch3" sheetId="4" r:id="rId5"/>
+    <sheet name="ch2" sheetId="4" r:id="rId4"/>
+    <sheet name="ch3" sheetId="5" r:id="rId5"/>
     <sheet name="ch4" sheetId="6" r:id="rId6"/>
     <sheet name="ch5" sheetId="7" r:id="rId7"/>
     <sheet name="ch6" sheetId="8" r:id="rId8"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="239">
   <si>
     <t>header1</t>
   </si>
@@ -123,12 +123,6 @@
 &lt;li&gt; バッテリー駆動時間 &lt;/li&gt;
 &lt;/ol&gt;
  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">まず、OSのバージョンを確認しましょう。画面左下のウィンドウアイコン を右クリックします。
-&lt;p class="spl"&gt;※「右クリック」はマウスの右ボタンをクリックする操作ですが、Surfaceにはマウスがついていません。その代わりに、タッチパッドの右下のあたりをタップするか、もしくは、画面を長くタップします。もしくは、ペンの側面ボタンを押しながら、ペン先で画面タップでも可。&lt;/p&gt;
-メニューが表示されるので、「システム」を探してクリックしてください。
-   </t>
   </si>
   <si>
     <t>win10-1-01.svg</t>
@@ -993,9 +987,6 @@
   </t>
   </si>
   <si>
-    <t>数分待つと、Windows10のデスクトップ画面が出てきます。Microsoft Teamsのアカウント入力が画面に出ますが、とりあえず左上の×マークをクリックして画面から消しましょう。</t>
-  </si>
-  <si>
     <t xml:space="preserve">Surfaceの電源を初めて入れて、デスクトップ画面が表示されるまでの設定内容について説明します。一番重要なのは、普段利用するユーザ名とパスワードを作成するところ。あとは概ね言われるままにしていけば大丈夫です。
 すでにデスクトップが表示されている方は、この章をスキップして次の「パソコンのスペック確認」へ進んでください。
  </t>
@@ -1008,11 +999,6 @@
   </si>
   <si>
     <t>ネットワークに接続した時点で、「Windowsをよりいっそう活用できるようになります」という画面が出ることがあります。これは初期設定のときにスキップした設定をするところですが、ここでは左下の「今はスキップ」をクリックしてください。ここで行う設定は後でできます。</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chromeのインストールはあっという間に終わります。自動的にChromeが起動して初期設定を行うよう促してきますが、ここでは左上の×をクリックして閉じてください。
-&lt;p class="spl"&gt;※ Windows10にはEdgeというWebブラウザが標準的なものとして付属してきますが、うまく表示できないWebページがときどきあります。そういうときに、「もう一つのブラウザ」としてこのChromeを使ってみてください。&lt;/p&gt;
-  </t>
   </si>
   <si>
     <t xml:space="preserve">自動アップデートのタイミング以外にDefenderを更新する方法について説明します。Windowsの自動更新機能で、Defenderは最新状態にたもたれます。しかし、緊急の脆弱性が発表された場合など、すぐに更新した方が良い時もあります。
@@ -1112,6 +1098,69 @@
   <si>
     <t xml:space="preserve">必携PC初期講習会では、みなさんのパソコンを広島大学のキャンパスで使用するための準備をおこないます。本日おこなうことを以下にあげます。おおむね90分くらいかかると思います。頑張ってください。
   </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Chromeのインストールはあっという間に終わります。自動的にChromeが起動して初期設定を行うよう促してきますが、ここでは右上の×をクリックして閉じてください。
+&lt;p class="spl"&gt;※ Windows10にはEdgeというWebブラウザが標準的なものとして付属してきますが、うまく表示できないWebページがときどきあります。そういうときに、「もう一つのブラウザ」としてこのChromeを使ってみてください。&lt;/p&gt;
+  </t>
+    <rPh sb="63" eb="65">
+      <t>ミギウエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>数分待つと、Windows10のデスクトップ画面が出てきます。Microsoft Teamsのアカウント入力が画面に出ますが、とりあえず右上の×マークをクリックして画面から消しましょう。</t>
+    <rPh sb="68" eb="69">
+      <t>ミギ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-0-13a.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">まず、OSのバージョンを確認しましょう。画面左下のウィンドウアイコン を右クリックします。
+&lt;p class="spl"&gt;※「右クリック」はマウスの右ボタンをクリックする操作ですが、Surfaceにはマウスがついていません。その代わりに、タッチパッドの右下のあたりをタップするか、もしくは、画面を長くタップします。もしくは、ペンの側面ボタンを押しながら、ペン先で画面タップでも可。&lt;/p&gt;
+メニューが表示されるので、「システム」を探してクリックしてください。
+   </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Microsoft Teams について。最近のWindows10パソコンでは、サインイン時にMicrosoft Teams が自動的に起動します。これはMicrosoftが提供しているグループチャットアプリで、広大アカウントでサインインして使うことができます。詳細はメディアセンターWebサイトの&lt;a href="https://www.media.hiroshima-u.ac.jp/services/communication/teams/"&gt;「Microsft Teams」&lt;/a&gt;で。また、使わない場合は画面左下のウィンドウアイコンから「設定」→「アプリ」→「スタートアップ」と進んでTeamsのスイッチを「オフ」にすると、自動起動を止めることができます。</t>
+    <rPh sb="21" eb="23">
+      <t>サイキン</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="64" eb="67">
+      <t>ジドウテキ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="106" eb="108">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="121" eb="122">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="131" eb="133">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="250" eb="251">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="254" eb="256">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="294" eb="295">
+      <t>スス</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1571,7 +1620,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -1579,7 +1628,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1593,7 +1642,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1613,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="19.5" x14ac:dyDescent="0.2"/>
@@ -1655,7 +1704,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
@@ -1663,7 +1712,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>5</v>
@@ -1672,11 +1721,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s" ph="1">
+      <c r="B7" s="1" t="s" ph="1">
         <v>10</v>
       </c>
       <c r="C7" t="s" ph="1">
@@ -1686,23 +1735,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B8" t="s" ph="1">
-        <v>202</v>
+      <c r="B8" s="1" t="s" ph="1">
+        <v>201</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B9" t="s" ph="1">
-        <v>203</v>
+      <c r="B9" s="1" t="s" ph="1">
+        <v>202</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>11</v>
@@ -1711,20 +1760,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B10" t="s" ph="1">
+    <row r="10" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s" ph="1">
+        <v>203</v>
+      </c>
+      <c r="D10" t="s" ph="1">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s" ph="1">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s" ph="1">
         <v>204</v>
-      </c>
-      <c r="D10" t="s" ph="1">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s" ph="1">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s" ph="1">
-        <v>205</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>11</v>
@@ -1733,12 +1782,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B12" t="s" ph="1">
-        <v>206</v>
+      <c r="B12" s="1" t="s" ph="1">
+        <v>205</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>11</v>
@@ -1747,33 +1796,33 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B13" t="s" ph="1">
+    <row r="13" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s" ph="1">
+        <v>206</v>
+      </c>
+      <c r="D13" t="s" ph="1">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s" ph="1">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s" ph="1">
         <v>207</v>
-      </c>
-      <c r="D13" t="s" ph="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s" ph="1">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s" ph="1">
-        <v>208</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B15" t="s" ph="1">
+      <c r="B15" s="1" t="s" ph="1">
         <v>16</v>
       </c>
       <c r="C15" t="s" ph="1">
@@ -1783,11 +1832,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B16" t="s" ph="1">
+      <c r="B16" s="1" t="s" ph="1">
         <v>18</v>
       </c>
       <c r="C16" t="s" ph="1">
@@ -1798,25 +1847,25 @@
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B17" t="s" ph="1">
+      <c r="B17" s="1" t="s" ph="1">
+        <v>208</v>
+      </c>
+      <c r="D17" t="s" ph="1">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s" ph="1">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s" ph="1">
         <v>209</v>
-      </c>
-      <c r="D17" t="s" ph="1">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s" ph="1">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s" ph="1">
-        <v>210</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1824,7 +1873,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s" ph="1">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>11</v>
@@ -1833,34 +1882,34 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B20" t="s" ph="1">
-        <v>201</v>
+    <row r="20" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s" ph="1">
+        <v>200</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B21" t="s" ph="1">
-        <v>211</v>
+      <c r="B21" s="1" t="s" ph="1">
+        <v>210</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="136.5" ph="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B22" t="s" ph="1">
-        <v>212</v>
+      <c r="B22" s="1" t="s" ph="1">
+        <v>211</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>11</v>
@@ -1869,18 +1918,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B23" t="s" ph="1">
-        <v>213</v>
+      <c r="B23" s="1" t="s" ph="1">
+        <v>235</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -1894,8 +1943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1935,7 +1984,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -1957,13 +2006,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
         <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="195" x14ac:dyDescent="0.2">
@@ -1971,13 +2020,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -1985,13 +2034,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -1999,21 +2048,21 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -2027,13 +2076,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>32</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2041,13 +2090,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2055,13 +2104,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2069,13 +2118,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
         <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2085,11 +2134,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A7" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2105,7 +2154,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2113,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2129,155 +2178,209 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="130" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="182" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="117" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="91" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="65" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="91" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="78" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>216</v>
-      </c>
-      <c r="D13" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="65" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="143" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" t="s">
-        <v>81</v>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2288,11 +2391,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2308,7 +2411,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2316,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2332,15 +2435,15 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="130" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2349,192 +2452,138 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="117" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="182" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>182</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="65" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
+        <v>214</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="143" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>181</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s">
-        <v>217</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2548,8 +2597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A19" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2565,7 +2614,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2573,7 +2622,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2589,7 +2638,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -2597,7 +2646,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2608,7 +2657,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2616,13 +2665,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>86</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2630,13 +2679,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>88</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2644,13 +2693,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2658,13 +2707,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2672,18 +2721,18 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>91</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2691,13 +2740,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2705,13 +2754,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2719,13 +2768,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
         <v>95</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2733,13 +2782,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2747,13 +2796,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2761,18 +2810,18 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2780,66 +2829,66 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
         <v>99</v>
       </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>101</v>
+      <c r="C25" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2847,13 +2896,13 @@
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2864,10 +2913,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2883,7 +2932,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2891,7 +2940,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2907,7 +2956,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -2915,7 +2964,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2926,7 +2975,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2948,13 +2997,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>106</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2962,18 +3011,18 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>108</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2995,13 +3044,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
         <v>111</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3009,13 +3058,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
         <v>113</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3023,7 +3072,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -3037,13 +3086,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" t="s">
         <v>116</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>117</v>
-      </c>
-      <c r="D16" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3051,13 +3100,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" t="s">
         <v>119</v>
-      </c>
-      <c r="C17" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3065,13 +3114,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
         <v>121</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3079,13 +3128,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
         <v>123</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3093,18 +3142,18 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
         <v>125</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -3126,13 +3175,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
         <v>128</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3140,13 +3189,13 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
         <v>130</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3154,18 +3203,18 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
         <v>132</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -3187,13 +3236,13 @@
         <v>5</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
         <v>135</v>
-      </c>
-      <c r="C28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3201,13 +3250,13 @@
         <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
         <v>137</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3215,13 +3264,13 @@
         <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
         <v>139</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3229,13 +3278,13 @@
         <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
         <v>141</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -3243,13 +3292,13 @@
         <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
         <v>143</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3257,13 +3306,13 @@
         <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3271,13 +3320,13 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
         <v>146</v>
-      </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3285,13 +3334,13 @@
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
         <v>148</v>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3299,13 +3348,13 @@
         <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
         <v>150</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3313,13 +3362,13 @@
         <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
         <v>152</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="169" x14ac:dyDescent="0.2">
@@ -3327,18 +3376,18 @@
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
         <v>154</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3346,7 +3395,7 @@
         <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -3360,13 +3409,13 @@
         <v>5</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C41" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3374,13 +3423,13 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
         <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3388,27 +3437,35 @@
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
       </c>
       <c r="D43" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="97.5" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s" ph="1">
+        <v>238</v>
+      </c>
+      <c r="D44" t="s" ph="1">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="91" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="C45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" t="s">
         <v>162</v>
-      </c>
-      <c r="C44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -3438,7 +3495,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3454,7 +3511,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3462,7 +3519,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -3473,12 +3530,12 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="208" x14ac:dyDescent="0.2">
@@ -3486,7 +3543,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
rev0.34 2-06a change to png (what's wrong in svg conveert?)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB342B8-7DAB-4C89-BB40-F068E26F56A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0A1F3A-3527-41BD-9A0A-FA94B35A4D4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27480" yWindow="2115" windowWidth="13500" windowHeight="8265" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1234,7 +1234,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win10-2-06a.svg</t>
+    <t>win10-2-06a.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2212,7 +2212,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B10" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
rev0.4 win10 pics fix(printer etc.)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0A1F3A-3527-41BD-9A0A-FA94B35A4D4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10ADC65-4EA2-4F55-A420-0940D4AAF665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27480" yWindow="2115" windowWidth="13500" windowHeight="8265" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30285" yWindow="570" windowWidth="14625" windowHeight="10140" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="242">
   <si>
     <t>header1</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>win10-0-10.svg</t>
-  </si>
-  <si>
-    <t>win10-0-12.svg</t>
   </si>
   <si>
     <t xml:space="preserve">自分のパソコンの基本的なスペックを確認しておきましょう。CPUの型式、OSのビット数、記憶容量など。 </t>
@@ -206,18 +203,10 @@
     <t>win10-2-03.svg</t>
   </si>
   <si>
-    <t xml:space="preserve">コピーが終わったらUSBメモリを取り外します。ウィンドウ左の「FIRST LEC (D:)」を右クリックして、「取り出し」をクリックします。
-  </t>
-  </si>
-  <si>
     <t>&lt;h2&gt;&lt;a name="office"&gt;&lt;/a&gt;Officeを入れる&lt;/h2&gt;</t>
   </si>
   <si>
     <t>win10-2-07.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">「すぐに完了します」などと出ますが、なかなか終わりません。気長に待ちましょう。10分くらいかかります。
-  </t>
   </si>
   <si>
     <t>win10-2-08.svg</t>
@@ -308,16 +297,6 @@
     <t xml:space="preserve">&lt;div class="panel-heading"&gt;&lt;span class="glyphicon glyphicon-warning-sign"&gt;&lt;/span&gt;
 パスワードを変更したら...&lt;/div&gt;
 &lt;div class="panel-body" style="padding:10px"&gt;この章の一番最初に「一度設定したら次回からは（同じエリアでは）設定不要です」などと書かれていますが、パスワードを変更した場合には再設定が必要になります。 &lt;/div&gt;
-  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">この章の設定をすると、今後は毎回アカウント名とパスワードを入れなくてもHINET Wi-Fiに接続できます。これは、入力されたものをWindowsが保存して、あなたの代わりに毎回送ってるからですね。
-ということは、パスワードを変更すると保存していたものでは繋がらなくなってしまいます。その際、「パスワードが違います」などという警告が出るわけでもなく、ただ無言で繋がらなくなりますので、メディアセンタに「突然繋がらなくなりました。壊れたんですか」って聞きに来る人も多いです。
-パスワードを変更をした場合は、以下のようにしてHINET Wi-Fiを再設定してください。
-&lt;ol&gt;&lt;li&gt;タスクバーのWi-Fiアイコンをクリック &lt;/li&gt;
-&lt;li&gt;&amp;quot;HU-CUPXX&amp;quot; で右クリック→削除。これを全てのHU-CUPXXで行います。 &lt;/li&gt;
-&lt;li&gt;すると、HU-CUPXXが未接続状態でまた表示されますので、この章でやったようにまた設定 &lt;/li&gt;
-&lt;/ol&gt;
   </t>
   </si>
   <si>
@@ -401,9 +380,6 @@
   </si>
   <si>
     <t>win10-5-12.svg</t>
-  </si>
-  <si>
-    <t>win10-5-13.svg</t>
   </si>
   <si>
     <t>win10-5-17.svg</t>
@@ -632,9 +608,6 @@
   <si>
     <t xml:space="preserve">以降は補足情報であり、講習会のときに設定しません。後日必要に応じて行ってください。
  </t>
-  </si>
-  <si>
-    <t>win10-6-24.svg</t>
   </si>
   <si>
     <t xml:space="preserve">Bb9を便利に利用できるスマホ用アプリもあります。iOSのApp StoreやAndroidのGoogle Playで&amp;quot;Blackboard&amp;quot;と検索してみてください。
@@ -748,14 +721,6 @@
 OneDriveのアプリは、Web版のOneDrive サイトから入手できます。
 詳細はメディアセンターWebサイトの&lt;a href="https://www.media.hiroshima-u.ac.jp/services/onedriveforbusiness/"&gt;「クラウドファイル保管サービス(OneDrive for Business)」&lt;/a&gt;
 で。
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Microsoft Office365 ProPlus の正規版がすでに入っている場合には、ここを飛ばして&lt;a href="#chrome"&gt;[10]に進んでください&lt;/a&gt;
-。Office2013が入っている場合は、それをそのままにしてOffice 365を追加インストールすることができます。
-デスクトップにコピーした「setup2020-win10」というフォルダをダブルクリックして開きます。さらに中に「officepropluswin-jp」というフォルダがあるので、ダブルクリックして開きます。
-「install」という項目をダブルクリックして実行してください。
   </t>
     <phoneticPr fontId="1"/>
   </si>
@@ -855,23 +820,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">「しばらくお待ちください」と言う旨のメッセージが表示され、処理が完了すると「準備が完了しました！」となります。「完了」をクリックしてください。
-これでOfficeを使用するための準備が完了しました。&lt;span class="check"&gt;check-8&lt;span&gt;&lt;/span&gt;
-&lt;/span&gt;
-以上でこの章の作業は終了です。
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win10-4-11.jpg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-0-11a.jpg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-0-25.jpg</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -959,12 +908,6 @@
     <t xml:space="preserve">システム全体のウイルスチェックを実施する方法を確認します。チェックには時間がかかりますので、講習会の会場では行わないでください。
 システム全体のウイルスチェックを「フルスキャン」と呼びます。それに対して「クイックスキャン」はよく攻撃される場所に限定して調査を行いますので、時間が短くて済みます。
 フルスキャンを行うには「現在の脅威」のところにある「スキャンのオプション」をクリックしましょう。
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">「同意してExcelを開始する」をクリックします。
-※この「同意する」は、ソフトウェアの使用許諾契約に同意することを意味します。
   </t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1235,6 +1178,126 @@
   </si>
   <si>
     <t>win10-2-06a.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Microsoft Office365 ProPlus の正規版がすでに入っている場合には、ここを飛ばして&lt;a href="#chrome"&gt;[10]に進んでください&lt;/a&gt;
+。Office2013が入っている場合は、それをそのままにしてOffice 365 ProPlus を追加インストールすることができます。
+デスクトップにコピーした「setup2020-win10」というフォルダをダブルクリックして開きます。さらに中に「officepropluswin-jp」というフォルダがあるので、ダブルクリックして開きます。
+「install」という項目をダブルクリックして実行してください。
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「すぐに完了します」などと出ますが、なかなか終わりません。気長に待ちましょう。10分くらいかかります。
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">この章の設定をすると、今後は毎回アカウント名とパスワードを入れなくてもHINET Wi-Fiに接続できます。これは、入力されたものをWindowsが保存して、あなたの代わりに毎回送ってるからですね。
+ということは、パスワードを変更すると保存していたものでは繋がらなくなってしまいます。その際、「パスワードが違います」などという警告が出るわけでもなく、ただ無言で繋がらなくなりますので、メディアセンタに「突然繋がらなくなりました。壊れたんですか」って聞きに来る人も多いです。
+パスワードを変更をした場合は、以下のようにしてHINET Wi-Fiを再設定してください。
+&lt;ol&gt;&lt;li&gt;タスクバーのWi-Fiアイコンをクリック &lt;/li&gt;
+&lt;li&gt;&amp;quot;HU-CUPXX&amp;quot; で右クリック→削除。これを全てのHU-CUPXXで行います。 &lt;/li&gt;
+&lt;li&gt;すると、HU-CUPXXが未接続状態でまた表示されますので、この章でやったようにまた設定します。 &lt;/li&gt;
+&lt;/ol&gt;
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-0-02a.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-0-25.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-0-11a.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-0-12.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">コピーが終わったらUSBメモリを取り外します。ウィンドウ左の「FIRST LEC (D:)」を右クリックして、「取り出し」をクリックします。
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「しばらくお待ちください」と言う旨のメッセージが表示され、処理が完了すると「準備が完了しました！」となります。「完了」をクリックしてください。
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「ライセンス契約に同意します」で「同意する」をクリックします。
+※本来は「利用許諾契約書を読む」で契約事項を読んでから同意するものですが、ここではそこまで厳密にはしません。「ファイル」→「アカウント」→「Excelのバージョン情報」と辿ることで、後でも読めます　これでOfficeを使用するための準備が完了しました。&lt;span class="check"&gt;check-8&lt;span&gt;&lt;/span&gt;
+&lt;/span&gt;
+以上でこの章の作業は終了です。</t>
+    <rPh sb="6" eb="8">
+      <t>ケイヤク</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ドウイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ドウイ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ホンライ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>キョダク</t>
+    </rPh>
+    <rPh sb="41" eb="44">
+      <t>ケイヤクショ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>ケイヤク</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ジコウ</t>
+    </rPh>
+    <rPh sb="54" eb="55">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>ドウイ</t>
+    </rPh>
+    <rPh sb="77" eb="79">
+      <t>ゲンミツ</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="117" eb="118">
+      <t>タド</t>
+    </rPh>
+    <rPh sb="123" eb="124">
+      <t>アト</t>
+    </rPh>
+    <rPh sb="126" eb="127">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-5-13a.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-5-22.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-6-24a.svg</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1694,7 +1757,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -1702,7 +1765,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1716,7 +1779,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1736,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="C20" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="19.5" x14ac:dyDescent="0.2"/>
@@ -1778,7 +1841,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
@@ -1786,7 +1849,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>5</v>
@@ -1814,18 +1877,21 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>11</v>
       </c>
+      <c r="D8" t="s" ph="1">
+        <v>232</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s" ph="1">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>11</v>
@@ -1836,10 +1902,10 @@
     </row>
     <row r="10" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s" ph="1">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1847,7 +1913,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s" ph="1">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>11</v>
@@ -1861,21 +1927,21 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s" ph="1">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s" ph="1">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
@@ -1883,13 +1949,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s" ph="1">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
@@ -1922,10 +1988,10 @@
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s" ph="1">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
@@ -1933,13 +1999,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s" ph="1">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1947,7 +2013,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s" ph="1">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>11</v>
@@ -1958,10 +2024,10 @@
     </row>
     <row r="20" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s" ph="1">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>186</v>
+        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1969,13 +2035,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s" ph="1">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>185</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="136.5" ph="1" x14ac:dyDescent="0.2">
@@ -1983,13 +2049,13 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s" ph="1">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>20</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1997,13 +2063,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s" ph="1">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2017,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="C11" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2034,7 +2100,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2042,7 +2108,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2058,7 +2124,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2066,7 +2132,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2080,13 +2146,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="195" x14ac:dyDescent="0.2">
@@ -2094,13 +2160,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2108,13 +2174,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -2122,21 +2188,21 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -2150,13 +2216,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2164,13 +2230,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2178,13 +2244,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2192,13 +2258,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
         <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2211,8 +2277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="B12" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2228,7 +2294,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2236,7 +2302,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2252,7 +2318,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="130" x14ac:dyDescent="0.2">
@@ -2260,7 +2326,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2271,7 +2337,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="182" x14ac:dyDescent="0.2">
@@ -2279,7 +2345,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -2290,7 +2356,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2298,13 +2364,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2312,13 +2378,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>42</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2326,13 +2392,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>44</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2340,13 +2406,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2354,18 +2420,18 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>236</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2373,13 +2439,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>173</v>
+        <v>229</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2387,13 +2453,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2401,13 +2467,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>230</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2415,18 +2481,18 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2434,13 +2500,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2448,13 +2514,13 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2468,8 +2534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="C14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A13" zoomScale="57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2485,7 +2551,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2493,7 +2559,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2509,7 +2575,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2517,7 +2583,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2531,13 +2597,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2545,13 +2611,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2559,13 +2625,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2573,13 +2639,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2587,13 +2653,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2601,21 +2667,21 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="D13" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2623,21 +2689,21 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -2651,13 +2717,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>73</v>
+        <v>231</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2671,8 +2737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="C23" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="C18" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2688,7 +2754,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2696,7 +2762,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2712,7 +2778,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -2720,7 +2786,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2731,7 +2797,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2739,13 +2805,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2753,13 +2819,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2767,13 +2833,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2781,13 +2847,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2795,18 +2861,18 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2814,13 +2880,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2828,13 +2894,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2842,13 +2908,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2856,13 +2922,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2870,13 +2936,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2884,18 +2950,18 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2903,55 +2969,55 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>236</v>
+        <v>196</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>212</v>
+        <v>240</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2959,24 +3025,27 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>208</v>
+        <v>237</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" t="s">
-        <v>95</v>
+      <c r="B26" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2990,8 +3059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView topLeftCell="C44" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3007,7 +3076,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3015,7 +3084,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3031,7 +3100,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -3039,7 +3108,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3050,7 +3119,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3072,13 +3141,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3086,18 +3155,18 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3119,13 +3188,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3133,13 +3202,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3147,7 +3216,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -3161,13 +3230,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C16" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D16" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3175,13 +3244,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D17" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3189,13 +3258,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3203,13 +3272,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3217,18 +3286,18 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -3250,13 +3319,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3264,13 +3333,13 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3278,18 +3347,18 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -3311,13 +3380,13 @@
         <v>5</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3325,13 +3394,13 @@
         <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3339,13 +3408,13 @@
         <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3353,13 +3422,13 @@
         <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -3367,13 +3436,13 @@
         <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3381,13 +3450,13 @@
         <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3395,13 +3464,13 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3409,13 +3478,13 @@
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3423,13 +3492,13 @@
         <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3437,13 +3506,13 @@
         <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="169" x14ac:dyDescent="0.2">
@@ -3451,18 +3520,18 @@
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3470,7 +3539,7 @@
         <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -3484,13 +3553,13 @@
         <v>5</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C41" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>151</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3498,13 +3567,13 @@
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C42" t="s">
         <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3512,21 +3581,21 @@
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3534,13 +3603,13 @@
         <v>5</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C45" t="s">
         <v>11</v>
       </c>
       <c r="D45" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -3570,7 +3639,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3586,7 +3655,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3594,7 +3663,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -3605,17 +3674,17 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="117" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3623,7 +3692,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
rev0.5 write win10e(except ch.0)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1960A15E-7629-42F2-AC3A-EBE49B88925A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273A644E-DA77-4315-A53E-8A8BFD6EEFCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32475" yWindow="0" windowWidth="13500" windowHeight="8265" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36660" yWindow="4710" windowWidth="17370" windowHeight="8265" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -951,43 +951,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Microsoft Teams について。最近のWindows10パソコンでは、サインイン時にMicrosoft Teams が自動的に起動します。これはMicrosoftが提供しているグループチャットアプリで、広大メールアドレスとパスワードでサインインして使うことができます。詳細はメディアセンターWebサイトの&lt;a href="https://www.media.hiroshima-u.ac.jp/services/communication/teams/"&gt;「Microsft Teams」&lt;/a&gt;で。また、使わない場合は画面左下のウィンドウアイコンから「設定」→「アプリ」→「スタートアップ」と進んでTeamsのスイッチを「オフ」にすると、自動起動を止めることができます。</t>
-    <rPh sb="21" eb="23">
-      <t>サイキン</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>トキ</t>
-    </rPh>
-    <rPh sb="64" eb="67">
-      <t>ジドウテキ</t>
-    </rPh>
-    <rPh sb="68" eb="70">
-      <t>キドウ</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>テイキョウ</t>
-    </rPh>
-    <rPh sb="106" eb="108">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="129" eb="130">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="139" eb="141">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="258" eb="259">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="262" eb="264">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="302" eb="303">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve"> &lt;/dl&gt;情報メディア教育研究センターでは、皆さんの必携PCをより活用してもらえるよう、F3S (First Three Steps) 講習会を開催しています。 
 学生生活を送る上で有用なパソコンの使い方について、一つでも多く身につけてもらえるようさまざまな内容を準備していますので、 興味のあるものが見つかったら、ぜひ参加してください。 
 &lt;ul&gt;&lt;li&gt;&lt;a href="https://f3s.riise.hiroshima-u.ac.jp"&gt;https://f3s.riise.hiroshima-u.ac.jp&lt;/a&gt;
@@ -1254,10 +1217,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win10-5-23.jpg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">「このデバイスではどこでもこのアカウントを使用する」と聞かれますので、「はい」と答えます。
 ※ これにより、Wordなどの他のOfficeアプリケーションを起動した時のサインイン作業が不要になります。
   </t>
@@ -1267,8 +1226,12 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>win10-5-23.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>「ライセンス契約に同意します」で「同意する」をクリックします。
-※本来は「利用許諾契約書を読む」で契約事項を読んでから同意するものですが、ここではそこまで厳密にはしません。「ファイル」→「アカウント」→「Excelのバージョン情報」と辿ることで、いつでも読めます。
+※本来は「利用許諾契約書を読む」で契約事項を読んでから同意するものですが、ここではそこまでしません。「ファイル」→「アカウント」→「Excelのバージョン情報」と辿ることで、いつでも読めます。
 これでOfficeを使用するための準備が完了しました。&lt;span class="check"&gt;check-8&lt;span&gt;&lt;/span&gt;
 &lt;/span&gt;
 以上でこの章の作業は終了です。</t>
@@ -1308,17 +1271,53 @@
     <rPh sb="59" eb="61">
       <t>ドウイ</t>
     </rPh>
-    <rPh sb="77" eb="79">
-      <t>ゲンミツ</t>
-    </rPh>
-    <rPh sb="113" eb="115">
+    <rPh sb="109" eb="111">
       <t>ジョウホウ</t>
     </rPh>
-    <rPh sb="117" eb="118">
+    <rPh sb="113" eb="114">
       <t>タド</t>
     </rPh>
-    <rPh sb="127" eb="128">
+    <rPh sb="123" eb="124">
       <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Microsoft Teams について。最近のWindows10パソコンでは、サインイン時にMicrosoft Teams が自動的に起動します。これはMicrosoftが提供しているグループチャットアプリで、広大メールアドレスとパスワードでサインインして使うことができます。
+詳細はメディアセンターWebサイトの&lt;a href="https://www.media.hiroshima-u.ac.jp/services/communication/teams/"&gt;「Microsft Teams」&lt;/a&gt;で。
+また、使わない場合は画面左下のウィンドウアイコンから「設定」→「アプリ」→「スタートアップ」と進んでTeamsのスイッチを「オフ」にすると、自動起動を止めることができます。</t>
+    <rPh sb="21" eb="23">
+      <t>サイキン</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="64" eb="67">
+      <t>ジドウテキ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="106" eb="108">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="129" eb="130">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="140" eb="142">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="260" eb="261">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="264" eb="266">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="304" eb="305">
+      <t>スス</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1821,8 +1820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="19.5" x14ac:dyDescent="0.2"/>
@@ -1905,7 +1904,7 @@
         <v>11</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1924,10 +1923,10 @@
     </row>
     <row r="10" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s" ph="1">
+        <v>212</v>
+      </c>
+      <c r="D10" t="s" ph="1">
         <v>213</v>
-      </c>
-      <c r="D10" t="s" ph="1">
-        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1955,7 +1954,7 @@
         <v>11</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1963,7 +1962,7 @@
         <v>183</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
@@ -1977,7 +1976,7 @@
         <v>11</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
@@ -2049,7 +2048,7 @@
         <v>178</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -2063,7 +2062,7 @@
         <v>11</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="136.5" ph="1" x14ac:dyDescent="0.2">
@@ -2077,7 +2076,7 @@
         <v>11</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -2085,13 +2084,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s" ph="1">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2105,8 +2104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2238,7 +2237,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -2252,7 +2251,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -2299,8 +2298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="B17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2434,7 +2433,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2442,13 +2441,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2461,13 +2460,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2489,7 +2488,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -2556,7 +2555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="57" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2739,7 +2738,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -2759,8 +2758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A24" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2861,7 +2860,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2875,7 +2874,7 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2908,7 +2907,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2922,7 +2921,7 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2964,7 +2963,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2972,13 +2971,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
         <v>221</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -3002,7 +3001,7 @@
     </row>
     <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D22" t="s">
         <v>244</v>
@@ -3013,7 +3012,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -3041,13 +3040,13 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3055,7 +3054,7 @@
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
@@ -3069,13 +3068,13 @@
         <v>5</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3089,8 +3088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="B15" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3243,10 +3242,10 @@
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D15" t="s">
         <v>240</v>
-      </c>
-      <c r="D15" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3254,13 +3253,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3597,7 +3596,7 @@
         <v>11</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3628,9 +3627,9 @@
         <v>147</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="78" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>204</v>
+        <v>246</v>
       </c>
       <c r="D45" t="s" ph="1">
         <v>202</v>
@@ -3660,7 +3659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3717,7 +3716,7 @@
     </row>
     <row r="7" spans="1:4" ht="117" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3730,7 +3729,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
win10e fix pics(captions in En)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273A644E-DA77-4315-A53E-8A8BFD6EEFCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5267DF5-6092-42EF-BFF3-E9E60F1A9D08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36660" yWindow="4710" windowWidth="17370" windowHeight="8265" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41790" yWindow="2685" windowWidth="11580" windowHeight="5505" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -351,16 +351,6 @@
   </si>
   <si>
     <t>&lt;h2&gt;&lt;a name="defender"&gt;&lt;/a&gt;Defenderの手動更新とフルスキャン&lt;/h2&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">「ウイルスと脅威の防止」をクリックしましょう。
-  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Defenderでは、ウイルスやスパイウェアその他の悪意を持つプログラム全般を「脅威」とし、それらを判別するルールを保存したファイルを「脅威の定義」と呼んでいます。
-「ウイルスと脅威の防止の更新」の下に、前回いつ「脅威の定義」が更新されたかが書かれています。&lt;span class="check"&gt;check-6,7&lt;/span&gt;
-脅威の定義を新しくするには「ウイルスと脅威の防止の更新」をクリックします。
-  </t>
   </si>
   <si>
     <t>win10-5-08.svg</t>
@@ -1319,6 +1309,50 @@
     <rPh sb="304" eb="305">
       <t>スス</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「ウイルスと脅威の防止」をクリックしましょう。
+※この部分に黄色のアイコンが出ている場合があります。これはランサムウェアに備えるためのOneDriveへのデータバックアップが設定されていないことを示していますが、この講習会ではまだ設定しません。気になるようでしたら「無視する」をクリックしてください。
+なおデータバックアップ設定はこのメニューからいつでもできます。
+  </t>
+    <rPh sb="27" eb="29">
+      <t>ブブン</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>キイロ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="98" eb="99">
+      <t>シメ</t>
+    </rPh>
+    <rPh sb="108" eb="111">
+      <t>コウシュウカイ</t>
+    </rPh>
+    <rPh sb="115" eb="117">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="122" eb="123">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="133" eb="135">
+      <t>ムシ</t>
+    </rPh>
+    <rPh sb="162" eb="164">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Defenderでは、ウイルスやスパイウェアその他の悪意を持つプログラム全般を「脅威」とし、それらを判別するルールを保存したファイルを「脅威の定義」と呼んでいます。
+「ウイルスと脅威の防止の更新」の下に、前回いつ「脅威の定義」が更新されたかが書かれています。&lt;span class="check"&gt;check-6,7&lt;/span&gt;
+脅威の定義を新しくするには「ウイルスと脅威の防止の更新」をクリックします。
+  </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1778,7 +1812,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -1786,7 +1820,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1800,7 +1834,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1862,7 +1896,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
@@ -1870,7 +1904,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>5</v>
@@ -1898,13 +1932,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1912,7 +1946,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s" ph="1">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>11</v>
@@ -1923,10 +1957,10 @@
     </row>
     <row r="10" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s" ph="1">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1934,7 +1968,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s" ph="1">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>11</v>
@@ -1948,21 +1982,21 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s" ph="1">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s" ph="1">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
@@ -1970,13 +2004,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s" ph="1">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
@@ -2009,10 +2043,10 @@
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s" ph="1">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
@@ -2020,13 +2054,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s" ph="1">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -2034,7 +2068,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s" ph="1">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>11</v>
@@ -2045,10 +2079,10 @@
     </row>
     <row r="20" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s" ph="1">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -2056,13 +2090,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s" ph="1">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="136.5" ph="1" x14ac:dyDescent="0.2">
@@ -2070,13 +2104,13 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s" ph="1">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -2084,13 +2118,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s" ph="1">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2145,7 +2179,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2167,7 +2201,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -2195,7 +2229,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -2209,7 +2243,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -2223,7 +2257,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -2237,7 +2271,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -2251,7 +2285,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -2265,7 +2299,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -2339,7 +2373,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="130" x14ac:dyDescent="0.2">
@@ -2366,7 +2400,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -2427,13 +2461,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2441,13 +2475,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2460,13 +2494,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2474,7 +2508,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -2488,7 +2522,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -2521,7 +2555,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -2535,7 +2569,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -2596,7 +2630,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2688,7 +2722,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -2699,10 +2733,10 @@
     </row>
     <row r="13" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2738,7 +2772,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -2758,8 +2792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:D27"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2799,7 +2833,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -2860,7 +2894,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2868,13 +2902,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2901,27 +2935,27 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>83</v>
+        <v>245</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2929,13 +2963,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>84</v>
+        <v>246</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2943,13 +2977,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2957,13 +2991,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2971,18 +3005,18 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2990,21 +3024,21 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D22" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3012,13 +3046,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3026,13 +3060,13 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3040,13 +3074,13 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3054,13 +3088,13 @@
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3068,13 +3102,13 @@
         <v>5</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -3105,7 +3139,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3113,7 +3147,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3129,7 +3163,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -3137,7 +3171,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3148,7 +3182,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3170,13 +3204,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3184,18 +3218,18 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3217,13 +3251,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3231,21 +3265,21 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D15" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3253,13 +3287,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3267,13 +3301,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" t="s">
         <v>103</v>
-      </c>
-      <c r="C17" t="s">
-        <v>104</v>
-      </c>
-      <c r="D17" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3281,13 +3315,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3295,13 +3329,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C19" t="s">
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3309,13 +3343,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3323,18 +3357,18 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -3356,13 +3390,13 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3370,13 +3404,13 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3384,18 +3418,18 @@
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -3417,13 +3451,13 @@
         <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3431,13 +3465,13 @@
         <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3445,13 +3479,13 @@
         <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3459,13 +3493,13 @@
         <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -3473,13 +3507,13 @@
         <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3487,13 +3521,13 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3501,13 +3535,13 @@
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3515,13 +3549,13 @@
         <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3529,13 +3563,13 @@
         <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3543,13 +3577,13 @@
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="169" x14ac:dyDescent="0.2">
@@ -3557,18 +3591,18 @@
         <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3576,7 +3610,7 @@
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -3590,13 +3624,13 @@
         <v>5</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C42" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3604,13 +3638,13 @@
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3618,21 +3652,21 @@
         <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C44" t="s">
         <v>11</v>
       </c>
       <c r="D44" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3640,13 +3674,13 @@
         <v>5</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C46" t="s">
         <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3659,7 +3693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3676,7 +3710,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3692,7 +3726,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3700,7 +3734,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -3711,17 +3745,17 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="117" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3729,7 +3763,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
rev0.5(3/10 rel.) win10e pic fix
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5267DF5-6092-42EF-BFF3-E9E60F1A9D08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1EAE95-7B9A-444B-AEAD-9FFFEEE8EF4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41790" yWindow="2685" windowWidth="11580" windowHeight="5505" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1970" yWindow="1980" windowWidth="13500" windowHeight="8260" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -521,20 +521,6 @@
   </si>
   <si>
     <t>win10-6-16.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2回目からはログインしたら、この画面が出ます。
-真ん中の「コース一覧」に、あなたがアクセスできるコースが表示されています。
-ここに並んでいるコースは、あなたが受講する授業に関連したものと、そうでないものがあります。今並んでいるものを簡単に説明すると：
-&lt;dl&gt;&lt;dt&gt;大学教育入門&lt;/dt&gt;
-&lt;dd&gt;「大学教育入門」は、大学で学ぶにあたり必要な事柄や、広島大学特有の事情について学習する授業です。全学部生必修です。このコースでは、授業の各週で使う資料をダウンロードしたり、確認テストを受験したりします。&lt;/dd&gt;
-&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
-&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届け」を提出する必要があります。このコースでは、点検届けが提出できます。この講習会のあとで各自開いて実施してください。&lt;/dd&gt;
-&lt;dt&gt;Information Security and Compliance (情報セキュリティ・コンプライアンス)&lt;/dt&gt;
-&lt;dd&gt;「情報セキュリティ・コンプライアンス講習」は、広島大学でパソコンやネットワークを安全に使うための講座です。学生だけでなく、教職員を含めた全構成員必修の内容です。講習は、教室での講義とオンライン学習（このコース）からなっています。6月末までにこのコースの中にある確認テストに合格し、「&lt;em&gt;アカウント利用確認&lt;/em&gt;
-」の手続きをおこなわないと、アカウントがロックされ、メール等が使えなくなります。&lt;/dd&gt;
- &lt;/dl&gt;
-  </t>
   </si>
   <si>
     <t>win10-6-17.svg</t>
@@ -1352,6 +1338,21 @@
     <t xml:space="preserve">Defenderでは、ウイルスやスパイウェアその他の悪意を持つプログラム全般を「脅威」とし、それらを判別するルールを保存したファイルを「脅威の定義」と呼んでいます。
 「ウイルスと脅威の防止の更新」の下に、前回いつ「脅威の定義」が更新されたかが書かれています。&lt;span class="check"&gt;check-6,7&lt;/span&gt;
 脅威の定義を新しくするには「ウイルスと脅威の防止の更新」をクリックします。
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2回目からはログインしたら、この画面が出ます。
+真ん中の「コース一覧」に、あなたがアクセスできるコースが表示されています。
+ここに並んでいるコースは、あなたが受講する授業に関連したものと、そうでないものがあります。今並んでいるものを簡単に説明すると：
+&lt;dl&gt;&lt;dt&gt;大学教育入門&lt;/dt&gt;
+&lt;dd&gt;「大学教育入門」は、大学で学ぶにあたり必要な事柄や、広島大学特有の事情について学習する授業です。全学部生必修です。このコースでは、授業の各週で使う資料をダウンロードしたり、確認テストを受験したりします。&lt;/dd&gt;
+&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
+&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届け」を提出する必要があります。このコースでは、点検届けが提出できます。この講習会のあとで各自開いて実施してください。&lt;/dd&gt;
+&lt;dt&gt;Information Security and Compliance (情報セキュリティ・コンプライアンス)&lt;/dt&gt;
+&lt;dd&gt;「情報セキュリティ・コンプライアンス講習」は、広島大学でパソコンやネットワークを安全に使うための講座です。学生だけでなく、教職員を含めた全構成員必修の内容です。講習は、教室での講義とオンライン学習（このコース）からなっています。6月末までにこのコースの中にある確認テストに合格し、「&lt;em&gt;アカウント利用確認&lt;/em&gt;
+」の手続きをおこなわないと、アカウントがロックされ、メール等が使えなくなります。&lt;/dd&gt;
+ &lt;/dl&gt;
   </t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1812,7 +1813,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -1820,7 +1821,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -1834,7 +1835,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1896,7 +1897,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
@@ -1904,7 +1905,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>5</v>
@@ -1932,13 +1933,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1946,7 +1947,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s" ph="1">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>11</v>
@@ -1957,10 +1958,10 @@
     </row>
     <row r="10" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s" ph="1">
+        <v>209</v>
+      </c>
+      <c r="D10" t="s" ph="1">
         <v>210</v>
-      </c>
-      <c r="D10" t="s" ph="1">
-        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -1968,7 +1969,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s" ph="1">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>11</v>
@@ -1982,21 +1983,21 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s" ph="1">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s" ph="1">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
@@ -2004,13 +2005,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s" ph="1">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
@@ -2043,10 +2044,10 @@
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s" ph="1">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
@@ -2054,13 +2055,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s" ph="1">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -2068,7 +2069,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s" ph="1">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>11</v>
@@ -2079,10 +2080,10 @@
     </row>
     <row r="20" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s" ph="1">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -2090,13 +2091,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s" ph="1">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="136.5" ph="1" x14ac:dyDescent="0.2">
@@ -2104,13 +2105,13 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s" ph="1">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -2118,13 +2119,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s" ph="1">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>11</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2179,7 +2180,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -2201,7 +2202,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -2229,7 +2230,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -2243,7 +2244,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -2257,7 +2258,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -2271,7 +2272,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -2285,7 +2286,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -2299,7 +2300,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -2373,7 +2374,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="130" x14ac:dyDescent="0.2">
@@ -2400,7 +2401,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -2461,13 +2462,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2475,13 +2476,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2494,13 +2495,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -2508,7 +2509,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -2522,7 +2523,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -2555,7 +2556,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -2569,7 +2570,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C22" t="s">
         <v>5</v>
@@ -2630,7 +2631,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2722,7 +2723,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -2733,10 +2734,10 @@
     </row>
     <row r="13" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -2772,7 +2773,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -2792,7 +2793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B16" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -2833,7 +2834,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -2894,7 +2895,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2902,13 +2903,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -2935,13 +2936,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -2949,13 +2950,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -2963,7 +2964,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -2977,7 +2978,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -2991,13 +2992,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C18" t="s">
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3005,13 +3006,13 @@
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
         <v>218</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -3035,10 +3036,10 @@
     </row>
     <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3046,13 +3047,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3060,13 +3061,13 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3074,13 +3075,13 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C25" t="s">
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3088,7 +3089,7 @@
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
@@ -3102,13 +3103,13 @@
         <v>5</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -3122,8 +3123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3163,7 +3164,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -3171,7 +3172,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3276,10 +3277,10 @@
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D15" t="s">
         <v>237</v>
-      </c>
-      <c r="D15" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3287,13 +3288,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3507,13 +3508,13 @@
         <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
         <v>128</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3521,13 +3522,13 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3535,13 +3536,13 @@
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
         <v>131</v>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3549,13 +3550,13 @@
         <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
         <v>133</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3563,13 +3564,13 @@
         <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
         <v>135</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3577,13 +3578,13 @@
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
         <v>137</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="169" x14ac:dyDescent="0.2">
@@ -3591,18 +3592,18 @@
         <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
         <v>139</v>
-      </c>
-      <c r="C39" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3610,7 +3611,7 @@
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -3624,13 +3625,13 @@
         <v>5</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C42" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3638,13 +3639,13 @@
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3652,21 +3653,21 @@
         <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C44" t="s">
         <v>11</v>
       </c>
       <c r="D44" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3674,18 +3675,19 @@
         <v>5</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C46" t="s">
         <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3694,7 +3696,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3710,7 +3712,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3726,7 +3728,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3734,7 +3736,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -3745,17 +3747,17 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="117" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -3763,7 +3765,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
win10 chapter Appendix changed
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F260479-B229-4799-B6CD-A466AEBBBE63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23D6F55-BBFF-4EDC-8A79-CCDC98D2A3CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37710" yWindow="1830" windowWidth="13500" windowHeight="8265" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26880" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,10 @@
     <sheet name="ch1" sheetId="3" r:id="rId3"/>
     <sheet name="ch2" sheetId="5" r:id="rId4"/>
     <sheet name="ch3" sheetId="4" r:id="rId5"/>
-    <sheet name="ch4" sheetId="9" r:id="rId6"/>
-    <sheet name="ch5" sheetId="6" r:id="rId7"/>
-    <sheet name="ch6" sheetId="7" r:id="rId8"/>
-    <sheet name="ch7" sheetId="8" r:id="rId9"/>
+    <sheet name="ch4" sheetId="6" r:id="rId6"/>
+    <sheet name="ch5" sheetId="7" r:id="rId7"/>
+    <sheet name="ch6" sheetId="8" r:id="rId8"/>
+    <sheet name="chA" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="246">
   <si>
     <t>header1</t>
   </si>
@@ -1469,66 +1469,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">※ 以下のサイト「Office365 ProPlus Windows PC向け インストール手順」をブラウザで開き、説明に従ってください。
-開く際にID,パスワードを要求されたら、広大ID（学生番号）と広大パスワード（学生証と一緒に配布された紙に書いてある）を入力してください。
-&lt;a href="https://mslicense.office.hiroshima-u.ac.jp/sw-room/ms/office2013Pro.html"&gt;https://mslicense.office.hiroshima-u.ac.jp/sw-room/ms/office2013Pro.html&lt;/a&gt;
- </t>
-    <rPh sb="55" eb="56">
-      <t>ヒラ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>このページの説明をひととおり下まで読んでから、左側メニューの「各種ソフトウェアのダウンロード」をクリックして進みます。</t>
-    <rPh sb="6" eb="8">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>ヒダリガワ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>カクシュ</t>
-    </rPh>
-    <rPh sb="54" eb="55">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「学生の個人所有PCへのインストールはここから」をクリック、さらに表示されるページの「個人所有PCのOffice製品は、Office365 Pro Plusをご利用ください」をクリックします。</t>
-    <rPh sb="1" eb="3">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ショユウ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="43" eb="45">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ショユウ</t>
-    </rPh>
-    <rPh sb="56" eb="58">
-      <t>セイヒン</t>
-    </rPh>
-    <rPh sb="80" eb="82">
-      <t>リヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>「職場または学校アカウントでサインインする」には広大メールアドレスを入力してください。パスワードには広大パスワードを入力します。</t>
     <rPh sb="1" eb="3">
       <t>ショクバ</t>
@@ -1551,131 +1491,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>あとは画面に従ってインストーラーをダウンロードして保存し、そのインストーラーを起動するとOffice365ProPlusがインストールされます。画面に従って進行し、最後に使用許諾契約を承諾するために「同意する」をクリックすると、インストール完了です。
-※この方法でインストールしたOfficeはアクティベーションも完了しているので、すぐに使うことができます。ただしこの章の最初に書いたように、&lt;strong&gt;広島大学を卒業した後は利用できなくなります&lt;/strong&gt;ので注意してください。</t>
-    <rPh sb="3" eb="5">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>キドウ</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="75" eb="76">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="78" eb="80">
-      <t>シンコウ</t>
-    </rPh>
-    <rPh sb="82" eb="84">
-      <t>サイゴ</t>
-    </rPh>
-    <rPh sb="85" eb="87">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>キョダク</t>
-    </rPh>
-    <rPh sb="89" eb="91">
-      <t>ケイヤク</t>
-    </rPh>
-    <rPh sb="92" eb="94">
-      <t>ショウダク</t>
-    </rPh>
-    <rPh sb="100" eb="102">
-      <t>ドウイ</t>
-    </rPh>
-    <rPh sb="120" eb="122">
-      <t>カンリョウ</t>
-    </rPh>
-    <rPh sb="129" eb="131">
-      <t>ホウホウ</t>
-    </rPh>
-    <rPh sb="157" eb="159">
-      <t>カンリョウ</t>
-    </rPh>
-    <rPh sb="169" eb="170">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="184" eb="185">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="186" eb="188">
-      <t>サイショ</t>
-    </rPh>
-    <rPh sb="189" eb="190">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="204" eb="206">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="206" eb="208">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="209" eb="211">
-      <t>ソツギョウ</t>
-    </rPh>
-    <rPh sb="213" eb="214">
-      <t>アト</t>
-    </rPh>
-    <rPh sb="215" eb="217">
-      <t>リヨウ</t>
-    </rPh>
-    <rPh sb="236" eb="238">
-      <t>チュウイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">次に、Microsoft Officeに含まれるアプリを起動しましょう。どれでも良いのですが、ここではExcelを起動します。
-左下のWindowsアイコンをクリックし、表示されるメニューから「Excel」を探してクリックしましょう。
-※ 見つからない時は、キーボードから「Excel」と打ち込んでみてください。
-それでもExcelが見つからないか起動しない場合は、まずPCにOfficeをインストールする必要があります。このテキストの次の章「Officeのインストール」に進んでOfficeのインストールを行ってください。
-  </t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="167" eb="168">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="174" eb="176">
-      <t>キドウ</t>
-    </rPh>
-    <rPh sb="179" eb="181">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="203" eb="205">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="220" eb="221">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="237" eb="238">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="254" eb="255">
-      <t>オコナ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ここでは、まだOfficeがインストールされていないPCにOfficeをインストールする方法を説明します。</t>
-    <rPh sb="44" eb="46">
-      <t>ホウホウ</t>
-    </rPh>
-    <rPh sb="47" eb="49">
-      <t>セツメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>学生個人所有のPCにMicrosoft Office をインストールする方法</t>
     <rPh sb="0" eb="2">
       <t>ガクセイ</t>
@@ -1693,90 +1508,6 @@
   </si>
   <si>
     <t>（付録A）Officeのインストール</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「ライセンス契約に同意します」で「同意する」をクリックします。
-※本来は「利用許諾契約書を読む」で契約事項を読んでから同意するものです。「ファイル」→「アカウント」→「Excelのバージョン情報」と辿ればいつでも読めるので、時間のある時に読んでおいてください。
-これでOfficeを使用するための準備が完了しました。&lt;span class="check"&gt;check-8&lt;span&gt;&lt;/span&gt;
-&lt;/span&gt;
-以上でこの章の作業は終了です。
-次の章「（付録A）Officeのインストール」は飛ばして、その次の章へ進んでください。</t>
-    <rPh sb="6" eb="8">
-      <t>ケイヤク</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ドウイ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ドウイ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>ホンライ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>リヨウ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>キョダク</t>
-    </rPh>
-    <rPh sb="41" eb="44">
-      <t>ケイヤクショ</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>ケイヤク</t>
-    </rPh>
-    <rPh sb="51" eb="53">
-      <t>ジコウ</t>
-    </rPh>
-    <rPh sb="54" eb="55">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="59" eb="61">
-      <t>ドウイ</t>
-    </rPh>
-    <rPh sb="95" eb="97">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="99" eb="100">
-      <t>タド</t>
-    </rPh>
-    <rPh sb="106" eb="107">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="112" eb="114">
-      <t>ジカン</t>
-    </rPh>
-    <rPh sb="117" eb="118">
-      <t>トキ</t>
-    </rPh>
-    <rPh sb="119" eb="120">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="224" eb="225">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="226" eb="227">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="229" eb="231">
-      <t>フロク</t>
-    </rPh>
-    <rPh sb="248" eb="249">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="255" eb="256">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="257" eb="258">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="259" eb="260">
-      <t>スス</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1859,9 +1590,58 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>win10-4-21.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-4-22.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">次に、Microsoft Officeに含まれるアプリを起動しましょう。どれでも良いのですが、ここではExcelを起動します。
+左下のWindowsアイコンをクリックし、表示されるメニューから「Excel」を探してクリックしましょう。
+※ 見つからない時は、キーボードから「Excel」と打ち込んでみてください。
+それでもExcelが見つからないか起動しない場合は、まずPCにOfficeをインストールする必要があります。このテキストの一番後ろにある章「（付録A）Officeのインストール」に進んでOfficeのインストールを行ってください。
+  </t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="167" eb="168">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="174" eb="176">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="179" eb="181">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="203" eb="205">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="218" eb="220">
+      <t>イチバン</t>
+    </rPh>
+    <rPh sb="220" eb="221">
+      <t>ウシ</t>
+    </rPh>
+    <rPh sb="225" eb="226">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="228" eb="230">
+      <t>フロク</t>
+    </rPh>
+    <rPh sb="247" eb="248">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="264" eb="265">
+      <t>オコナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t xml:space="preserve">右のように「サインインしてOffieを設定する」の画面が出た場合は、Officeのアクティベーションが必要です。これは、ソフトウェアが正当なコピーであることを確認し、PCで使えるようにするための作業です。Officeの正当な利用者であることを示すために、広大の学生であることを証明する必要があるわけです。
 「サインインしてOffieを設定する」で「サインイン」をクリックして、下の項目に進んでください。
-※右のような画面が出ずにExcelを使い始められる場合は、そのまま使っていただいて構いません。この下の項目と次の章を飛ばして、次の次の章「自動アップデートのセットアップと、PCのフルスキャン」に進んでください。
+※右のような画面が出ずにExcelを使い始められる場合は、そのまま使っていただいて構いません。この下の項目は飛ばして、次の章「自動アップデートのセットアップと、PCのフルスキャン」に進んでください。
   </t>
     <rPh sb="0" eb="1">
       <t>ミギ</t>
@@ -1921,34 +1701,267 @@
       <t>コウモク</t>
     </rPh>
     <rPh sb="256" eb="257">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="261" eb="262">
       <t>ツギ</t>
     </rPh>
-    <rPh sb="258" eb="259">
+    <rPh sb="263" eb="264">
       <t>ショウ</t>
     </rPh>
-    <rPh sb="260" eb="261">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="265" eb="266">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="267" eb="268">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="269" eb="270">
+    <rPh sb="293" eb="294">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「ライセンス契約に同意します」で「同意する」をクリックします。
+※本来は「利用許諾契約書を読む」で契約事項を読んでから同意するものです。「ファイル」→「アカウント」→「Excelのバージョン情報」と辿ればいつでも読めるので、時間のある時に読んでおいてください。
+これでOfficeを使用するための準備が完了しました。&lt;span class="check"&gt;check-8&lt;span&gt;&lt;/span&gt;
+&lt;/span&gt;
+以上でこの章の作業は終了です。</t>
+    <rPh sb="6" eb="8">
+      <t>ケイヤク</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ドウイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ドウイ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ホンライ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>キョダク</t>
+    </rPh>
+    <rPh sb="41" eb="44">
+      <t>ケイヤクショ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>ケイヤク</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ジコウ</t>
+    </rPh>
+    <rPh sb="54" eb="55">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>ドウイ</t>
+    </rPh>
+    <rPh sb="95" eb="97">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="99" eb="100">
+      <t>タド</t>
+    </rPh>
+    <rPh sb="106" eb="107">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="117" eb="118">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="119" eb="120">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>このテキストの第４章「自動アップデートのセットアップと、PCのフルスキャン」に戻ってください。</t>
+    <rPh sb="7" eb="8">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
       <t>ショウ</t>
     </rPh>
-    <rPh sb="299" eb="300">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-4-21.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-4-22.png</t>
+    <rPh sb="39" eb="40">
+      <t>モド</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ここでは、まだOfficeがインストールされていないPCに広島大学の提供するOffice365ProPlusをインストールする方法を説明します。</t>
+    <rPh sb="29" eb="31">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2&gt;広島大学学生向けOffice365ProPlusのインストール&lt;/h2&gt;</t>
+    <rPh sb="4" eb="6">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ム</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">以下のサイト「Office365 ProPlus Windows PC向け インストール手順」をブラウザで開き、説明に従ってください。
+開く際にID,パスワードを要求されたら、広大ID（学生番号）と広大パスワード（学生証と一緒に配布された紙に書いてある）を入力してください。
+&lt;a href="https://mslicense.office.hiroshima-u.ac.jp/sw-room/ms/office2013Pro.html"&gt;https://mslicense.office.hiroshima-u.ac.jp/sw-room/ms/office2013Pro.html&lt;/a&gt;
+ </t>
+    <rPh sb="53" eb="54">
+      <t>ヒラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>このページの説明をひととおり下まで読んでから、左側メニューの「各種ソフトウェアのダウンロード」をクリックします。</t>
+    <rPh sb="6" eb="8">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ヒダリガワ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>カクシュ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「学生の個人所有PCへのインストールはここから」をクリック、さらに表示されるページにある「個人所有PCのOffice製品は、Office365 Pro Plusをご利用ください」をクリックします。</t>
+    <rPh sb="1" eb="3">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ショユウ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>ショユウ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>セイヒン</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>リヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>あとは画面に従ってインストーラーをダウンロードして保存し、そのインストーラーを起動するとOffice365ProPlusがインストールされます。画面に従って進行し、最後に使用許諾契約を承諾するために「同意する」をクリックすると、インストール完了です。
+※この方法でインストールしたOfficeはアクティベーションも済んでいるので、すぐに使うことができます。ただしこの章の最初に書いたように、&lt;strong&gt;広島大学を卒業した後は利用できなくなります&lt;/strong&gt;ので注意してください。</t>
+    <rPh sb="3" eb="5">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="75" eb="76">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>シンコウ</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>サイゴ</t>
+    </rPh>
+    <rPh sb="85" eb="87">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>キョダク</t>
+    </rPh>
+    <rPh sb="89" eb="91">
+      <t>ケイヤク</t>
+    </rPh>
+    <rPh sb="92" eb="94">
+      <t>ショウダク</t>
+    </rPh>
+    <rPh sb="100" eb="102">
+      <t>ドウイ</t>
+    </rPh>
+    <rPh sb="120" eb="122">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="129" eb="131">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="157" eb="158">
+      <t>ス</t>
+    </rPh>
+    <rPh sb="168" eb="169">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="183" eb="184">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="185" eb="187">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="188" eb="189">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="203" eb="205">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="205" eb="207">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="208" eb="210">
+      <t>ソツギョウ</t>
+    </rPh>
+    <rPh sb="212" eb="213">
+      <t>アト</t>
+    </rPh>
+    <rPh sb="214" eb="216">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="235" eb="237">
+      <t>チュウイ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3123,8 +3136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3191,7 +3204,7 @@
         <v>218</v>
       </c>
       <c r="D8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3199,7 +3212,7 @@
         <v>219</v>
       </c>
       <c r="D9" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3207,7 +3220,7 @@
         <v>220</v>
       </c>
       <c r="D10" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3248,7 +3261,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -3259,7 +3272,7 @@
     </row>
     <row r="15" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D15" t="s">
         <v>190</v>
@@ -3321,12 +3334,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>5</v>
@@ -3343,11 +3356,906 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="78" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:D46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="234" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="234" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="169" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="117" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D45" t="s" ph="1">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="117" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392D1BFF-FF5C-4A7E-8C9C-E750AF0FFFAF}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3363,7 +4271,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3371,7 +4279,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3390,12 +4298,12 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3414,945 +4322,60 @@
         <v>222</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="78" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
       <c r="B11" s="1" t="s">
-        <v>225</v>
+        <v>243</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="65" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+      <c r="D12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D19"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="104" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>57</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="65" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
       <c r="B14" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="78" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="91" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="91" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>175</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D46"/>
-  <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="234" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="65" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="65" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="234" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="104" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="52" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="169" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C39" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C41" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="117" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>5</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C42" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="39" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>5</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C43" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="104" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="91" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D45" t="s" ph="1">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="91" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>5</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C46" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" t="s">
-        <v>119</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.6328125" customWidth="1"/>
-    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="117" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="104" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add reboot at startup win10/win10e
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75431178-EF5B-436F-B240-9570DEEC90CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527CC9F5-B032-430E-BE5C-C897BD9BA8EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29295" yWindow="2070" windowWidth="17925" windowHeight="12450" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30930" yWindow="1545" windowWidth="17925" windowHeight="12450" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="284">
   <si>
     <t>header1</t>
   </si>
@@ -155,14 +155,6 @@
   </si>
   <si>
     <t>win10-4-04.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">「ユーザ名」のところにアカウント名を入力します。
-&lt;p class="spl"&gt;※ アカウント名は学生番号の最初のアルファベットが小文字のものになります&lt;/p&gt;
-「パスワード」には広大パスワードを記入します。
-&lt;p class="spl"&gt;※ 大文字を入力するときは、SHIFTキーを押しながら文字キーを押します。&lt;/p&gt;
-両方を入力したら「OK」をクリックしてください。
-   </t>
   </si>
   <si>
     <t>win10-4-05.svg</t>
@@ -599,10 +591,6 @@
     <t>「パスワードの確認」として、先ほど決めたパスワードをもう一度入力します。</t>
   </si>
   <si>
-    <t xml:space="preserve">「デジタルアシスタントの利用」も、今の所は「拒否」としておきます。後から使うように変更できます。
-  </t>
-  </si>
-  <si>
     <t xml:space="preserve">自動アップデートのタイミング以外にDefenderを更新する方法について説明します。Windowsの自動更新機能で、Defenderは最新状態にたもたれます。しかし、緊急の脆弱性が発表された場合など、すぐに更新した方が良い時もあります。
 ウィンドウ左のリストから「Windows セキュリティ」をクリックし、「Windows セキュリティを開く」をクリックします。
   </t>
@@ -827,10 +815,6 @@
     <rPh sb="304" eb="305">
       <t>スス</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「インターネットに接続すると、・・・」と再度確認の画面が出ます。左下の「制限された設定で続行する」をクリックして飛ばします。</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -2521,6 +2505,82 @@
 第1週の授業で説明されるのは&lt;em&gt;第1章と第6章&lt;/em&gt;
 です。これらの章のファイルを同様にして保存してください。&lt;span class="check"&gt;check-11&lt;/span&gt;
   </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「ユーザ名」のところにアカウント名を入力します。
+&lt;p class="spl"&gt;※ アカウント名は学生番号の最初のアルファベットが小文字のものになります&lt;/p&gt;
+「パスワード」には広大パスワードを記入します。
+&lt;p class="spl"&gt;※ 大文字を入力するときは、SHIFTキーを押しながら文字キーを押します。&lt;/p&gt;
+両方を入力したら「OK」をクリックしてください。
+   </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「インターネットに接続すると、・・・」と再度確認の画面が出ます。左下の「制限された設定で続行する」をクリックして飛ばします。
+&lt;p class="spl"&gt;※ Surface GO では右下の選択肢から「No」をクリックして飛ばします。&lt;/p&gt;
+</t>
+    <rPh sb="93" eb="95">
+      <t>ミギシタ</t>
+    </rPh>
+    <rPh sb="96" eb="99">
+      <t>センタクシ</t>
+    </rPh>
+    <rPh sb="112" eb="113">
+      <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>再起動した後、再度ネットワークへの接続を促されますが、もう一度「インターネットに接続していません」「制限された設定で続行する」をクリックして飛ばします。</t>
+    <rPh sb="0" eb="3">
+      <t>サイキドウ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>アト</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>サイド</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ウナガ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>イチド</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>セイゲン</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>ゾッコウ</t>
+    </rPh>
+    <rPh sb="70" eb="71">
+      <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「デジタルアシスタントの利用」も、今の所は「拒否」としておきます。後から使うように変更できます。
+&lt;p class="spl"&gt;※ Surface GO ではCortanaを使うかどうかを尋ねられます。やはり「拒否」をクリックして飛 ばします。&lt;/p&gt;
+  </t>
+    <rPh sb="87" eb="88">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="94" eb="95">
+      <t>タズ</t>
+    </rPh>
+    <rPh sb="105" eb="107">
+      <t>キョヒ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2958,7 +3018,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2974,7 +3034,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2982,7 +3042,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -2996,7 +3056,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3033,7 +3093,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3041,7 +3101,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3057,7 +3117,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3065,7 +3125,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3076,7 +3136,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3084,13 +3144,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3098,13 +3158,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3112,13 +3172,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3126,13 +3186,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3140,18 +3200,18 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3159,13 +3219,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3173,13 +3233,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3187,13 +3247,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3201,18 +3261,18 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3220,13 +3280,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3234,7 +3294,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -3252,10 +3312,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A13" zoomScale="79" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="19.5" x14ac:dyDescent="0.2"/>
@@ -3272,7 +3332,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s" ph="1">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -3296,7 +3356,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
@@ -3304,7 +3364,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -3332,13 +3392,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -3346,7 +3406,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s" ph="1">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>9</v>
@@ -3357,10 +3417,10 @@
     </row>
     <row r="10" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s" ph="1">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -3368,7 +3428,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s" ph="1">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>9</v>
@@ -3382,149 +3442,157 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s" ph="1">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s" ph="1">
-        <v>177</v>
+        <v>281</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s" ph="1">
-        <v>4</v>
-      </c>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s" ph="1">
-        <v>135</v>
-      </c>
-      <c r="C14" t="s" ph="1">
-        <v>9</v>
+        <v>282</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s" ph="1">
-        <v>180</v>
+        <v>134</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s" ph="1">
-        <v>14</v>
+        <v>177</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D16" t="s" ph="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s" ph="1">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s" ph="1">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s" ph="1">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s" ph="1">
-        <v>136</v>
-      </c>
-      <c r="D17" t="s" ph="1">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s" ph="1">
-        <v>4</v>
-      </c>
+    <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s" ph="1">
-        <v>178</v>
-      </c>
-      <c r="C18" t="s" ph="1">
-        <v>9</v>
+        <v>135</v>
       </c>
       <c r="D18" t="s" ph="1">
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s" ph="1">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D19" t="s" ph="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s" ph="1">
+        <v>178</v>
+      </c>
+      <c r="C20" t="s" ph="1">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s" ph="1">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s" ph="1">
-        <v>131</v>
-      </c>
-      <c r="D20" t="s" ph="1">
-        <v>162</v>
-      </c>
-    </row>
     <row r="21" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s" ph="1">
-        <v>4</v>
-      </c>
       <c r="B21" s="1" t="s" ph="1">
-        <v>137</v>
-      </c>
-      <c r="C21" t="s" ph="1">
-        <v>9</v>
+        <v>130</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="136.5" ph="1" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s" ph="1">
-        <v>182</v>
+        <v>283</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="136.5" ph="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s" ph="1">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>155</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="s" ph="1">
+        <v>180</v>
+      </c>
+      <c r="C24" t="s" ph="1">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s" ph="1">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3539,7 +3607,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3555,7 +3623,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3579,7 +3647,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3587,7 +3655,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3601,7 +3669,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -3615,7 +3683,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -3629,7 +3697,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -3643,7 +3711,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -3657,7 +3725,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -3671,7 +3739,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -3685,7 +3753,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -3699,7 +3767,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -3713,7 +3781,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -3733,8 +3801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3774,17 +3842,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3792,13 +3860,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3806,7 +3874,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -3820,7 +3888,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -3834,7 +3902,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -3862,13 +3930,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -3876,21 +3944,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3898,7 +3966,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -3912,13 +3980,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3933,7 +4001,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView topLeftCell="B17" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3949,7 +4017,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3957,7 +4025,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3973,7 +4041,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3981,7 +4049,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3992,7 +4060,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4000,13 +4068,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>43</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4014,13 +4082,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4028,13 +4096,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -4042,13 +4110,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4056,18 +4124,18 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>48</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4075,13 +4143,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -4089,13 +4157,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -4103,13 +4171,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4117,13 +4185,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -4131,13 +4199,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4145,13 +4213,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -4182,7 +4250,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4206,7 +4274,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -4214,7 +4282,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4230,7 +4298,7 @@
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -4238,7 +4306,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -4249,39 +4317,39 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D11" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" t="s">
         <v>197</v>
-      </c>
-      <c r="D12" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D13" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D14" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4289,13 +4357,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4303,7 +4371,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -4314,7 +4382,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -4322,21 +4390,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4344,13 +4412,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4358,13 +4426,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4372,13 +4440,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4386,13 +4454,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="5" customFormat="1" ht="91" x14ac:dyDescent="0.2">
@@ -4400,13 +4468,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -4420,7 +4488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
@@ -4437,7 +4505,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4445,7 +4513,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4461,7 +4529,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -4469,7 +4537,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4480,7 +4548,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4502,13 +4570,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>57</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4516,18 +4584,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>59</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4549,13 +4617,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>62</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4563,21 +4631,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>64</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4585,13 +4653,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4599,13 +4667,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
         <v>66</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>67</v>
-      </c>
-      <c r="D17" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4613,13 +4681,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" t="s">
         <v>69</v>
-      </c>
-      <c r="C18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4627,13 +4695,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4641,13 +4709,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>72</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4655,18 +4723,18 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
         <v>74</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -4688,13 +4756,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
         <v>77</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4702,13 +4770,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4716,18 +4784,18 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>80</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -4749,13 +4817,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
         <v>83</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4763,13 +4831,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
         <v>85</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4777,13 +4845,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
         <v>87</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4791,13 +4859,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
         <v>89</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -4805,13 +4873,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4819,13 +4887,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4833,13 +4901,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
         <v>93</v>
-      </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4847,13 +4915,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
         <v>95</v>
-      </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4861,13 +4929,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
         <v>97</v>
-      </c>
-      <c r="C37" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4875,13 +4943,13 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
         <v>99</v>
-      </c>
-      <c r="C38" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="169" x14ac:dyDescent="0.2">
@@ -4889,18 +4957,18 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C39" t="s">
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4908,7 +4976,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -4922,13 +4990,13 @@
         <v>4</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C42" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4936,13 +5004,13 @@
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4950,21 +5018,21 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C44" t="s">
         <v>9</v>
       </c>
       <c r="D44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -4972,13 +5040,13 @@
         <v>4</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C46" t="s">
         <v>9</v>
       </c>
       <c r="D46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -5006,10 +5074,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5017,7 +5085,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5033,7 +5101,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -5041,7 +5109,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5052,17 +5120,17 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -5070,7 +5138,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -5107,7 +5175,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5115,7 +5183,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5131,7 +5199,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -5139,7 +5207,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5155,15 +5223,15 @@
     </row>
     <row r="8" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -5171,13 +5239,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5185,37 +5253,37 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D12" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D13" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -5223,23 +5291,23 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win10 ch5 change (Bb9 pdf download)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527CC9F5-B032-430E-BE5C-C897BD9BA8EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66C5D05-1C06-42A4-A935-55AAE76D38E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30930" yWindow="1545" windowWidth="17925" windowHeight="12450" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35655" yWindow="735" windowWidth="17925" windowHeight="11400" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="278">
   <si>
     <t>header1</t>
   </si>
@@ -346,41 +344,6 @@
   </si>
   <si>
     <t>win10-6-17.svg</t>
-  </si>
-  <si>
-    <t>win10-6-18.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">左メニューの「テキスト・スライド資料」をクリックすると右側にフォルダが表示されます。各週の資料がまとめられていますね。
-「第1章　大学で何を学ぶか（各学部・プログラム）」をクリックして開きましょう。
-  </t>
-  </si>
-  <si>
-    <t>win10-6-19.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">フォルダの中には三つのファイルがありました。
-「第1章テキスト (PDF)」の内容を確認してみましょう。
-  </t>
-  </si>
-  <si>
-    <t>win10-6-20.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">このようにPDFファイルの内容が表示されます。使っているソフト（「環境」といったりしますね）によっては、画面に直接表示されない場合もあります。そのときは、「ここをクリックして〇〇を開いてください」をクリックします。
-内容を確認したら、上の方の閲覧履歴が出てるところの「第1章...」をクリックして前の画面に戻りましょう。
-  </t>
-  </si>
-  <si>
-    <t>win10-6-21.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">掲載されているファイルを保存（ダウンロード）する一番簡単な方法は、この画面でリンクを右クリック→保存とすることです。
-「第1章テキスト (PDF)」を左クリックして表示されるメニューから「対象をファイルに保存」とします。
-  </t>
-  </si>
-  <si>
-    <t>win10-6-22.svg</t>
   </si>
   <si>
     <t>win10-6-23.svg</t>
@@ -476,15 +439,6 @@
 &lt;ul&gt; &lt;/ul&gt;
 &lt;/ul&gt;
 </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Bb9で配布されている教材を開けることを確認するため、「大学教育入門」のコースをみてみましょう。
-転入生の方は、「大学教育入門」がありませんので、「Information Security and Compliance」のコースを開いて、スライドなどがみられることを確認してください。
- 「大学教育入門」では、授業に参加する前に各自必携PCに教材をダウンロードしておくことが求められています。先ほど開いたメールにその旨の指示が来ていたと思います。
-ここでは、第1週に実施される講義の資料をダウンロードする手順を紹介しておきます。
-まず、コース一覧から「2020大学教育入門...」をクリックしてコースを開きましょう。
-  </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1927,36 +1881,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">2回目からはログインしたら、この画面が出ます。
-真ん中の「コース一覧」に、あなたがアクセスできるコースが表示されています。
-ここに並んでいるコースは、あなたが受講する授業に関連したものと、そうでないものがあります。今並んでいるものを簡単に説明すると：
-&lt;dl&gt;&lt;dt&gt;大学教育入門&lt;/dt&gt;
-&lt;dd&gt;「大学教育入門」は、大学で学ぶにあたり必要な事柄や、広島大学特有の事情について学習する授業です。全学部生必修です。このコースでは、授業の各週で使う資料をダウンロードしたり、確認テストを受験したりします。&lt;/dd&gt;
-&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
-&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届け」を提出する必要があります。このコースでは、点検届けが提出できます。&lt;strong&gt;このテキストによる設定・点検を済ませたあと、できるだけ早くにこのコースを開いて点検届を提出してください。&lt;/strong&gt;&lt;/dd&gt;
-&lt;dt&gt;Information Security and Compliance (情報セキュリティ・コンプライアンス)&lt;/dt&gt;
-&lt;dd&gt;「情報セキュリティ・コンプライアンス講習」は、広島大学でパソコンやネットワークを安全に使うための講座です。学生だけでなく、教職員を含めた全構成員必修の内容です。講習は、教室での講義とオンライン学習（このコース）からなっています。6月末までにこのコースの中にある確認テストに合格し、「&lt;em&gt;アカウント利用確認&lt;/em&gt;
-」の手続きをおこなわないと、アカウントがロックされ、メール等が使えなくなります。&lt;/dd&gt;
- &lt;/dl&gt;
-  </t>
-    <rPh sb="383" eb="385">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="386" eb="388">
-      <t>テンケン</t>
-    </rPh>
-    <rPh sb="389" eb="390">
-      <t>ス</t>
-    </rPh>
-    <rPh sb="401" eb="402">
-      <t>ハヤ</t>
-    </rPh>
-    <rPh sb="410" eb="411">
-      <t>ヒラ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">「ウイルスと脅威の防止」をクリックしましょう。
 &lt;p class="spl"&gt;※この部分に黄色のアイコンが出ている場合があります。これはランサムウェアに備えるためのOneDriveへのデータバックアップが設定されていないことを示していますが、この講習会ではまだ設定しません。気になるようでしたら「無視する」をクリックしてください。となおデータバックアップ設定はこのメニューからいつでもできます。&lt;/p&gt;
   </t>
@@ -2498,16 +2422,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">このようなパネルが表示されます。
-まず、保存されるファイルの名称と種類を確認しましょう。Edgeを使っていると、教員がつけたファイル名がここに出ているはずです。出ていなかったら、適切な名前を記入してください。ファイル形式も「PDF」になっていることを確認しましょう。HTMLとか別のものになっている場合は、違う場所で右クリックしていた可能性があります。
-次にファイルが保存されるフォルダを確認します。初期状態では「ダウンロード」フォルダです。わかりやすい場所にこれ用のフォルダを作ってそこに保存するのも良いでしょう。「ダウンロード」以外のフォルダに保存したい場合は、左側の欄を利用してフォルダを指定できます。指定したフォルダが、図の「(2) 保存先の...」のところに表示されていることを確認しましょう。
-右下の「保存」ボタンをクリックすれば保存されます。
-第1週の授業で説明されるのは&lt;em&gt;第1章と第6章&lt;/em&gt;
-です。これらの章のファイルを同様にして保存してください。&lt;span class="check"&gt;check-11&lt;/span&gt;
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">「ユーザ名」のところにアカウント名を入力します。
 &lt;p class="spl"&gt;※ アカウント名は学生番号の最初のアルファベットが小文字のものになります&lt;/p&gt;
 「パスワード」には広大パスワードを記入します。
@@ -2580,6 +2494,188 @@
     </rPh>
     <rPh sb="105" eb="107">
       <t>キョヒ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Bb9で配布されている教材をダウンロードできることを確認するため、「ノートパソコン点検届」のコースをみてみましょう。
+まず、コース一覧から「ノートパソコン点検届2020」をクリックしてコースを開きましょう。
+  </t>
+    <rPh sb="41" eb="43">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="77" eb="79">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="79" eb="80">
+      <t>トドケ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">このようにPDFファイルの内容が表示されます。使っているソフト（「環境」といったりしますね）によっては、画面に直接表示されない場合もあります。そのときは、「ここをクリックして〇〇を開いてください」をクリックします。
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">左メニューの「教材」をクリックすると右側にフォルダが表示されます。いちばん上は、点検届を提出するためのリンクです。
+２番目にある「点検届ワークシート/Checkllist worksheet」をクリックして開きましょう。
+  </t>
+    <rPh sb="7" eb="9">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>テイシュツ</t>
+    </rPh>
+    <rPh sb="59" eb="61">
+      <t>バンメ</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="67" eb="68">
+      <t>トドケ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">掲載されているファイルを保存（ダウンロード）する一番簡単な方法は、この画面で表示内容を右クリックして保存することです。
+左クリックして表示されるメニューから「名前を付けて保存」をクリックします。
+  </t>
+    <rPh sb="38" eb="40">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="82" eb="83">
+      <t>ツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">このようなパネルが表示されます。
+まず、保存されるファイルの名称と種類を確認しましょう。Edgeを使っていると、教員がつけたファイル名がここに出ているはずです。出ていなかったら、適切な名前を記入してください。ファイル形式も「PDF」になっていることを確認しましょう。HTMLとか別のものになっている場合は、違う場所で右クリックしていた可能性があります。
+次にファイルが保存されるフォルダを確認します。初期状態では「ダウンロード」フォルダです。わかりやすい場所にこれ用のフォルダを作ってそこに保存するのも良いでしょう。「ダウンロード」以外のフォルダに保存したい場合は、左側の欄を利用してフォルダを指定できます。指定したフォルダが、図の「(2) 保存先の...」のところに表示されていることを確認しましょう。
+右下の「保存」ボタンをクリックすれば保存されます。
+&lt;span class="check"&gt;check-11&lt;/span&gt;
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2回目からはログインしたら、この画面が出ます。
+真ん中の「コース一覧」に、あなたがアクセスできるコースが表示されています。
+これらは、あなたの履修課目に関する授業支援や、広島大学において自習すべき教材などのコースです。新入生共通で表示されるものを簡単に説明すると：
+&lt;dl&gt;
+&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
+&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届」を提出する必要があります。このコースでは、点検届が提出できます。&lt;strong&gt;このテキストによる設定・点検を済ませたあと、できるだけ早くにこのコースを開いて点検届を提出してください。&lt;/strong&gt;&lt;/dd&gt;
+&lt;dt&gt;大学教育入門&lt;/dt&gt;
+&lt;dd&gt;「大学教育入門」は、大学で学ぶにあたり必要な事柄や、広島大学特有の事情について学習する授業です。全学部生必修です。このコースでは、授業の各週で使う資料をダウンロードしたり、確認テストを受験したりします。&lt;/dd&gt; &lt;/dl&gt;
+  &lt;p class="spl"&gt;※今年の「大学教育入門」は、新型コロナウィルス対策のために受講方法が例年と異なります。「もみじ」などでの案内によく注意してください。&lt;/p&gt;</t>
+    <rPh sb="71" eb="73">
+      <t>リシュウ</t>
+    </rPh>
+    <rPh sb="73" eb="75">
+      <t>カモク</t>
+    </rPh>
+    <rPh sb="76" eb="77">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>ジュギョウ</t>
+    </rPh>
+    <rPh sb="81" eb="83">
+      <t>シエン</t>
+    </rPh>
+    <rPh sb="85" eb="87">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="93" eb="95">
+      <t>ジシュウ</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="109" eb="112">
+      <t>シンニュウセイ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>キョウツウ</t>
+    </rPh>
+    <rPh sb="115" eb="117">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="262" eb="264">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="265" eb="267">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="268" eb="269">
+      <t>ス</t>
+    </rPh>
+    <rPh sb="280" eb="281">
+      <t>ハヤ</t>
+    </rPh>
+    <rPh sb="289" eb="290">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="471" eb="473">
+      <t>コトシ</t>
+    </rPh>
+    <rPh sb="475" eb="477">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="477" eb="479">
+      <t>キョウイク</t>
+    </rPh>
+    <rPh sb="479" eb="481">
+      <t>ニュウモン</t>
+    </rPh>
+    <rPh sb="484" eb="486">
+      <t>シンガタ</t>
+    </rPh>
+    <rPh sb="493" eb="495">
+      <t>タイサク</t>
+    </rPh>
+    <rPh sb="499" eb="501">
+      <t>ジュコウ</t>
+    </rPh>
+    <rPh sb="501" eb="503">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="504" eb="506">
+      <t>レイネン</t>
+    </rPh>
+    <rPh sb="507" eb="508">
+      <t>コト</t>
+    </rPh>
+    <rPh sb="522" eb="524">
+      <t>アンナイ</t>
+    </rPh>
+    <rPh sb="527" eb="529">
+      <t>チュウイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -3018,7 +3114,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3034,7 +3130,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3042,7 +3138,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -3056,7 +3152,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3093,7 +3189,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3101,7 +3197,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3117,7 +3213,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3125,7 +3221,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3136,7 +3232,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3144,13 +3240,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3158,13 +3254,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3172,13 +3268,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3186,13 +3282,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3200,18 +3296,18 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3219,13 +3315,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3233,13 +3329,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3247,13 +3343,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3261,18 +3357,18 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3280,13 +3376,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3294,7 +3390,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -3332,7 +3428,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s" ph="1">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -3356,7 +3452,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
@@ -3364,7 +3460,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -3392,13 +3488,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -3406,7 +3502,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s" ph="1">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>9</v>
@@ -3417,10 +3513,10 @@
     </row>
     <row r="10" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s" ph="1">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -3428,7 +3524,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s" ph="1">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>9</v>
@@ -3442,29 +3538,29 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s" ph="1">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s" ph="1">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s" ph="1">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
@@ -3472,13 +3568,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s" ph="1">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
@@ -3486,7 +3582,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s" ph="1">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>9</v>
@@ -3511,10 +3607,10 @@
     </row>
     <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s" ph="1">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
@@ -3522,13 +3618,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s" ph="1">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -3536,7 +3632,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s" ph="1">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>9</v>
@@ -3547,10 +3643,10 @@
     </row>
     <row r="21" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s" ph="1">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
@@ -3558,13 +3654,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s" ph="1">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="136.5" ph="1" x14ac:dyDescent="0.2">
@@ -3572,13 +3668,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s" ph="1">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -3586,13 +3682,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s" ph="1">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -3623,7 +3719,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3647,7 +3743,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3655,7 +3751,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3669,7 +3765,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -3683,7 +3779,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -3697,7 +3793,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -3711,7 +3807,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -3725,7 +3821,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -3739,7 +3835,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -3753,7 +3849,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -3767,7 +3863,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -3781,7 +3877,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -3842,17 +3938,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3860,7 +3956,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -3874,7 +3970,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -3888,7 +3984,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -3902,7 +3998,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -3930,7 +4026,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -3944,7 +4040,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -3955,10 +4051,10 @@
     </row>
     <row r="15" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D15" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3966,7 +4062,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -3980,7 +4076,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -4017,7 +4113,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4025,7 +4121,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4041,7 +4137,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -4049,7 +4145,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4102,7 +4198,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -4110,13 +4206,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4143,13 +4239,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -4157,13 +4253,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -4171,7 +4267,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -4185,7 +4281,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -4199,13 +4295,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4213,13 +4309,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -4250,7 +4346,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4274,7 +4370,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -4282,7 +4378,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4298,7 +4394,7 @@
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -4306,7 +4402,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -4317,39 +4413,39 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="D11" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="D12" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="D13" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="D14" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4357,13 +4453,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4371,7 +4467,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -4382,7 +4478,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -4390,7 +4486,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -4401,10 +4497,10 @@
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="D19" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4412,13 +4508,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4426,13 +4522,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4440,13 +4536,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4454,7 +4550,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -4468,13 +4564,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -4486,10 +4582,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4513,7 +4609,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4529,7 +4625,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -4537,7 +4633,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4642,10 +4738,10 @@
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D15" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4653,13 +4749,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4695,7 +4791,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -4770,7 +4866,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -4868,12 +4964,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="234" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="182" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>259</v>
+        <v>277</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -4882,18 +4978,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="104" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>120</v>
+        <v>272</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
-      </c>
-      <c r="D34" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4901,13 +4994,10 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>92</v>
+        <v>274</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4915,13 +5005,10 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>94</v>
+        <v>273</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4929,124 +5016,107 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>96</v>
+        <v>275</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
-      <c r="D37" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="52" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:4" ht="156" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>98</v>
+        <v>276</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="169" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>4</v>
-      </c>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="C39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
       <c r="B40" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="117" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>102</v>
+      <c r="B41" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="117" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>122</v>
+      <c r="B42" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="C42" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="104" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>4</v>
-      </c>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C44" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" t="s" ph="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="91" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" t="s">
         <v>9</v>
       </c>
-      <c r="D44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="91" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D45" t="s" ph="1">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="91" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C46" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" t="s">
-        <v>107</v>
+      <c r="D45" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -5074,10 +5144,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5085,7 +5155,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5101,7 +5171,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -5109,7 +5179,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5120,17 +5190,17 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -5138,7 +5208,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -5175,7 +5245,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5183,7 +5253,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5199,7 +5269,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -5207,7 +5277,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5223,15 +5293,15 @@
     </row>
     <row r="8" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="D8" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -5239,13 +5309,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5253,37 +5323,37 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="D12" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="D13" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D14" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -5291,23 +5361,23 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add pics win10 (pdf download)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66C5D05-1C06-42A4-A935-55AAE76D38E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B3AEAF-4B35-4B53-B528-26A5623CFE5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35655" yWindow="735" windowWidth="17925" windowHeight="11400" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="610" yWindow="120" windowWidth="17930" windowHeight="11400" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="280">
   <si>
     <t>header1</t>
   </si>
@@ -344,9 +344,6 @@
   </si>
   <si>
     <t>win10-6-17.svg</t>
-  </si>
-  <si>
-    <t>win10-6-23.svg</t>
   </si>
   <si>
     <t>&lt;h2&gt;&lt;a name="omake"&gt;&lt;/a&gt;おまけ&lt;/h2&gt;</t>
@@ -2677,6 +2674,18 @@
     <rPh sb="527" eb="529">
       <t>チュウイ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-6-32.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-6-33.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-6-31.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3114,7 +3123,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3130,7 +3139,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3138,7 +3147,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -3152,7 +3161,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3189,7 +3198,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3197,7 +3206,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3213,7 +3222,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3221,7 +3230,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3232,7 +3241,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3240,13 +3249,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>216</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3254,13 +3263,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>218</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3268,13 +3277,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>220</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3282,13 +3291,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>222</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3296,18 +3305,18 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>224</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -3315,13 +3324,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>227</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -3329,13 +3338,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>229</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3343,13 +3352,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -3357,18 +3366,18 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -3376,13 +3385,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>236</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3390,7 +3399,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -3428,7 +3437,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s" ph="1">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -3452,7 +3461,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
@@ -3460,7 +3469,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -3488,13 +3497,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -3502,7 +3511,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s" ph="1">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>9</v>
@@ -3513,10 +3522,10 @@
     </row>
     <row r="10" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s" ph="1">
+        <v>140</v>
+      </c>
+      <c r="D10" t="s" ph="1">
         <v>141</v>
-      </c>
-      <c r="D10" t="s" ph="1">
-        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -3524,7 +3533,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s" ph="1">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>9</v>
@@ -3538,29 +3547,29 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s" ph="1">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s" ph="1">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s" ph="1">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
@@ -3568,13 +3577,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s" ph="1">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="58.5" ph="1" x14ac:dyDescent="0.2">
@@ -3582,7 +3591,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s" ph="1">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>9</v>
@@ -3607,10 +3616,10 @@
     </row>
     <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s" ph="1">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="117" ph="1" x14ac:dyDescent="0.2">
@@ -3618,13 +3627,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s" ph="1">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -3632,7 +3641,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s" ph="1">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>9</v>
@@ -3643,10 +3652,10 @@
     </row>
     <row r="21" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s" ph="1">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="78" ph="1" x14ac:dyDescent="0.2">
@@ -3654,13 +3663,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s" ph="1">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="136.5" ph="1" x14ac:dyDescent="0.2">
@@ -3668,13 +3677,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s" ph="1">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39" ph="1" x14ac:dyDescent="0.2">
@@ -3682,13 +3691,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s" ph="1">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>9</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3719,7 +3728,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3743,7 +3752,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -3751,7 +3760,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3765,7 +3774,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -3779,7 +3788,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -3793,7 +3802,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -3807,7 +3816,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -3821,7 +3830,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -3835,7 +3844,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -3849,7 +3858,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -3863,7 +3872,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -3877,7 +3886,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -3938,17 +3947,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -3956,7 +3965,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -3970,7 +3979,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -3984,7 +3993,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -3998,7 +4007,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -4026,7 +4035,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -4040,7 +4049,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -4051,10 +4060,10 @@
     </row>
     <row r="15" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4062,7 +4071,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -4076,7 +4085,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -4113,7 +4122,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4121,7 +4130,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4137,7 +4146,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -4145,7 +4154,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4198,7 +4207,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -4206,13 +4215,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -4239,13 +4248,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -4253,13 +4262,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="143" x14ac:dyDescent="0.2">
@@ -4267,7 +4276,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -4281,7 +4290,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -4295,13 +4304,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -4309,13 +4318,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -4346,7 +4355,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4370,7 +4379,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -4378,7 +4387,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4394,7 +4403,7 @@
     </row>
     <row r="8" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="117" x14ac:dyDescent="0.2">
@@ -4402,7 +4411,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -4413,39 +4422,39 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4453,13 +4462,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -4467,7 +4476,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -4478,7 +4487,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -4486,7 +4495,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -4497,10 +4506,10 @@
     </row>
     <row r="19" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4508,13 +4517,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4522,13 +4531,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4536,13 +4545,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4550,7 +4559,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -4564,13 +4573,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -4584,8 +4593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4609,7 +4618,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4625,7 +4634,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="234" x14ac:dyDescent="0.2">
@@ -4633,7 +4642,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -4738,10 +4747,10 @@
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" t="s">
         <v>158</v>
-      </c>
-      <c r="D15" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4749,13 +4758,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4791,7 +4800,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -4866,7 +4875,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -4969,7 +4978,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -4983,7 +4992,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -4994,7 +5003,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -5005,10 +5014,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="52" x14ac:dyDescent="0.2">
@@ -5016,10 +5028,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="156" x14ac:dyDescent="0.2">
@@ -5027,18 +5042,18 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>278</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -5046,7 +5061,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -5060,13 +5075,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -5074,13 +5089,13 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42" t="s">
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -5088,21 +5103,21 @@
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C43" t="s">
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="91" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="91" x14ac:dyDescent="0.2">
@@ -5110,13 +5125,13 @@
         <v>4</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C45" t="s">
         <v>9</v>
       </c>
       <c r="D45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -5144,10 +5159,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5155,7 +5170,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5171,7 +5186,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -5179,7 +5194,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5190,17 +5205,17 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="104" x14ac:dyDescent="0.2">
@@ -5208,7 +5223,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -5245,7 +5260,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5253,7 +5268,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5269,7 +5284,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -5277,7 +5292,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5293,15 +5308,15 @@
     </row>
     <row r="8" spans="1:4" ht="104" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="78" x14ac:dyDescent="0.2">
@@ -5309,13 +5324,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5323,37 +5338,37 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D13" t="s">
         <v>244</v>
-      </c>
-      <c r="D13" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" t="s">
         <v>158</v>
-      </c>
-      <c r="D14" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -5361,23 +5376,23 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="78" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win10e reviewed/ win10 add pics Bb9 course list
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0057E948-2AD1-4BDB-B105-70A1F9C14419}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2AD98D-F568-45E8-9955-4DE0B212C2EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34620" yWindow="3420" windowWidth="13425" windowHeight="10575" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38715" yWindow="2490" windowWidth="13425" windowHeight="10575" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="284">
   <si>
     <t>header1</t>
   </si>
@@ -2734,6 +2734,10 @@
   </si>
   <si>
     <t>win10-6-35.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-6-36.svg</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4641,8 +4645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="B33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -5044,6 +5048,9 @@
       </c>
       <c r="C34" t="s">
         <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="52" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix win10/win10e pic pointers
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seigo Kishiba\Documents\GitHub\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2AD98D-F568-45E8-9955-4DE0B212C2EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18452752-259A-4809-BEF0-53F42B9CAC12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38715" yWindow="2490" windowWidth="13425" windowHeight="10575" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29970" yWindow="2535" windowWidth="13425" windowHeight="10575" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="285">
   <si>
     <t>header1</t>
   </si>
@@ -2738,6 +2738,10 @@
   </si>
   <si>
     <t>win10-6-36.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win10-6-41.svg</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4645,8 +4649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="B44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4802,7 +4806,7 @@
         <v>157</v>
       </c>
       <c r="D15" t="s">
-        <v>158</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix a pic for win10
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:1_{4E73EF56-EA13-4BCA-972F-7F8EEF561B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87986728-D1B7-4D04-9775-DF238F83C192}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="13_ncr:1_{4E73EF56-EA13-4BCA-972F-7F8EEF561B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1915950F-DF24-4563-A897-7FC7341B6D30}"/>
   <bookViews>
     <workbookView xWindow="3787" yWindow="1890" windowWidth="16216" windowHeight="13590" tabRatio="782" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4205,10 +4205,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ms-download-home.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>以下のサイト「ダウンロード（マイクロソフト包括ライセンス）」をブラウザで開いて、その中の「Microsoft Office」「個人所有PC用のダウンロードはこちらから」のリンクをクリックしてください。
 &lt;a href="https://www.media.hiroshima-u.ac.jp/services/ms-ees/ms-download/"&gt;https://www.media.hiroshima-u.ac.jp/services/ms-ees/ms-download/&lt;/a&gt;</t>
     <rPh sb="21" eb="23">
@@ -4828,6 +4824,10 @@
     <rPh sb="160" eb="162">
       <t>リョウカイ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ms-download-office.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5511,10 +5511,10 @@
     </row>
     <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D10" t="s">
-        <v>282</v>
+        <v>307</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5525,7 +5525,7 @@
         <v>87</v>
       </c>
       <c r="D11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5533,31 +5533,31 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>285</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D14" t="s">
         <v>288</v>
-      </c>
-      <c r="D14" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -6009,7 +6009,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s" ph="1">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6041,7 +6041,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6311,7 +6311,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6538,7 +6538,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6890,7 +6890,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6925,7 +6925,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6946,7 +6946,7 @@
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D9" t="s">
         <v>216</v>
@@ -6990,7 +6990,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7001,7 +7001,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7126,7 +7126,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7519,7 +7519,7 @@
     </row>
     <row r="30" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -7527,7 +7527,7 @@
     </row>
     <row r="31" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -7538,7 +7538,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -7552,7 +7552,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -7563,7 +7563,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -7577,7 +7577,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -7591,7 +7591,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
win10ja: update how to access Office365 portal
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E705D10-41FA-4E1D-B3AE-4FCB41EA7C7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C13EF0-1109-4C96-AEA3-096DA4D4932E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3792" yWindow="1896" windowWidth="16212" windowHeight="13596" tabRatio="782" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3792" yWindow="1896" windowWidth="16212" windowHeight="13596" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="309">
   <si>
     <t>header1</t>
   </si>
@@ -3335,37 +3335,6 @@
     <t>win11ja-momiji-before-login0.png</t>
   </si>
   <si>
-    <t>microsoft.comにアクセスします。画面の一番上に広告が出てくることがありますが、「結構です」で消しておきましょう。右上に「サインイン」と注された人型アイコンがあるので、クリックします。URLフォームの横にある人型アイコンではないことに注意してください。</t>
-    <rPh sb="22" eb="24">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>イチバン</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>ウエ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>コウコク</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="46" eb="48">
-      <t>ケッコウ</t>
-    </rPh>
-    <rPh sb="52" eb="53">
-      <t>ケ</t>
-    </rPh>
-    <rPh sb="62" eb="64">
-      <t>ミギウエ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-ms-signin.png</t>
-  </si>
-  <si>
     <t>IMCアカウントを「@hiroshima-u.ac.jp」つきで入力し、さらにパスワードも入力します。このサイトはMicrosoftのサイトなので、「@hiroshima-u.ac.jp」がついていないと貴方の学生番号がどの大学のものか判らないため、「@hiroshima-u.ac.jp」を加える必要があります。</t>
     <rPh sb="32" eb="34">
       <t>ニュウリョク</t>
@@ -3429,68 +3398,6 @@
   </si>
   <si>
     <t>win11ja-ms-signin3.png</t>
-  </si>
-  <si>
-    <t>サインインが完了すると、右上の人型のマークが社員証のマークに変わっています。これをクリックしてサブメニューを表示させ、さらに「アカウントを表示」に進みます。「マイアカウント」というページに移動します。</t>
-    <rPh sb="6" eb="8">
-      <t>カンリョウ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ミギウエ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ヒトガタ</t>
-    </rPh>
-    <rPh sb="22" eb="25">
-      <t>シャインショウ</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="54" eb="56">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="69" eb="71">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="73" eb="74">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="94" eb="96">
-      <t>イドウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-ms-myaccount.png</t>
-  </si>
-  <si>
-    <t>「マイアカウント」のページの左上に3x3個の点が並んでいるアイコンがあるので、これをクリックしてサブメニューを表示させます。その中の「Office」をクリックすると、「マイアカウント」から「Office365」のページに移動します。</t>
-    <rPh sb="14" eb="16">
-      <t>ヒダリウエ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>コ</t>
-    </rPh>
-    <rPh sb="22" eb="23">
-      <t>テン</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>ナラ</t>
-    </rPh>
-    <rPh sb="55" eb="57">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="64" eb="65">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="110" eb="112">
-      <t>イドウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-ms-office365.png</t>
   </si>
   <si>
     <t>Office365のページの左側にブラウザ内で使用できるアプリのアイコンが並びます。「O」の文字があるOutlook for Webをクリックします。</t>
@@ -3691,34 +3598,6 @@
     </rPh>
     <rPh sb="134" eb="135">
       <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Outlook for Webのページが開き、新着メールを確認することができます。大学からのメール連絡は広大メールに来ますので、常にメールチェックするようにしてください。&lt;span class="check"&gt;check-11&lt;span&gt;&lt;/span&gt;</t>
-    <rPh sb="20" eb="21">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>シンチャク</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>レンラク</t>
-    </rPh>
-    <rPh sb="52" eb="54">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="58" eb="59">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="64" eb="65">
-      <t>ツネ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4904,6 +4783,51 @@
     </rPh>
     <rPh sb="233" eb="234">
       <t>オコナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メディアセンタのMicrosoft 365ポータルサイト&lt;a href="https://www.media.hiroshima-u.ac.jp/services/webmail-portal/" target="_blank" rel="noreferrer"&gt;https://www.media.hiroshima-u.ac.jp/services/webmail-portal/&lt;/a&gt;にジャンプします。水色の「Microsoft365ポータル」を押すと&lt;a href="https://portal.office.com/" target="_blank" rel="noreferrer"&gt;https://portal.office.com/&lt;/a&gt;に移動します。</t>
+    <rPh sb="205" eb="207">
+      <t>ミズイロ</t>
+    </rPh>
+    <rPh sb="227" eb="228">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="331" eb="333">
+      <t>イドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-imc-office365-portal.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Outlook for Webのページが開き、新着メールを確認することができます。大学からのメール連絡は広大メールに来ますので、常にメールチェックするようにしてください。</t>
+    <rPh sb="20" eb="21">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>シンチャク</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>レンラク</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>ツネ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5341,7 +5265,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5379,7 +5303,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5416,7 +5340,7 @@
         <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5440,17 +5364,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5458,12 +5382,12 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D9" t="s">
         <v>210</v>
@@ -5471,17 +5395,17 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -5523,7 +5447,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5531,7 +5455,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5547,22 +5471,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5570,7 +5494,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -5586,7 +5510,7 @@
     </row>
     <row r="14" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D14" t="s">
         <v>109</v>
@@ -5599,10 +5523,10 @@
     </row>
     <row r="16" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="D16" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5613,7 +5537,7 @@
         <v>87</v>
       </c>
       <c r="D17" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5621,41 +5545,41 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="D20" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -5912,7 +5836,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s" ph="1">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -5936,7 +5860,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -5944,7 +5868,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6214,7 +6138,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6441,7 +6365,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6457,7 +6381,7 @@
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -6793,7 +6717,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6828,7 +6752,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6844,12 +6768,12 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="D9" t="s">
         <v>210</v>
@@ -6893,7 +6817,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6904,7 +6828,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6931,7 +6855,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DD8924-3FAE-44AB-A508-09E9136389D4}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -6991,7 +6915,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7015,7 +6939,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7023,13 +6947,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7073,7 +6997,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7107,10 +7031,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7233,346 +7157,312 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
+    <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D13" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D14" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D17" t="s">
         <v>238</v>
       </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>240</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="19" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D19" t="s">
+    <row r="24" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="5" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
       <c r="D24" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D25" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="D25" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>308</v>
+      <c r="C26" t="s">
+        <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>256</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
       <c r="B29" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>4</v>
+        <v>275</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
-      <c r="D30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
       <c r="B32" s="1" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
-      <c r="D33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="66" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
+        <v>291</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
       <c r="B38" s="1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>271</v>
+      <c r="B39" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>62</v>
+      <c r="B40" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>4</v>
-      </c>
+      <c r="D40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" t="s" ph="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" t="s">
         <v>8</v>
       </c>
-      <c r="D41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" t="s" ph="1">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C43" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="D42" t="s">
         <v>58</v>
       </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D50" ph="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -7610,7 +7500,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7626,7 +7516,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win10ja, win11ja: visit Office365 portal instead of EES.
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C13EF0-1109-4C96-AEA3-096DA4D4932E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3792" yWindow="1896" windowWidth="16212" windowHeight="13596" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3792" yWindow="1896" windowWidth="16212" windowHeight="13596" tabRatio="782" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="303">
   <si>
     <t>header1</t>
   </si>
@@ -404,11 +404,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">Office365にサインインする画面になります。まず「IMCアカウント名@hiroshima-u.ac.jp」を記入し「次へ」をクリックします。
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Microsoft Teams について。最近のWindows10パソコンでは、サインイン時にMicrosoft Teams が自動的に起動します。これはMicrosoftが提供しているグループチャットアプリで、広大メールアドレスとパスワードでサインインして使うことができます。
 詳細はメディアセンターWebサイトの&lt;a href="https://www.media.hiroshima-u.ac.jp/services/communication/teams/"&gt;「Microsft Teams」&lt;/a&gt;で。
 また、使わない場合は画面左下のウィンドウアイコンから「設定」→「アプリ」→「スタートアップ」と進んでTeamsのスイッチを「オフ」にすると、自動起動を止めることができます。</t>
@@ -3960,61 +3955,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>以下のサイト「ダウンロード（マイクロソフト包括ライセンス）」をブラウザで開いて、その中の「Microsoft Office」「個人所有PC用のダウンロードはこちらから」のリンクをクリックしてください。
-&lt;a href="https://www.media.hiroshima-u.ac.jp/services/ms-ees/ms-download/"&gt;https://www.media.hiroshima-u.ac.jp/services/ms-ees/ms-download/&lt;/a&gt;</t>
-    <rPh sb="21" eb="23">
-      <t>ホウカツ</t>
-    </rPh>
-    <rPh sb="42" eb="43">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="65" eb="67">
-      <t>ショユウ</t>
-    </rPh>
-    <rPh sb="69" eb="70">
-      <t>ヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ch5-hirodai-login.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">広大パスワードを入力し「サインイン」をクリックします。
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ch5-hirodai-login-password.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>学外からのアクセスのときは、ここで多要素認証（MFA）の認証手続きが入る場合があります。</t>
-    <rPh sb="0" eb="2">
-      <t>ガクガイ</t>
-    </rPh>
-    <rPh sb="17" eb="22">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>ニンショウ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>テツヅ</t>
-    </rPh>
-    <rPh sb="34" eb="35">
-      <t>ハイ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Office365にサインインした状態になります。&lt;span class="check"&gt;check-11&lt;/span&gt;
 ここでは左右を縮めて表示していますが、画面の右側のほうに「Officeのインストール」というメニューがありますので、そこからOffice 365アプリを選びます。</t>
     <rPh sb="17" eb="19">
@@ -4582,10 +4522,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ms-download-office.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>FRESTA-TEXT-2022 Win10 chap.9</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -4829,6 +4765,10 @@
     <rPh sb="64" eb="65">
       <t>ツネ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>学外からのアクセスのときは、ここで多要素認証（MFA）の認証手続きが入る場合があります。</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5265,7 +5205,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5281,7 +5221,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -5289,7 +5229,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -5303,7 +5243,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5337,10 +5277,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5364,17 +5304,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5382,30 +5322,30 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -5430,8 +5370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392D1BFF-FF5C-4A7E-8C9C-E750AF0FFFAF}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -5447,7 +5387,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5455,7 +5395,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5471,22 +5411,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5494,7 +5434,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -5510,81 +5450,72 @@
     </row>
     <row r="14" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D16" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D17" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D19" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D20" t="s">
         <v>267</v>
       </c>
-      <c r="D16" t="s">
+    </row>
+    <row r="21" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="D20" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -5593,218 +5524,218 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C42" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D42" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C48" t="s">
         <v>8</v>
       </c>
       <c r="D48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -5836,7 +5767,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s" ph="1">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -5844,7 +5775,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s" ph="1">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -5860,7 +5791,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -5868,7 +5799,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -5888,7 +5819,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
@@ -5896,7 +5827,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>8</v>
@@ -5910,13 +5841,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s" ph="1">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
@@ -5924,7 +5855,7 @@
         <v>76</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -5938,7 +5869,7 @@
         <v>8</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="142.80000000000001" ph="1" x14ac:dyDescent="0.2">
@@ -5946,29 +5877,29 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s" ph="1">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s" ph="1">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s" ph="1">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="122.4" ph="1" x14ac:dyDescent="0.2">
@@ -5982,7 +5913,7 @@
         <v>8</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="102" ph="1" x14ac:dyDescent="0.2">
@@ -5990,13 +5921,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s" ph="1">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
@@ -6004,13 +5935,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s" ph="1">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6018,7 +5949,7 @@
         <v>69</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="122.4" ph="1" x14ac:dyDescent="0.2">
@@ -6026,13 +5957,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s" ph="1">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6040,18 +5971,18 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s" ph="1">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s" ph="1">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D21" t="s" ph="1">
         <v>84</v>
@@ -6062,7 +5993,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s" ph="1">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>8</v>
@@ -6076,24 +6007,24 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s" ph="1">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s" ph="1">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -6101,7 +6032,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s" ph="1">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>8</v>
@@ -6138,7 +6069,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6146,7 +6077,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6162,7 +6093,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -6170,7 +6101,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6198,7 +6129,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -6226,7 +6157,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -6240,7 +6171,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -6254,7 +6185,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -6296,7 +6227,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -6333,7 +6264,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6341,7 +6272,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6357,7 +6288,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -6365,7 +6296,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6381,7 +6312,7 @@
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -6483,7 +6414,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -6497,7 +6428,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -6525,7 +6456,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -6539,13 +6470,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -6576,7 +6507,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6584,7 +6515,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6600,7 +6531,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -6608,7 +6539,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6624,44 +6555,44 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6669,13 +6600,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6717,7 +6648,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6725,7 +6656,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6741,7 +6672,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -6752,7 +6683,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6768,15 +6699,15 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6784,13 +6715,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>211</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -6798,18 +6729,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>213</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6817,7 +6748,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6828,7 +6759,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6839,7 +6770,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -6853,10 +6784,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DD8924-3FAE-44AB-A508-09E9136389D4}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6872,7 +6803,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6880,7 +6811,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6896,7 +6827,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6904,7 +6835,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6915,12 +6846,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -6928,7 +6859,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -6939,7 +6870,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6947,21 +6878,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D12" t="s">
         <v>221</v>
-      </c>
-      <c r="D12" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -6969,49 +6900,46 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>223</v>
       </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>225</v>
       </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="132" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
         <v>226</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="132" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -7019,6 +6947,14 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
         <v>4</v>
       </c>
     </row>
@@ -7033,8 +6969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7058,7 +6994,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7074,7 +7010,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="264" x14ac:dyDescent="0.2">
@@ -7082,7 +7018,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7135,7 +7071,7 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -7159,53 +7095,53 @@
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="D13" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D14" t="s">
         <v>232</v>
-      </c>
-      <c r="D14" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D15" t="s">
         <v>234</v>
-      </c>
-      <c r="D15" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D16" t="s">
         <v>236</v>
-      </c>
-      <c r="D16" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="D17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>239</v>
-      </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -7216,7 +7152,7 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -7243,29 +7179,29 @@
         <v>4</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>242</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D25" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7273,7 +7209,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -7317,7 +7253,7 @@
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -7325,7 +7261,7 @@
     </row>
     <row r="31" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -7336,7 +7272,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -7350,7 +7286,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -7361,7 +7297,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -7375,7 +7311,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -7389,12 +7325,12 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7402,7 +7338,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
@@ -7441,7 +7377,7 @@
     </row>
     <row r="41" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D41" t="s" ph="1">
         <v>73</v>
@@ -7500,7 +7436,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7516,17 +7452,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7534,7 +7470,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -7548,7 +7484,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -7562,7 +7498,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7576,7 +7512,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7604,7 +7540,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7629,7 +7565,7 @@
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D15" t="s">
         <v>66</v>
@@ -7640,7 +7576,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -7654,7 +7590,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
change pic edge-icon win10(ja)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CAC1FB1-4951-4E7B-BB74-A31649A1D7DC}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DF9B637-1AE1-40A1-8791-FAE78BEA51E3}"/>
   <bookViews>
-    <workbookView xWindow="54135" yWindow="975" windowWidth="18225" windowHeight="11880" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2573" yWindow="2573" windowWidth="18224" windowHeight="11872" tabRatio="782" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="315">
   <si>
     <t>header1</t>
   </si>
@@ -4732,32 +4732,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-start-edge-taskbar.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>まずWebブラウザを起動しましょう。画面の最下部のタスクバーに「e」を模した青緑のアイコンがありますので、これをクリックしてMicrosoft Edgeを起動します。</t>
-    <rPh sb="10" eb="12">
-      <t>キドウ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="21" eb="24">
-      <t>サイカブ</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>モ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>アオミドリ</t>
-    </rPh>
-    <rPh sb="77" eb="79">
-      <t>キドウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">Edgeの規定の新規タブには大量の広告が入ってくるので、オンライン授業などで画面共有の際に憚られるような画面になる場合があります。右上の歯車アイコンを押して、画面レイアウトを「シンプル」にしましょう。これでEdgeの基本的な設定は終わります。
 </t>
     <rPh sb="5" eb="7">
@@ -4985,58 +4959,48 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;strong&gt;初めてWebブラウザを起動するときにはいくつかの設定に同意を求められることがあります。これらはいったんキャンセルまたは拒否して進める方が無難です。この設定は後でも変えられるので、ある程度使い慣れてから見直しましょう。&lt;/strong&gt;
-※　以下ではEdgeを初めて起動したときについて説明します。</t>
-    <rPh sb="8" eb="9">
-      <t>ハジ</t>
-    </rPh>
-    <rPh sb="19" eb="21">
+    <t>edge-icon.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>まずWebブラウザを起動しましょう。画面の最下部のタスクバーに「e」を模した青緑のアイコンがありますので、これをクリックしてMicrosoft Edgeを起動します。
+&lt;strong&gt;初めてWebブラウザを起動するときにはいくつかの設定に同意を求められることがあります。これらはいったんキャンセルまたは拒否して進める方が無難です。この設定は後でも変えられるので、ある程度使い慣れてから見直しましょう。以下ではEdgeを初めて起動したときについて説明します。&lt;/strong&gt;
+※ Edgeを起動するのが２回目以降のときは、下の「Google Chromeを入れる」まで飛んでください。</t>
+    <rPh sb="10" eb="12">
       <t>キドウ</t>
     </rPh>
-    <rPh sb="67" eb="69">
-      <t>キョヒ</t>
-    </rPh>
-    <rPh sb="71" eb="72">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="74" eb="75">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="76" eb="78">
-      <t>ブナン</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="86" eb="87">
-      <t>アト</t>
-    </rPh>
-    <rPh sb="89" eb="90">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="99" eb="101">
-      <t>テイド</t>
-    </rPh>
-    <rPh sb="101" eb="102">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="103" eb="104">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="108" eb="110">
-      <t>ミナオ</t>
-    </rPh>
-    <rPh sb="128" eb="130">
-      <t>イカ</t>
-    </rPh>
-    <rPh sb="137" eb="138">
-      <t>ハジ</t>
-    </rPh>
-    <rPh sb="140" eb="142">
+    <rPh sb="18" eb="20">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="21" eb="24">
+      <t>サイカブ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>アオミドリ</t>
+    </rPh>
+    <rPh sb="77" eb="79">
       <t>キドウ</t>
     </rPh>
-    <rPh sb="150" eb="152">
-      <t>セツメイ</t>
+    <rPh sb="245" eb="247">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="252" eb="254">
+      <t>カイメ</t>
+    </rPh>
+    <rPh sb="254" eb="256">
+      <t>イコウ</t>
+    </rPh>
+    <rPh sb="261" eb="262">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="278" eb="279">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="284" eb="285">
+      <t>ト</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -6036,7 +6000,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s" ph="1">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6338,7 +6302,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6757,10 +6721,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43F54BA-B356-43A4-B76F-707ED0C70724}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6808,7 +6772,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6827,115 +6791,110 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="D9" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+      <c r="D10" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D11" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D12" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D13" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="D14" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+      <c r="D16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>314</v>
+        <v>103</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="D18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D19" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
       <c r="B20" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
         <v>19</v>
       </c>
     </row>
@@ -7197,7 +7156,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7288,7 +7247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -7416,7 +7375,7 @@
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D14" t="s">
         <v>232</v>

</xml_diff>

<commit_message>
change Chrome install procedure win10(ja)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DF9B637-1AE1-40A1-8791-FAE78BEA51E3}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78E95A1A-DC2E-4191-8F6C-814F4DF20422}"/>
   <bookViews>
-    <workbookView xWindow="2573" yWindow="2573" windowWidth="18224" windowHeight="11872" tabRatio="782" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6098" yWindow="3472" windowWidth="18225" windowHeight="11873" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="319">
   <si>
     <t>header1</t>
   </si>
@@ -620,33 +620,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">「このアプリがデバイスに変更を加えることを許可しますか」と聞かれるので「はい」と答えてください。
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Google Chrome 利用規約が表示されるので、「同意してインストール」をクリックします。
-</t>
-    <rPh sb="14" eb="16">
-      <t>リヨウ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>キヤク</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>ドウイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Microsoft Update を使って、Windows と Office がつねに最新版で使えるように設定します。またウィルス対策ソフトも自動アップデートで最新のウィルス防御機能を維持できるようにしておきます。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-2-42.png</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -675,59 +649,6 @@
   </si>
   <si>
     <t>win10-2-41.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-2-43.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-2-44.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>しばらくすると画面の下のところでアイコンが黄色く点滅するので、それをクリックします。
-&lt;p class="spl"&gt;※自動的に画面が切り替わることもありますので、その場合は下の項目に進んでください。&lt;/p&gt;</t>
-    <rPh sb="7" eb="9">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>キイロ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>テンメツ</t>
-    </rPh>
-    <rPh sb="59" eb="62">
-      <t>ジドウテキ</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="66" eb="67">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="68" eb="69">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="86" eb="87">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="88" eb="90">
-      <t>コウモク</t>
-    </rPh>
-    <rPh sb="91" eb="92">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win10-2-10a.svg</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -770,53 +691,6 @@
   </si>
   <si>
     <t>description</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ダウンロードしたファイルを実行します。
-&lt;p class="spl"&gt;※右の図はWebブラウザにMicrosoft Edgeを使った場合の表示です。他のブラウザを使った場合、表示が少し違うものになりますが「ダウンロードしたファイルを実行する」ことは同じです。</t>
-    <rPh sb="13" eb="15">
-      <t>ジッコウ</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>ミギ</t>
-    </rPh>
-    <rPh sb="38" eb="39">
-      <t>ズ</t>
-    </rPh>
-    <rPh sb="63" eb="64">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="66" eb="68">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="69" eb="71">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="74" eb="75">
-      <t>タ</t>
-    </rPh>
-    <rPh sb="81" eb="82">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="84" eb="86">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="90" eb="91">
-      <t>スコ</t>
-    </rPh>
-    <rPh sb="92" eb="93">
-      <t>チガ</t>
-    </rPh>
-    <rPh sb="116" eb="118">
-      <t>ジッコウ</t>
-    </rPh>
-    <rPh sb="124" eb="125">
-      <t>オナ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -4283,27 +4157,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>次のリンクから広島大学オンライン学習支援システム（広大moodle）にアクセスしてください。
-&lt;a href="https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/"&gt;https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/&lt;/a&gt;
-「広大IDでログイン」をクリックしましょう。</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="7" eb="11">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="16" eb="20">
-      <t>ガクシュウシエン</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="166" eb="168">
-      <t>ヒロダイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>大学で提供されているオンラインサービスはいくつもありますが、まずオンライン学習支援システムの広大moodleにログインしてみましょう。
  &lt;ul&gt;
 &lt;li&gt;&lt;a href="#moodle"&gt;広大moodleにログインする&lt;/a&gt;
@@ -4816,16 +4669,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">この章から、テキストにあるリンク（URL）をクリックしてWebブラウザを使うと作業しやすい場面が多くなります。
-できれば作業しているPCでこのテキストを見ながら作業しましょう。ネットワークに接続していればできるはずです。
-&lt;a href="https;//riise.hiroshima-u.ac.jp/fresta/2022/"&gt;https;//riise.hiroshima-u.ac.jp/fresta/2022/&lt;/a&gt;
-</t>
-    <rPh sb="2" eb="3">
-      <t>ショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>それでは、まずMicrosoft Officeが既にインストールされているか確認しましょう。タスクバーのスタートボタンを押し、スタートメニューを開きます。その中にWord, Excel, PowerPointなどがあれば既にインストールされているのですが、見つからない場合には検索フォームにExcelなどと入力して探します。Excelが見つからない場合は、まだPCにOfficeがインストールされていないようです。このテキストの後のほうにある付録に従ってインストールしてから続きを行いましょう。</t>
     <rPh sb="24" eb="25">
       <t>スデ</t>
@@ -4942,20 +4785,6 @@
   </si>
   <si>
     <t xml:space="preserve">自分のパソコンの基本的なスペックを確認しておきましょう。CPUの型式、OSのビット数、記憶容量など。 </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">まずGoogle Chromeを入れます。Web上の配布サイトから直接ダウンロードしましょう。
-&lt;a href="https://www.google.com/chrome/" target="_blank" rel="noreferrer"&gt;https://www.google.com/chrome/&lt;/a&gt;
-　（または「Chrome インストール」を検索して出てくるChromeダウンロードページ）
-で、「Chromeをダウンロード」をクリックしてください。
-</t>
-    <rPh sb="178" eb="180">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="182" eb="183">
-      <t>デ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5001,6 +4830,219 @@
     </rPh>
     <rPh sb="284" eb="285">
       <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">この章から、テキストにあるリンク（URL）をクリックしてWebブラウザを使うと作業しやすい場面が多くなります。
+できれば作業しているPCでこのテキストを見ながら作業しましょう。ネットワークに接続していればできるはずです。
+&lt;a href="https://riise.hiroshima-u.ac.jp/fresta/2022/"&gt;https://riise.hiroshima-u.ac.jp/fresta/2022/&lt;/a&gt;
+</t>
+    <rPh sb="2" eb="3">
+      <t>ショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Googleのダウンロードページにジャンプしました。Google Chromeのブラウザ内部のデータをGoogleに送信しても良いかという許可チェックボックスがありますが、このチェックを外してダウンロードを行います。</t>
+    <rPh sb="44" eb="46">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>ソウシン</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>キョカ</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="103" eb="104">
+      <t>オコナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-google-chrome-download-page.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ダウンロードが終わるとEdgeの右上に「↓」マークが現れます。これに緑のマークがついていたらダウンロードが完了しています。「↓」をクリックしてダウンロードしたファイルのリストを出し、右横のフォルダアイコンをクリックします。マウスポインタを持っていかないとフォルダアイコンが出ないので気をつけてください。</t>
+    <rPh sb="7" eb="8">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ミギウエ</t>
+    </rPh>
+    <rPh sb="26" eb="27">
+      <t>アラワ</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>ミドリ</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="88" eb="89">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="91" eb="93">
+      <t>ミギヨコ</t>
+    </rPh>
+    <rPh sb="119" eb="120">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="136" eb="137">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="141" eb="142">
+      <t>キ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-edge-download-file.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ファイル操作のためのウィンドウ(エクスプローラ）が開きます。ダウンロードしたGoogleChromeファイルを左側のクイックアクセスにあるデスクトップフォルダに移動しましょう。</t>
+    <rPh sb="4" eb="6">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="55" eb="57">
+      <t>ヒダリガワ</t>
+    </rPh>
+    <rPh sb="80" eb="82">
+      <t>イドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-explorer.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Edgeやエクスプローラのウィンドウを閉じてデスクトップを出すとGoogleChromeファイルがデスクトップにあります。これをクリックしてインストールを開始します。</t>
+    <rPh sb="19" eb="20">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ダ</t>
+    </rPh>
+    <rPh sb="77" eb="79">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-google-chrome-desktop.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「このアプリがデバイスに変更を加えることを許可しますか?」と確認を求められます。「確認済みの発行先: Google LLC」となっていることを確認し、「はい」で進めます。Google Chrome本体のダウンロードが開始されます。</t>
+    <rPh sb="12" eb="14">
+      <t>ヘンコウ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>クワ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>キョカ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>モト</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>ズ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ハッコウ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>サキ</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="80" eb="81">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>ホンタイ</t>
+    </rPh>
+    <rPh sb="108" eb="110">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-chrome-install-check.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>完了するとGoogle Chromeが自動的に起動します。</t>
+    <rPh sb="0" eb="2">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="19" eb="22">
+      <t>ジドウテキ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>キドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11ja-chrome-hello.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">まずGoogle Chromeを入れます。Web上の配布サイトから直接ダウンロードしましょう。
+&lt;a href="https://www.google.com/chrome/" target="_blank" rel="noreferrer"&gt;https://www.google.com/chrome/&lt;/a&gt;
+　（または「Chrome インストール」を検索して出てくるChromeダウンロードページ）
+を開いてください。
+</t>
+    <rPh sb="178" eb="180">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="182" eb="183">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="204" eb="205">
+      <t>ヒラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次のリンクから広島大学オンライン学習支援システム（広大moodle）にアクセスしてください。
+&lt;a href="https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/" target="_blank" rel="noreferrer"&gt;https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/&lt;/a&gt;
+「広大IDでログイン」をクリックしましょう。</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="7" eb="11">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="16" eb="20">
+      <t>ガクシュウシエン</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="199" eb="201">
+      <t>ヒロダイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5438,7 +5480,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5454,7 +5496,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -5462,7 +5504,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -5476,7 +5518,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5510,10 +5552,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5537,17 +5579,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5555,30 +5597,30 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="D9" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5620,7 +5662,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5628,7 +5670,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5644,22 +5686,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5667,7 +5709,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -5683,72 +5725,72 @@
     </row>
     <row r="14" spans="1:4" ht="102" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="D16" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="D17" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D19" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="D20" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -5759,216 +5801,216 @@
     </row>
     <row r="28" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="102" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C42" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="D42" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C48" t="s">
         <v>8</v>
       </c>
       <c r="D48" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -6000,7 +6042,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s" ph="1">
-        <v>310</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6008,7 +6050,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s" ph="1">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6024,7 +6066,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
@@ -6032,7 +6074,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6052,7 +6094,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="57.4" ph="1" x14ac:dyDescent="0.25">
@@ -6060,7 +6102,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>8</v>
@@ -6074,13 +6116,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s" ph="1">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -6088,7 +6130,7 @@
         <v>76</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -6102,7 +6144,7 @@
         <v>8</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="133.9" ph="1" x14ac:dyDescent="0.25">
@@ -6110,29 +6152,29 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s" ph="1">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s" ph="1">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s" ph="1">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="114.75" ph="1" x14ac:dyDescent="0.25">
@@ -6146,7 +6188,7 @@
         <v>8</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="95.65" ph="1" x14ac:dyDescent="0.25">
@@ -6154,13 +6196,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s" ph="1">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
@@ -6168,13 +6210,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s" ph="1">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6182,7 +6224,7 @@
         <v>69</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="114.75" ph="1" x14ac:dyDescent="0.25">
@@ -6196,7 +6238,7 @@
         <v>8</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6204,18 +6246,18 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s" ph="1">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="57.4" ph="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s" ph="1">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D21" t="s" ph="1">
         <v>84</v>
@@ -6226,7 +6268,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s" ph="1">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>8</v>
@@ -6246,18 +6288,18 @@
         <v>8</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s" ph="1">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -6302,7 +6344,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6310,7 +6352,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6326,7 +6368,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
@@ -6334,7 +6376,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6497,7 +6539,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6505,7 +6547,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6521,7 +6563,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6529,7 +6571,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6545,7 +6587,7 @@
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6647,7 +6689,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -6661,7 +6703,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -6689,7 +6731,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -6703,13 +6745,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -6721,10 +6763,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43F54BA-B356-43A4-B76F-707ED0C70724}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6740,7 +6782,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6748,7 +6790,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6764,7 +6806,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -6772,7 +6814,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6788,113 +6830,126 @@
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="D9" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D10" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D11" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="D12" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D13" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
       <c r="B17" s="1" t="s">
-        <v>103</v>
+        <v>305</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>306</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>117</v>
+        <v>307</v>
       </c>
       <c r="D18" t="s">
-        <v>110</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>112</v>
+        <v>309</v>
       </c>
       <c r="D19" t="s">
-        <v>111</v>
+        <v>310</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
       <c r="B20" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
+        <v>311</v>
       </c>
       <c r="D20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D21" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D22" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6909,8 +6964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475A5B02-452F-483B-8907-D83726E9A70E}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6926,7 +6981,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6934,7 +6989,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6950,7 +7005,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6961,7 +7016,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6977,15 +7032,15 @@
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>276</v>
+        <v>318</v>
       </c>
       <c r="D9" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6993,13 +7048,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
@@ -7007,18 +7062,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7026,7 +7081,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7037,7 +7092,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7048,7 +7103,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7064,8 +7119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DD8924-3FAE-44AB-A508-09E9136389D4}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A12" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7081,7 +7136,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7089,7 +7144,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7105,7 +7160,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7113,7 +7168,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7124,12 +7179,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7137,7 +7192,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -7148,7 +7203,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7156,21 +7211,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D12" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7178,18 +7233,18 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7197,13 +7252,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7211,13 +7266,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -7247,8 +7302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7272,7 +7327,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7288,7 +7343,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -7296,7 +7351,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7335,7 +7390,7 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -7359,53 +7414,53 @@
     </row>
     <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="D12" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="D13" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="D14" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="D15" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="D16" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -7416,7 +7471,7 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -7443,29 +7498,29 @@
         <v>4</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D23" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="D24" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7473,7 +7528,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -7517,7 +7572,7 @@
     </row>
     <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -7525,7 +7580,7 @@
     </row>
     <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -7536,7 +7591,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -7550,7 +7605,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -7561,7 +7616,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -7575,7 +7630,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -7589,12 +7644,12 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7602,7 +7657,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -7700,7 +7755,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7716,17 +7771,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7748,7 +7803,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -7804,7 +7859,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
fix starting Chrome  win10(ja)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78E95A1A-DC2E-4191-8F6C-814F4DF20422}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABC7027F-6E80-4975-9BC6-55DD98CD6C0C}"/>
   <bookViews>
-    <workbookView xWindow="6098" yWindow="3472" windowWidth="18225" windowHeight="11873" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52830" yWindow="1410" windowWidth="18225" windowHeight="11880" tabRatio="782" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="317">
   <si>
     <t>header1</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>&lt;h2&gt;この章を始める前に&lt;/h2&gt;</t>
-  </si>
-  <si>
-    <t>win10-2-11.svg</t>
   </si>
   <si>
     <t>無線LANで学内ネットワークに接続できるように設定しましょう。</t>
@@ -4989,19 +4986,6 @@
   </si>
   <si>
     <t>win11ja-chrome-install-check.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>完了するとGoogle Chromeが自動的に起動します。</t>
-    <rPh sb="0" eb="2">
-      <t>カンリョウ</t>
-    </rPh>
-    <rPh sb="19" eb="22">
-      <t>ジドウテキ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>キドウ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5480,7 +5464,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5496,7 +5480,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -5504,7 +5488,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -5518,7 +5502,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5552,10 +5536,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5563,7 +5547,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5579,17 +5563,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5597,30 +5581,30 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5662,7 +5646,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5670,7 +5654,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5686,22 +5670,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5709,7 +5693,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -5725,72 +5709,72 @@
     </row>
     <row r="14" spans="1:4" ht="102" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D16" t="s">
         <v>285</v>
-      </c>
-      <c r="D16" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D17" t="s">
         <v>221</v>
-      </c>
-      <c r="D17" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D19" t="s">
         <v>223</v>
-      </c>
-      <c r="D19" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D20" t="s">
         <v>256</v>
-      </c>
-      <c r="D20" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -5801,216 +5785,216 @@
     </row>
     <row r="28" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="102" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C48" t="s">
         <v>8</v>
       </c>
       <c r="D48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -6042,7 +6026,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s" ph="1">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6050,7 +6034,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s" ph="1">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6066,7 +6050,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
@@ -6074,7 +6058,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6094,7 +6078,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="57.4" ph="1" x14ac:dyDescent="0.25">
@@ -6102,13 +6086,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -6116,21 +6100,21 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s" ph="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s" ph="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -6138,13 +6122,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s" ph="1">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="133.9" ph="1" x14ac:dyDescent="0.25">
@@ -6152,29 +6136,29 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s" ph="1">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s" ph="1">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s" ph="1">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="114.75" ph="1" x14ac:dyDescent="0.25">
@@ -6182,13 +6166,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s" ph="1">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="95.65" ph="1" x14ac:dyDescent="0.25">
@@ -6196,13 +6180,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s" ph="1">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
@@ -6210,21 +6194,21 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s" ph="1">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s" ph="1">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="114.75" ph="1" x14ac:dyDescent="0.25">
@@ -6232,13 +6216,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s" ph="1">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6246,21 +6230,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s" ph="1">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="57.4" ph="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s" ph="1">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="95.65" ph="1" x14ac:dyDescent="0.25">
@@ -6268,13 +6252,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s" ph="1">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="133.9" ph="1" x14ac:dyDescent="0.25">
@@ -6282,24 +6266,24 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s" ph="1">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s" ph="1">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -6307,13 +6291,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s" ph="1">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -6344,7 +6328,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6352,7 +6336,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6368,7 +6352,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
@@ -6376,7 +6360,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6390,7 +6374,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -6404,7 +6388,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -6418,7 +6402,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -6432,7 +6416,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -6446,7 +6430,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -6460,7 +6444,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -6474,7 +6458,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6488,7 +6472,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6502,7 +6486,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -6539,7 +6523,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6547,7 +6531,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6563,7 +6547,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6571,7 +6555,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6587,12 +6571,12 @@
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6600,13 +6584,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6614,13 +6598,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6628,13 +6612,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6642,13 +6626,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6656,18 +6640,18 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6675,13 +6659,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6689,13 +6673,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
@@ -6703,13 +6687,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -6717,13 +6701,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6731,13 +6715,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6745,13 +6729,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -6763,10 +6747,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43F54BA-B356-43A4-B76F-707ED0C70724}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6782,7 +6766,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6790,7 +6774,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6806,7 +6790,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -6814,7 +6798,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6830,65 +6814,65 @@
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D10" t="s">
         <v>289</v>
-      </c>
-      <c r="D10" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D11" t="s">
         <v>291</v>
-      </c>
-      <c r="D11" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D12" t="s">
         <v>293</v>
-      </c>
-      <c r="D12" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6896,61 +6880,50 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D17" t="s">
         <v>305</v>
-      </c>
-      <c r="D17" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D18" t="s">
         <v>307</v>
-      </c>
-      <c r="D18" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D19" t="s">
         <v>309</v>
-      </c>
-      <c r="D19" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="D20" t="s">
         <v>311</v>
-      </c>
-      <c r="D20" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D21" t="s">
         <v>313</v>
       </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="22" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" t="s">
         <v>314</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="D22" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -6981,7 +6954,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6989,7 +6962,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7005,7 +6978,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -7016,7 +6989,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7032,15 +7005,15 @@
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7048,13 +7021,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>200</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
@@ -7062,18 +7035,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>202</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7081,7 +7054,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7092,7 +7065,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7103,7 +7076,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7136,7 +7109,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7144,7 +7117,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7160,7 +7133,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7168,7 +7141,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7179,12 +7152,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7192,18 +7165,18 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7211,21 +7184,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" t="s">
         <v>210</v>
-      </c>
-      <c r="D12" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7233,18 +7206,18 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>212</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7252,13 +7225,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>214</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7266,13 +7239,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -7302,7 +7275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -7319,7 +7292,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7327,7 +7300,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7343,7 +7316,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -7351,7 +7324,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7362,7 +7335,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7370,13 +7343,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>43</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7384,18 +7357,18 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7414,69 +7387,69 @@
     </row>
     <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D12" t="s">
         <v>285</v>
-      </c>
-      <c r="D12" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D13" t="s">
         <v>221</v>
-      </c>
-      <c r="D13" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D15" t="s">
         <v>225</v>
-      </c>
-      <c r="D15" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>228</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -7498,29 +7471,29 @@
         <v>4</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
         <v>231</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D24" t="s">
         <v>281</v>
-      </c>
-      <c r="D24" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7528,13 +7501,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7542,18 +7515,18 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>50</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -7572,7 +7545,7 @@
     </row>
     <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -7580,7 +7553,7 @@
     </row>
     <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -7591,13 +7564,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7605,7 +7578,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -7616,13 +7589,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7630,13 +7603,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7644,12 +7617,12 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7657,7 +7630,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -7671,13 +7644,13 @@
         <v>4</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -7685,21 +7658,21 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7707,13 +7680,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="4:4" ht="19.149999999999999" x14ac:dyDescent="0.25">
@@ -7747,7 +7720,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7755,7 +7728,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7771,17 +7744,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7789,13 +7762,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
@@ -7803,13 +7776,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7817,13 +7790,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7831,13 +7804,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7845,13 +7818,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7859,13 +7832,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7873,21 +7846,21 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7895,7 +7868,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -7909,13 +7882,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix some message in win10(ja)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABC7027F-6E80-4975-9BC6-55DD98CD6C0C}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66726D51-3ECD-4F27-936F-7B359CBB8E08}"/>
   <bookViews>
-    <workbookView xWindow="52830" yWindow="1410" windowWidth="18225" windowHeight="11880" tabRatio="782" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1395" yWindow="2835" windowWidth="18225" windowHeight="11873" tabRatio="782" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="318">
   <si>
     <t>header1</t>
   </si>
@@ -140,11 +140,6 @@
   </si>
   <si>
     <t xml:space="preserve">「更新とセキュリティ」をクリックします。
-  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">「Windowsの更新時に他のMicrosoft製品の更新プログラムも入手します」にチェックを入れてください。これにより、Officeも自動更新されるようになります。
-画面左上の「←」をクリックして、前の画面に戻ってください。
   </t>
   </si>
   <si>
@@ -191,10 +186,6 @@
   </si>
   <si>
     <t>win10-6-11.svg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">閲覧が済んだら、画面右上の「ログアウト」をクリックしましょう。
-  </t>
   </si>
   <si>
     <t>win10-6-12.svg</t>
@@ -248,14 +239,6 @@
 詳細はメディアセンターWebサイトの&lt;a href="https://www.media.hiroshima-u.ac.jp/services/print/webprint"&gt;「Webプリントサービス」&lt;/a&gt;
 で。
   </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">左メニューから「地域と言語」をクリックしてください。
- 真ん中の「優先する言語」から「日本語」をクリックしてください。 その後表示される「オプション」をクリックしてください。   </t>
-    <rPh sb="33" eb="35">
-      <t>ユウセン</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -315,12 +298,6 @@
     <t>「パスワードの確認」として、先ほど決めたパスワードをもう一度入力します。</t>
   </si>
   <si>
-    <t xml:space="preserve">自動アップデートのタイミング以外にDefenderを更新する方法について説明します。Windowsの自動更新機能で、Defenderは最新状態にたもたれます。しかし、緊急の脆弱性が発表された場合など、すぐに更新した方が良い時もあります。
-ウィンドウ左のリストから「Windows セキュリティ」をクリックし、「Windows セキュリティを開く」をクリックします。
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">この画面で「更新プログラムのチェック」をクリックすると、脅威の定義の新しいものが出ているか確認を行い、あればそれを入手します。普段は、定期的に自動で確認されているので、これを押す必要はありません。
   </t>
     <phoneticPr fontId="1"/>
@@ -477,22 +454,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">「バージョン情報」という名前のウィンドウが開きます。中にPCに関する情報がたくさん表示されています。
-「Windowsの仕様」をみると「エディション」のところに「Windows 10 Pro」とありますね。これがOSの種類です。「バージョン」のところには詳細なバージョン番号（いつの時点のOSか）が書かれています。&lt;span class="check"&gt;check-1&lt;span&gt;&lt;/span&gt;
-&lt;/span&gt;
-その上の方に「デバイスの仕様」がありますね。ここの「システムの種類」を見ると、OSのビット数がわかります。&amp;quot;64ビットオペレーティングシステム&amp;quot; とあります。この場合は64ビットですね。二進法で64桁のデータを一度に処理できるOSであるということを示しています。&lt;span class="check"&gt;check-2&lt;span&gt;&lt;/span&gt;
-&lt;/span&gt;
-その上に「実装RAM」と書かれたところがあります。ここを見ると、主記憶装置（メインメモリ）の容量がわかります。この場合は8GB（ギガバイト）ですね。この容量が大きいほど、大量のデータを一括して扱えたり、多くのプログラムを同時に動作させたりすることがスムーズにできるようになります。
-  </t>
-    <rPh sb="298" eb="300">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="455" eb="457">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">最後にバッテリー駆動時間を確認しましょう。
 画面下のタスクバーのバッテリーアイコンをクリックしてください。すると、バッテリー残量がパーセント表示され、およそあと何時間利用できるかの推定値が表示されます。
 100%充電時のここの残り時間表示が、あなたのPCのバッテリー駆動時間の推定値ということになります。（例：80%で「残り6時間」であれば、6÷0.8=7.5なので、バッテリー駆動時間は7.5時間）
@@ -537,14 +498,6 @@
     </rPh>
     <rPh sb="157" eb="158">
       <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">左メニューの真ん中あたりにある「レイアウトを変更する」をクリックしてください。
- すると青い画面がでますので，「英語キーボード(101/102キー）」となっているのを「日本語キーボード(106/109キー）」に変更し、「サインアウト」をクリックしてください。 これでキーボードが日本語の設定になりました。 一度サインアウトしてから、このパソコンのユーザ名とパスワードでもう一度入り直してください。   </t>
-    <rPh sb="176" eb="177">
-      <t>メイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -717,56 +670,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">「ウイルスと脅威の防止」をクリックしましょう。
-&lt;p class="spl"&gt;※この部分に黄色のアイコンが出ている場合があります。これはランサムウェアに備えるためのOneDriveへのデータバックアップが設定されていないことを示していますが、この講習会ではまだ設定しません。気になるようでしたら「無視する」をクリックしてください。となおデータバックアップ設定はこのメニューからいつでもできます。&lt;/p&gt;
-  </t>
-    <rPh sb="42" eb="44">
-      <t>ブブン</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>キイロ</t>
-    </rPh>
-    <rPh sb="53" eb="54">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="57" eb="59">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="113" eb="114">
-      <t>シメ</t>
-    </rPh>
-    <rPh sb="123" eb="126">
-      <t>コウシュウカイ</t>
-    </rPh>
-    <rPh sb="130" eb="132">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="137" eb="138">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="148" eb="150">
-      <t>ムシ</t>
-    </rPh>
-    <rPh sb="177" eb="179">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">設定にはいる前に、広島大学で情報サービスを使うときに必要がIDが二種類あることを確認しましょう。二種類とも学生番号をもとにしています。
-一つは「広大ID」。これは学生番号と同じ文字列です。もう一つはメディアセンターの「アカウント名(IMCアカウント名)」です。こちらは、先頭の一文字を小文字にしたものになっています。
-対応するパスワードは、どちらも共通です。「広大パスワード」と呼んでいます。学生証と一緒に配布されます。
-IMCアカウント名に「@hiroshima-u.ac.jp」をつけたものを広大メールアドレスと呼んでいます。このメールアドレスは、広大学生として公式のものになります。事務連絡、教員からの連絡等ありますので、日常的にチェックするようにしましょう。チェックする方法は、第５章で紹介します。
-  </t>
-    <rPh sb="343" eb="344">
-      <t>ダイ</t>
-    </rPh>
-    <rPh sb="345" eb="346">
-      <t>ショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">Defenderでは、ウイルスやスパイウェアその他の悪意を持つプログラム全般を「脅威」とし、それらを判別するルールを保存したファイルを「脅威の定義」と呼んでいます。
 「ウイルスと脅威の防止の更新」の下に、前回いつ「脅威の定義」が更新されたかが書かれています。&lt;span class="check"&gt;check-5,6&lt;/span&gt;
 &lt;p class="spl"&gt;※ここで「他のプログラム（ウィルスバスター、マカフィーリブセーフなど）が有効になっている」という旨の表示がされた場合、ウィルス対策はその表示されたプログラムが行っています。その場合はこの下の項目は飛ばして、別途そのプログラムの「利用期限」と「更新方法」「フルスキャンの実施方法」を確認してください。とくに「利用期限」が切れてウィルス対策に穴ができることがないよう注意してください。あとで Defender の利用に戻すこともできます。&lt;/p&gt;
@@ -1064,70 +967,6 @@
     <t>Microsoft Office を使えるようにしましょう。</t>
     <rPh sb="18" eb="19">
       <t>ツカ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>広島大学では、学生の皆さんの個人所有のPCにMicrosoft Office365 Pro Plusを5台までインストールすることができる包括ライセンスを結んでいます。ただし、卒業して学籍を失うと、利用することができなくなってしまいます。ご自分で別途Microsoft Officeを購入してインストールした方は、この章を飛ばしていただいて構いません。</t>
-    <rPh sb="0" eb="2">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>ミナ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>ショユウ</t>
-    </rPh>
-    <rPh sb="52" eb="53">
-      <t>ダイ</t>
-    </rPh>
-    <rPh sb="69" eb="71">
-      <t>ホウカツ</t>
-    </rPh>
-    <rPh sb="77" eb="78">
-      <t>ムス</t>
-    </rPh>
-    <rPh sb="88" eb="90">
-      <t>ソツギョウ</t>
-    </rPh>
-    <rPh sb="92" eb="94">
-      <t>ガクセキ</t>
-    </rPh>
-    <rPh sb="95" eb="96">
-      <t>ウシナ</t>
-    </rPh>
-    <rPh sb="99" eb="101">
-      <t>リヨウ</t>
-    </rPh>
-    <rPh sb="120" eb="122">
-      <t>ジブン</t>
-    </rPh>
-    <rPh sb="123" eb="125">
-      <t>ベット</t>
-    </rPh>
-    <rPh sb="142" eb="144">
-      <t>コウニュウ</t>
-    </rPh>
-    <rPh sb="154" eb="155">
-      <t>カタ</t>
-    </rPh>
-    <rPh sb="159" eb="160">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="161" eb="162">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="170" eb="171">
-      <t>カマ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1369,25 +1208,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;p class="spl"&gt;※学生番号と、学生番号と一緒にもらえる「広大パスワード」が必要です。&lt;/p&gt;</t>
-    <rPh sb="16" eb="18">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t>イッショ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="44" eb="46">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>包括ライセンスでMicrosoft Office365 Pro Plusをインストールした場合は、Microsoft Teamsは既にインストールされている筈です。検索ウィンドウで「Teams」を検索すれば出てくる筈です。
 もし別途Officeを購入したため、Microsoft Teamsがまだ入っていないという場合は、https://www.microsoft.com/ja-jp/microsoft-teams/download-app からダウンロードしてインストールしてください(Office365と違ってアカウントにサインインしなくてもダウンロードできます)。また、iOS機器(iPhone, iPad)やAndroid機器でも動きますが、ここではPCでの確認手順を説明します。</t>
     <rPh sb="0" eb="2">
@@ -2426,73 +2246,6 @@
     </rPh>
     <rPh sb="266" eb="268">
       <t>サンコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">最初に、目の前のPCがどんなものなのかを確認しましょう。PCの処理能力や容量の目安になるさまざまな要素を「スペック」と呼ぶことがあります。ここでは以下のスペックを確認しましょう。
-&lt;ol&gt;&lt;li&gt; OSのバージョン &lt;/li&gt;
-&lt;li&gt; メモリ容量（主記憶容量） &lt;/li&gt;
-&lt;li&gt; HDD/SSD容量（副記憶容量） &lt;/li&gt;
-&lt;li&gt; バッテリー駆動時間 &lt;/li&gt;
-&lt;/ol&gt;
-この章は広島大学の学生番号がわかる前に実施することができます。 
- </t>
-    <rPh sb="204" eb="206">
-      <t>バンゴウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>この章では、Wi-Fiで広島大学の学内ネットワークに接続するための設定を行います。このテキストは自宅にネットワークがなく、大学にしかネットワークがない場合の順序で書いてあります。以下の手順はアカウントに関連したサービスが全て利用可能になる4/2 以降に実施してください。
-自宅などにインターネット接続環境がある場合は、「自宅ネットワークでの自習形式」のテキストを参照してください。</t>
-    <rPh sb="2" eb="3">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ガクナイ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>ジタク</t>
-    </rPh>
-    <rPh sb="61" eb="63">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="75" eb="77">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="78" eb="80">
-      <t>ジュンジョ</t>
-    </rPh>
-    <rPh sb="81" eb="82">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="160" eb="162">
-      <t>ジタク</t>
-    </rPh>
-    <rPh sb="170" eb="172">
-      <t>ジシュウ</t>
-    </rPh>
-    <rPh sb="172" eb="174">
-      <t>ケイシキ</t>
-    </rPh>
-    <rPh sb="181" eb="183">
-      <t>サンショウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -2798,141 +2551,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">ログインしたら、この画面が出ます。&lt;span class="check"&gt;check-8&lt;/span&gt;
-真ん中に見える「コース概要」に、あなたがアクセスできるコースが表示されています。これらは、あなたの履修課目に関する授業支援や、広島大学において自習すべき教材などのコースです。（この図は在学生向けの一例で、新入生に表示されるものとは異なります）
-新入生向けに共通で表示されるものを簡単に説明すると：
-&lt;dl&gt;
-&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
-&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届」を提出する必要があります。このコースでは、点検届が提出できます。&lt;strong&gt;このテキストによる設定・点検を済ませたあと、できるだけ早くにこのコースを開いて点検届を提出してください。&lt;/strong&gt;&lt;/dd&gt;
-&lt;dt&gt;MFA21 MFA設定ガイド&lt;/dt&gt;
-&lt;dd&gt;広島大学ではパスワード窃取・アカウント乗っ取りの防止策として、広大IDを持つ全ての構成員に対しIMCアカウントおよび広大IDの多要素認証（MFA）設定を義務付けています。この「MFA設定ガイド」で、広島大学でMFA設定を行うための手順を説明しています&lt;/dd&gt; &lt;/dl&gt;
-</t>
-    <rPh sb="56" eb="57">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>ガイヨウ</t>
-    </rPh>
-    <rPh sb="101" eb="103">
-      <t>リシュウ</t>
-    </rPh>
-    <rPh sb="103" eb="105">
-      <t>カモク</t>
-    </rPh>
-    <rPh sb="106" eb="107">
-      <t>カン</t>
-    </rPh>
-    <rPh sb="109" eb="111">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="111" eb="113">
-      <t>シエン</t>
-    </rPh>
-    <rPh sb="115" eb="117">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="117" eb="119">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="123" eb="125">
-      <t>ジシュウ</t>
-    </rPh>
-    <rPh sb="128" eb="130">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="147" eb="148">
-      <t>ム</t>
-    </rPh>
-    <rPh sb="174" eb="177">
-      <t>シンニュウセイ</t>
-    </rPh>
-    <rPh sb="177" eb="178">
-      <t>ム</t>
-    </rPh>
-    <rPh sb="180" eb="182">
-      <t>キョウツウ</t>
-    </rPh>
-    <rPh sb="183" eb="185">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="330" eb="332">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="333" eb="335">
-      <t>テンケン</t>
-    </rPh>
-    <rPh sb="336" eb="337">
-      <t>ス</t>
-    </rPh>
-    <rPh sb="348" eb="349">
-      <t>ハヤ</t>
-    </rPh>
-    <rPh sb="357" eb="358">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="401" eb="403">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="416" eb="420">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="427" eb="429">
-      <t>セッシュ</t>
-    </rPh>
-    <rPh sb="435" eb="436">
-      <t>ノ</t>
-    </rPh>
-    <rPh sb="437" eb="438">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="447" eb="449">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="452" eb="453">
-      <t>モ</t>
-    </rPh>
-    <rPh sb="454" eb="455">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="457" eb="460">
-      <t>コウセイイン</t>
-    </rPh>
-    <rPh sb="461" eb="462">
-      <t>タイ</t>
-    </rPh>
-    <rPh sb="474" eb="476">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="479" eb="484">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="489" eb="491">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="492" eb="495">
-      <t>ギムヅ</t>
-    </rPh>
-    <rPh sb="507" eb="509">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="515" eb="519">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="523" eb="525">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="526" eb="527">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="531" eb="533">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="534" eb="536">
-      <t>セツメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>moodle-top.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -3177,37 +2795,6 @@
     <t>win11ja-momiji-before-login0.png</t>
   </si>
   <si>
-    <t>IMCアカウントを「@hiroshima-u.ac.jp」つきで入力し、さらにパスワードも入力します。このサイトはMicrosoftのサイトなので、「@hiroshima-u.ac.jp」がついていないと貴方の学生番号がどの大学のものか判らないため、「@hiroshima-u.ac.jp」を加える必要があります。</t>
-    <rPh sb="32" eb="34">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="102" eb="104">
-      <t>アナタ</t>
-    </rPh>
-    <rPh sb="105" eb="107">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="107" eb="109">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="112" eb="114">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="118" eb="119">
-      <t>ワカ</t>
-    </rPh>
-    <rPh sb="146" eb="147">
-      <t>クワ</t>
-    </rPh>
-    <rPh sb="149" eb="151">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win11ja-ms-signin2.png</t>
   </si>
   <si>
@@ -3242,35 +2829,7 @@
     <t>win11ja-ms-signin3.png</t>
   </si>
   <si>
-    <t>Office365のページの左側にブラウザ内で使用できるアプリのアイコンが並びます。「O」の文字があるOutlook for Webをクリックします。</t>
-    <rPh sb="14" eb="16">
-      <t>ヒダリガワ</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>ナイ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>ナラ</t>
-    </rPh>
-    <rPh sb="46" eb="48">
-      <t>モジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11ja-office365-outlook-start.png</t>
-  </si>
-  <si>
     <t>win11ja-outlook-for-web.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">次に、Office365のオンラインストレージのOneDriveを見て見ましょう。画面左上のつぶつぶをクリックします。
-するとOffice365で使用できるアプリケーション一覧が表示されます。その中にある「OneDrive」をクリックしましょう
-  </t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>win11ja-office365-from-outlook-to-onedrive.png</t>
@@ -3286,16 +2845,6 @@
   </si>
   <si>
     <t>win11ja-momiji-before-login.png</t>
-  </si>
-  <si>
-    <t>広大IDとパスワードを入力し、「ログイン」をクリックします。</t>
-    <rPh sb="0" eb="2">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>ニュウリョク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>FRESTA-TEXT-2022 Win10 chap.7</t>
@@ -3444,13 +2993,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check-13&lt;/span&gt;
-履修登録をしたり、成績を確認することができます。
-また「掲示」では、授業や学部からの連絡が表示されます。
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>FRESTA-TEXT-2022 Win10 conclusion</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -3516,84 +3058,6 @@
       <t>テンケントドケ</t>
     </rPh>
     <rPh sb="8" eb="10">
-      <t>テイシュツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>このテキストの第１章からここまで順に進んでいれば、点検届チェックリストがすべてチェックできているはずです。
-&lt;strong&gt;Moodleの「ノートパソコン点検届」コースを開いて、点検届を提出しましょう！&lt;/strong&gt;</t>
-    <rPh sb="7" eb="8">
-      <t>ダイ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>ジュン</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>テンケン</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>トドケ</t>
-    </rPh>
-    <rPh sb="77" eb="79">
-      <t>テンケン</t>
-    </rPh>
-    <rPh sb="79" eb="80">
-      <t>トドケ</t>
-    </rPh>
-    <rPh sb="85" eb="86">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="89" eb="91">
-      <t>テンケン</t>
-    </rPh>
-    <rPh sb="91" eb="92">
-      <t>トドケ</t>
-    </rPh>
-    <rPh sb="93" eb="95">
-      <t>テイシュツツカバアイスス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>次のリンクから広島大学オンライン学習支援システム（Moodle）にアクセスしてください。
-&lt;a href="https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/"&gt;https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/&lt;/a&gt;
-「広大IDでログイン」をクリックしてログインしましょう。</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="7" eb="11">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="16" eb="20">
-      <t>ガクシュウシエン</t>
-    </rPh>
-    <rPh sb="164" eb="166">
-      <t>ヒロダイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;strong&gt;「コース概要」の中にある「ノートパソコン点検届」から、点検届を提出してください。&lt;/strong&gt;</t>
-    <rPh sb="12" eb="14">
-      <t>ガイヨウ</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="28" eb="31">
-      <t>テンケントドケ</t>
-    </rPh>
-    <rPh sb="35" eb="38">
-      <t>テンケントドケ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
       <t>テイシュツ</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -3802,32 +3266,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Office365にサインインした状態になります。&lt;span class="check"&gt;check-11&lt;/span&gt;
-ここでは左右を縮めて表示していますが、画面の右側のほうに「Officeのインストール」というメニューがありますので、そこからOffice 365アプリを選びます。</t>
-    <rPh sb="17" eb="19">
-      <t>ジョウタイ</t>
-    </rPh>
-    <rPh sb="65" eb="67">
-      <t>サユウ</t>
-    </rPh>
-    <rPh sb="68" eb="69">
-      <t>チヂ</t>
-    </rPh>
-    <rPh sb="71" eb="73">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="80" eb="82">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>ミギガワ</t>
-    </rPh>
-    <rPh sb="137" eb="138">
-      <t>エラ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ch5-download-from-portal-office365.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -4176,34 +3614,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>広大moodleの「コース概要」の中の「MFA21 MFA設定ガイド」をクリックして、まず表示される「広大IDとIMCアカウントの概要」を読んでください。</t>
-    <rPh sb="0" eb="2">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>ガイヨウ</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="51" eb="53">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="65" eb="67">
-      <t>ガイヨウ</t>
-    </rPh>
-    <rPh sb="69" eb="70">
-      <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>さらに下の方にある「IMCアカウントのMFA設定」の説明に従ってIMCアカウントの多要素認証（MFA）設定を行ってください。&lt;span class="check"&gt;check-9&lt;/span&gt;</t>
     <rPh sb="3" eb="4">
       <t>シタ</t>
@@ -4233,60 +3643,6 @@
   </si>
   <si>
     <t>win10ja-search-excel.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>※ ここまでの実習の中で、広島大学には２つのオンライン学習支援システム「広大moodle」「Bb9」があることに気づかれたと思います。
-広島大学では今年度「広大moodle」「Bb9」の２つのオンライン学習支援システムを併用します。来年度からは「広大moodle」に一本化する予定です。
-しばらく面倒をおかけしますが、ご了解ください。</t>
-    <rPh sb="7" eb="9">
-      <t>ジッシュウ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="13" eb="17">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="27" eb="31">
-      <t>ガクシュウシエン</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="56" eb="57">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="62" eb="63">
-      <t>オモ</t>
-    </rPh>
-    <rPh sb="78" eb="80">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="101" eb="105">
-      <t>ガクシュウシエン</t>
-    </rPh>
-    <rPh sb="110" eb="112">
-      <t>ヘイヨウ</t>
-    </rPh>
-    <rPh sb="116" eb="119">
-      <t>ライネンド</t>
-    </rPh>
-    <rPh sb="123" eb="125">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="133" eb="136">
-      <t>イッポンカ</t>
-    </rPh>
-    <rPh sb="138" eb="140">
-      <t>ヨテイ</t>
-    </rPh>
-    <rPh sb="148" eb="150">
-      <t>メンドウ</t>
-    </rPh>
-    <rPh sb="160" eb="162">
-      <t>リョウカイ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -4841,28 +4197,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Googleのダウンロードページにジャンプしました。Google Chromeのブラウザ内部のデータをGoogleに送信しても良いかという許可チェックボックスがありますが、このチェックを外してダウンロードを行います。</t>
-    <rPh sb="44" eb="46">
-      <t>ナイブ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>ソウシン</t>
-    </rPh>
-    <rPh sb="63" eb="64">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="69" eb="71">
-      <t>キョカ</t>
-    </rPh>
-    <rPh sb="93" eb="94">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="103" eb="104">
-      <t>オコナ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win11ja-google-chrome-download-page.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -5030,12 +4364,825 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t xml:space="preserve">「詳細情報」という名前のウィンドウが開きます。中にPCに関する情報がたくさん表示されています。
+「Wind+B13owsの仕様」をみると「エディション」のところに「Windows 10 Pro」とありますね。これがOSの種類です。「バージョン」のところには詳細なバージョン番号（いつの時点のOSか）が書かれています。&lt;span class="check"&gt;check-1&lt;span&gt;&lt;/span&gt;
+&lt;/span&gt;
+その上の方に「デバイスの仕様」がありますね。ここの「システムの種類」を見ると、OSのビット数がわかります。&amp;quot;64ビットオペレーティングシステム&amp;quot; とあります。この場合は64ビットですね。二進法で64桁のデータを一度に処理できるOSであるということを示しています。&lt;span class="check"&gt;check-2&lt;span&gt;&lt;/span&gt;
+&lt;/span&gt;
+その上に「実装RAM」と書かれたところがあります。ここを見ると、主記憶装置（メインメモリ）の容量がわかります。この場合は8GB（ギガバイト）ですね。この容量が大きいほど、大量のデータを一括して扱えたり、多くのプログラムを同時に動作させたりすることがスムーズにできるようになります。
+  </t>
+    <rPh sb="1" eb="3">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="299" eb="301">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="456" eb="458">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">左メニューから「言語」（または「地域と言語」）をクリックしてください。
+ 真ん中の「優先する言語」から「日本語」をクリックしてください。 その後表示される「オプション」をクリックしてください。   </t>
+    <rPh sb="8" eb="10">
+      <t>ゲンゴ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ユウセン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">最初に、目の前のPCがどんなものなのかを確認しましょう。PCの処理能力や容量の目安になるさまざまな要素を「スペック」と呼ぶことがあります。ここでは以下のスペックを確認しましょう。
+&lt;ol&gt;&lt;li&gt; OSのバージョン &lt;/li&gt;
+&lt;li&gt; メモリ容量（主記憶容量） &lt;/li&gt;
+&lt;li&gt; HDD/SSD容量（副記憶容量） &lt;/li&gt;
+&lt;li&gt; バッテリー駆動時間 &lt;/li&gt;
+&lt;/ol&gt;
+この章は広島大学の学生番号がわかる前に実施することができます。 
+※ Windows10はバージョン番号が同じでもバリエーションがあったり、出荷時期によって違いがあります。以下の手順にある画面の表現が少し異なることもありますが、適当に読み替えて作業を進めてください。
+ </t>
+    <rPh sb="204" eb="206">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="307" eb="309">
+      <t>テキトウ</t>
+    </rPh>
+    <rPh sb="310" eb="311">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="312" eb="313">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="315" eb="317">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="318" eb="319">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">左メニューの真ん中あたりにある「レイアウトを変更する」をクリックしてください。
+ すると青い画面がでますので，「英語キーボード(101/102キー）」となっているのを「日本語キーボード(106/109キー）」に変更し、「今すぐ再起動する」（または「サインアウト」）をクリックしてください。 これでパソコンを再起動したあと、キーボードが日本語の設定になります。   </t>
+    <rPh sb="110" eb="111">
+      <t>イマ</t>
+    </rPh>
+    <rPh sb="113" eb="116">
+      <t>サイキドウ</t>
+    </rPh>
+    <rPh sb="153" eb="156">
+      <t>サイキドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「Windowsの更新時に他のMicrosoft製品の更新プログラムを受け取る」にチェックを入れてください。これにより、Officeも自動更新されるようになります。
+画面左上の「←」をクリックして、前の画面に戻ってください。
+  </t>
+    <rPh sb="35" eb="36">
+      <t>ウ</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>ト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「ウイルスと脅威の防止」をクリックしましょう。
+&lt;p class="spl"&gt;※この部分に黄色のアイコンが出ている場合があります。また、すぐ下に「OneDriveのセットアップ」ボタンが出ている場合があります。これらはランサムウェアに備えるためのOneDriveへのデータバックアップを設定するための表示ですが、この実習ではまだ設定しません。気になるようでしたら「無視」をクリックしてください。なお、データバックアップ設定はこのメニューからいつでもできます。&lt;/p&gt;
+  </t>
+    <rPh sb="42" eb="44">
+      <t>ブブン</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>キイロ</t>
+    </rPh>
+    <rPh sb="53" eb="54">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="143" eb="145">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="150" eb="152">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="158" eb="160">
+      <t>ジッシュウ</t>
+    </rPh>
+    <rPh sb="164" eb="166">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="171" eb="172">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="182" eb="184">
+      <t>ムシ</t>
+    </rPh>
+    <rPh sb="209" eb="211">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">自動アップデートのタイミング以外にDefenderを更新する方法について説明します。Windowsの自動更新機能で、Defenderは最新状態に保たれます。しかし、緊急の脆弱性が発表された場合など、すぐに更新した方が良い時もあります。
+ウィンドウ左のリストから「Windows セキュリティ」をクリックし、「Windows セキュリティを開く」をクリックします。
+  </t>
+    <rPh sb="72" eb="73">
+      <t>タモ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Googleのダウンロードページにジャンプしました。Google Chromeのブラウザ内部のデータをGoogleに送信しても良いかという許可チェックボックスがありますが、このチェックを外してダウンロードを行います。
+※ Edgeを使って作業している場合、右上に「EdgeのほうがChromeより良い」という旨の広告メッセージが出ますが、いまは無視してください。</t>
+    <rPh sb="44" eb="46">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>ソウシン</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>キョカ</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="103" eb="104">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="116" eb="117">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="119" eb="121">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="125" eb="127">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="128" eb="130">
+      <t>ミギウエ</t>
+    </rPh>
+    <rPh sb="148" eb="149">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="154" eb="155">
+      <t>ムネ</t>
+    </rPh>
+    <rPh sb="164" eb="165">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="172" eb="174">
+      <t>ムシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広大moodleの「コースツリー」の中の「MFA設定ガイド」をクリックすると、コースのトップページが表示されます。少し下の方にスクロールして表示される「広大IDとIMCアカウントの概要」を、まず読んでください。</t>
+    <rPh sb="0" eb="2">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="57" eb="58">
+      <t>スコ</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="90" eb="92">
+      <t>ガイヨウ</t>
+    </rPh>
+    <rPh sb="97" eb="98">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ログインしたら、この画面（ダッシュボード）が出ます。&lt;span class="check"&gt;check-8&lt;/span&gt;
+真ん中に見える「コースツリー」に、あなたがアクセスできるコースが表示されています。これらは、あなたの履修課目に関する授業支援や、広島大学において自習すべき教材などのコースです。（この図は在学生向けの一例で、新入生に表示されるものとは異なります）
+新入生向けに共通で表示されるものを簡単に説明すると：
+&lt;dl&gt;
+&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
+&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届」を提出する必要があります。このコースでは、点検届が提出できます。&lt;strong&gt;このテキストによる設定・点検を済ませたあと、できるだけ早くにこのコースを開いて点検届を提出してください。&lt;/strong&gt;&lt;/dd&gt;
+&lt;dt&gt;MFA設定ガイド&lt;/dt&gt;
+&lt;dd&gt;広島大学ではパスワード窃取・アカウント乗っ取りの防止策として、広大IDを持つ全ての構成員に対しIMCアカウントおよび広大IDの多要素認証（MFA）設定を義務付けています。この「MFA設定ガイド」で、広島大学でMFA設定を行うための手順を説明しています&lt;/dd&gt; &lt;/dl&gt;
+</t>
+    <rPh sb="65" eb="66">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="111" eb="113">
+      <t>リシュウ</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>カモク</t>
+    </rPh>
+    <rPh sb="116" eb="117">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="119" eb="121">
+      <t>ジュギョウ</t>
+    </rPh>
+    <rPh sb="121" eb="123">
+      <t>シエン</t>
+    </rPh>
+    <rPh sb="125" eb="127">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="127" eb="129">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="133" eb="135">
+      <t>ジシュウ</t>
+    </rPh>
+    <rPh sb="138" eb="140">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="157" eb="158">
+      <t>ム</t>
+    </rPh>
+    <rPh sb="184" eb="187">
+      <t>シンニュウセイ</t>
+    </rPh>
+    <rPh sb="187" eb="188">
+      <t>ム</t>
+    </rPh>
+    <rPh sb="190" eb="192">
+      <t>キョウツウ</t>
+    </rPh>
+    <rPh sb="193" eb="195">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="340" eb="342">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="343" eb="345">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="346" eb="347">
+      <t>ス</t>
+    </rPh>
+    <rPh sb="358" eb="359">
+      <t>ハヤ</t>
+    </rPh>
+    <rPh sb="367" eb="368">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="405" eb="407">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="420" eb="424">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="431" eb="433">
+      <t>セッシュ</t>
+    </rPh>
+    <rPh sb="439" eb="440">
+      <t>ノ</t>
+    </rPh>
+    <rPh sb="441" eb="442">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="451" eb="453">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="456" eb="457">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="458" eb="459">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="461" eb="464">
+      <t>コウセイイン</t>
+    </rPh>
+    <rPh sb="465" eb="466">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="478" eb="480">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="483" eb="488">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="493" eb="495">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="496" eb="499">
+      <t>ギムヅ</t>
+    </rPh>
+    <rPh sb="511" eb="513">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="519" eb="523">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="527" eb="529">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="530" eb="531">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="535" eb="537">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="538" eb="540">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広島大学では、学生の皆さんの個人所有のPCにMicrosoft 365 Apps for enterprise（Office365 Pro Plus）を5台までインストールすることができる包括ライセンスを結んでいます。ただし、卒業して学籍を失うと、利用することができなくなってしまいます。ご自分で別途Microsoft Officeを購入してインストールした方は、この章を飛ばしていただいて構いません。</t>
+    <rPh sb="0" eb="2">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ミナ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ショユウ</t>
+    </rPh>
+    <rPh sb="77" eb="78">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>ホウカツ</t>
+    </rPh>
+    <rPh sb="102" eb="103">
+      <t>ムス</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>ソツギョウ</t>
+    </rPh>
+    <rPh sb="117" eb="119">
+      <t>ガクセキ</t>
+    </rPh>
+    <rPh sb="120" eb="121">
+      <t>ウシナ</t>
+    </rPh>
+    <rPh sb="124" eb="126">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="145" eb="147">
+      <t>ジブン</t>
+    </rPh>
+    <rPh sb="148" eb="150">
+      <t>ベット</t>
+    </rPh>
+    <rPh sb="167" eb="169">
+      <t>コウニュウ</t>
+    </rPh>
+    <rPh sb="179" eb="180">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="184" eb="185">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="186" eb="187">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="195" eb="196">
+      <t>カマ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メディアセンタのMicrosoft 365ポータルサイト&lt;a href="https://www.media.hiroshima-u.ac.jp/services/webmail-portal/" target="_blank" rel="noreferrer"&gt;https://www.media.hiroshima-u.ac.jp/services/webmail-portal/&lt;/a&gt;にジャンプします。水色の「Microsoft365ポータル」を押すと&lt;a href="https://portal.office.com/" target="_blank" rel="noreferrer"&gt;https://portal.office.com/&lt;/a&gt;に移動します。
+※ もみじトップページの右側にある「Webメール」バナーをクリックしても同じページに移動できます。</t>
+    <rPh sb="205" eb="207">
+      <t>ミズイロ</t>
+    </rPh>
+    <rPh sb="227" eb="228">
+      <t>オ</t>
+    </rPh>
+    <rPh sb="331" eb="333">
+      <t>イドウ</t>
+    </rPh>
+    <rPh sb="350" eb="352">
+      <t>ミギガワ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMCアカウントを「@hiroshima-u.ac.jp」つきで入力し、さらにパスワードも入力します。このサイトはMicrosoftのサイトなので、「@hiroshima-u.ac.jp」がついていないと貴方の学生番号がどの大学のものか判らないため、「@hiroshima-u.ac.jp」を加える必要があります。
+※学外からログインする場合は、ここで多要素認証の手続きが入ります。</t>
+    <rPh sb="32" eb="34">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>アナタ</t>
+    </rPh>
+    <rPh sb="105" eb="107">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="107" eb="109">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="118" eb="119">
+      <t>ワカ</t>
+    </rPh>
+    <rPh sb="146" eb="147">
+      <t>クワ</t>
+    </rPh>
+    <rPh sb="149" eb="151">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="159" eb="161">
+      <t>ガクガイ</t>
+    </rPh>
+    <rPh sb="169" eb="171">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="176" eb="181">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="182" eb="184">
+      <t>テツヅ</t>
+    </rPh>
+    <rPh sb="186" eb="187">
+      <t>ハイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>o365-outlook.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Office365のページの左側にブラウザ内で使用できるアプリのアイコンが並びます。「O」の文字があるOutlookをクリックします。</t>
+    <rPh sb="14" eb="16">
+      <t>ヒダリガワ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="37" eb="38">
+      <t>ナラ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>モジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">次に、Office365のオンラインストレージのOneDriveを見て見ましょう。画面左上のつぶつぶをクリックします。
+するとOffice365で使用できるアプリケーション一覧が表示されます。その中にある「OneDrive」をクリックしましょう。
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広大IDとパスワードを入力し、「ログイン」をクリックします。
+※ 学外からのログインする場合は、ここで多要素認証の手続きが入ります。</t>
+    <rPh sb="0" eb="2">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>ガクガイ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="51" eb="56">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="57" eb="59">
+      <t>テツヅ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>ハイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check-13&lt;/span&gt;
+これを「Myもみじのトップページ」と呼ぶことにしましょう。
+履修登録をしたり、成績を確認することができます。
+また「掲示」では、授業や学部からの連絡が表示されます。
+  </t>
+    <rPh sb="70" eb="71">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">この実習では、このままで次の「Bb9」の使い方に進みます。
+※ Myもみじの閲覧が済んだら、できるだけ画面右上の「ログアウト」をクリックするようにしましょう。
+  </t>
+    <rPh sb="2" eb="4">
+      <t>ジッシュウ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;strong&gt;※ ここまでの実習の中で、広島大学には２つのオンライン学習支援システム「広大moodle」「Bb9」があることに気づかれたと思います。
+広島大学では今年度「広大moodle」「Bb9」の２つのオンライン学習支援システムを併用します。来年度からは「広大moodle」に一本化する予定です。
+しばらく面倒をおかけしますが、ご了解ください。&lt;/strong&gt;</t>
+    <rPh sb="15" eb="17">
+      <t>ジッシュウ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="21" eb="25">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="35" eb="39">
+      <t>ガクシュウシエン</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="70" eb="71">
+      <t>オモ</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="109" eb="113">
+      <t>ガクシュウシエン</t>
+    </rPh>
+    <rPh sb="118" eb="120">
+      <t>ヘイヨウ</t>
+    </rPh>
+    <rPh sb="124" eb="127">
+      <t>ライネンド</t>
+    </rPh>
+    <rPh sb="131" eb="133">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="141" eb="144">
+      <t>イッポンカ</t>
+    </rPh>
+    <rPh sb="146" eb="148">
+      <t>ヨテイ</t>
+    </rPh>
+    <rPh sb="156" eb="158">
+      <t>メンドウ</t>
+    </rPh>
+    <rPh sb="168" eb="170">
+      <t>リョウカイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">この章では、Wi-Fiで広島大学の学内ネットワークに接続するための設定を行います。この章の設定は、広島大学キャンパスに来たときに行ってください。学生番号と、学生番号と一緒にもらえる「広大パスワード」が必要です。
+</t>
+    <rPh sb="2" eb="3">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ガクナイ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="49" eb="53">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>オコナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">設定にはいる前に、広島大学で情報サービスを使うときに必要なIDが二種類あることを確認しましょう。二種類とも学生番号をもとにしています。
+一つは「広大ID」。これは学生番号と同じ文字列です。もう一つはメディアセンターの「アカウント名(IMCアカウント名)」です。こちらは、先頭の一文字を小文字にしたものになっています。
+対応するパスワードは、どちらも共通です。「広大パスワード」と呼んでいます。学生証と一緒に配布されます。
+IMCアカウント名に「@hiroshima-u.ac.jp」をつけたものを広大メールアドレスと呼んでいます。このメールアドレスは、広大学生として公式のものになります。事務連絡、教員からの連絡等ありますので、日常的にチェックするようにしましょう。チェックする方法は、第６章で紹介します。
+  </t>
+    <rPh sb="343" eb="344">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="345" eb="346">
+      <t>ショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>このテキストの第１章からここまで順に進んでいれば、点検届チェックリストがすべてチェックできているはずです。
+&lt;strong&gt;広大moodleの「ノートパソコン点検届」コースを開いて、点検届を提出しましょう！&lt;/strong&gt;</t>
+    <rPh sb="7" eb="8">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ジュン</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="81" eb="82">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="87" eb="88">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="91" eb="93">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="95" eb="97">
+      <t>テイシュツツカバアイスス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次のリンクから広島大学オンライン学習支援システム（広大moodle）にアクセスしてください。
+&lt;a href="https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/"&gt;https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/&lt;/a&gt;
+「広大IDでログイン」をクリックしてログインしましょう。</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="7" eb="11">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="16" eb="20">
+      <t>ガクシュウシエン</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="166" eb="168">
+      <t>ヒロダイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;strong&gt;「コースツリー」の中にある「ノートパソコン点検届」から、点検届を提出してください。&lt;/strong&gt;</t>
+    <rPh sb="17" eb="18">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="29" eb="32">
+      <t>テンケントドケ</t>
+    </rPh>
+    <rPh sb="36" eb="39">
+      <t>テンケントドケ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>テイシュツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMCアカウントを「@hiroshima-u.ac.jp」つきで入力し、さらにパスワードも入力します。このサイトはMicrosoftのサイトなので、「@hiroshima-u.ac.jp」がついていないと貴方の学生番号がどの大学のものか判らないため、「@hiroshima-u.ac.jp」を加える必要があります。
+※ 学外からのアクセスの場合は、ここで多要素認証（MFA）の認証手続きが入ります</t>
+    <rPh sb="32" eb="34">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>アナタ</t>
+    </rPh>
+    <rPh sb="105" eb="107">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="107" eb="109">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="118" eb="119">
+      <t>ワカ</t>
+    </rPh>
+    <rPh sb="146" eb="147">
+      <t>クワ</t>
+    </rPh>
+    <rPh sb="149" eb="151">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="170" eb="172">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Office365にサインインした状態になります。
+ここでは左右を縮めて表示していますが、画面の右上のほうに「Officeのインストール」というメニューがありますので、そこからOffice 365アプリを選びます。</t>
+    <rPh sb="17" eb="19">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>サユウ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>チヂ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="102" eb="103">
+      <t>エラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5061,6 +5208,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5092,7 +5245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5106,6 +5259,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5464,7 +5620,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>248</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5480,7 +5636,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -5488,7 +5644,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -5502,7 +5658,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5536,10 +5692,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5547,7 +5703,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5563,17 +5719,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5581,30 +5737,30 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>242</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>243</v>
+        <v>314</v>
       </c>
       <c r="D9" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>244</v>
+      <c r="B10" s="4" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>245</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>246</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5627,10 +5783,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392D1BFF-FF5C-4A7E-8C9C-E750AF0FFFAF}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5646,7 +5802,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5654,7 +5810,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5670,22 +5826,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5693,7 +5849,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>253</v>
+        <v>231</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -5709,273 +5865,279 @@
     </row>
     <row r="14" spans="1:4" ht="102" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>254</v>
+        <v>232</v>
       </c>
       <c r="D14" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
       <c r="D16" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>220</v>
+        <v>316</v>
       </c>
       <c r="D17" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="D18" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>222</v>
+        <v>317</v>
       </c>
       <c r="D19" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="D20" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>183</v>
+        <v>114</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="51" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>176</v>
+        <v>115</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="51" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="102" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="C41" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42" t="s">
         <v>8</v>
       </c>
-      <c r="D41" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" ht="102" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C42" t="s">
-        <v>172</v>
-      </c>
       <c r="D42" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
       </c>
       <c r="D44" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>167</v>
       </c>
@@ -5983,18 +6145,7 @@
         <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C48" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -6009,7 +6160,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="19.149999999999999" x14ac:dyDescent="0.25"/>
@@ -6026,7 +6177,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s" ph="1">
-        <v>299</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6034,7 +6185,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s" ph="1">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6050,7 +6201,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>249</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
@@ -6058,7 +6209,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>264</v>
+        <v>241</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6078,7 +6229,7 @@
         <v>8</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="57.4" ph="1" x14ac:dyDescent="0.25">
@@ -6086,13 +6237,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -6100,21 +6251,21 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s" ph="1">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s" ph="1">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -6122,13 +6273,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s" ph="1">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="133.9" ph="1" x14ac:dyDescent="0.25">
@@ -6136,29 +6287,29 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s" ph="1">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s" ph="1">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s" ph="1">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="114.75" ph="1" x14ac:dyDescent="0.25">
@@ -6166,13 +6317,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s" ph="1">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="95.65" ph="1" x14ac:dyDescent="0.25">
@@ -6180,13 +6331,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s" ph="1">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
@@ -6194,21 +6345,21 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s" ph="1">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s" ph="1">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="114.75" ph="1" x14ac:dyDescent="0.25">
@@ -6216,13 +6367,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s" ph="1">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6230,21 +6381,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s" ph="1">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="57.4" ph="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s" ph="1">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="95.65" ph="1" x14ac:dyDescent="0.25">
@@ -6252,13 +6403,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s" ph="1">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="133.9" ph="1" x14ac:dyDescent="0.25">
@@ -6266,24 +6417,24 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s" ph="1">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s" ph="1">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -6291,13 +6442,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s" ph="1">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>8</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -6311,8 +6462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6328,7 +6479,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>300</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6336,7 +6487,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6352,15 +6503,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>179</v>
+        <v>293</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6374,7 +6525,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -6383,12 +6534,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="178.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>291</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -6402,7 +6553,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -6416,7 +6567,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -6430,7 +6581,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -6444,7 +6595,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -6458,7 +6609,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6472,7 +6623,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>62</v>
+        <v>292</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6486,7 +6637,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>94</v>
+        <v>294</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -6506,8 +6657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A19" zoomScale="112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6523,7 +6674,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6531,7 +6682,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6547,7 +6698,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6555,7 +6706,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>265</v>
+        <v>242</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6571,7 +6722,7 @@
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6618,7 +6769,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6626,32 +6777,32 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6659,27 +6810,27 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>69</v>
+        <v>297</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>110</v>
+      <c r="B17" s="4" t="s">
+        <v>296</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
@@ -6687,13 +6838,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -6701,13 +6852,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6715,13 +6866,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6729,13 +6880,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -6749,7 +6900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43F54BA-B356-43A4-B76F-707ED0C70724}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="118" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -6766,7 +6917,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6774,7 +6925,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6790,7 +6941,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -6798,7 +6949,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>296</v>
+        <v>271</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6814,116 +6965,116 @@
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>302</v>
+        <v>277</v>
       </c>
       <c r="D9" t="s">
-        <v>301</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>288</v>
+        <v>263</v>
       </c>
       <c r="D10" t="s">
-        <v>289</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>290</v>
+        <v>265</v>
       </c>
       <c r="D11" t="s">
-        <v>291</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>292</v>
+        <v>267</v>
       </c>
       <c r="D12" t="s">
-        <v>293</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>295</v>
+        <v>270</v>
       </c>
       <c r="D13" t="s">
-        <v>294</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>315</v>
+        <v>289</v>
       </c>
       <c r="D16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="D17" t="s">
-        <v>305</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>306</v>
+        <v>280</v>
       </c>
       <c r="D18" t="s">
-        <v>307</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>308</v>
+        <v>282</v>
       </c>
       <c r="D19" t="s">
-        <v>309</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>310</v>
+        <v>284</v>
       </c>
       <c r="D20" t="s">
-        <v>311</v>
+        <v>285</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>312</v>
+        <v>286</v>
       </c>
       <c r="D21" t="s">
-        <v>313</v>
+        <v>287</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>314</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -6938,7 +7089,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6954,7 +7105,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6962,7 +7113,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6978,7 +7129,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -6989,7 +7140,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7005,15 +7156,15 @@
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>250</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>316</v>
+        <v>290</v>
       </c>
       <c r="D9" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7021,32 +7172,32 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>201</v>
+      <c r="B11" s="4" t="s">
+        <v>300</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7054,7 +7205,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>268</v>
+        <v>299</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7065,7 +7216,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7076,7 +7227,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7092,8 +7243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DD8924-3FAE-44AB-A508-09E9136389D4}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7109,7 +7260,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7117,7 +7268,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7133,7 +7284,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7141,7 +7292,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7152,12 +7303,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>121</v>
+        <v>301</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7165,7 +7316,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -7176,7 +7327,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7184,21 +7335,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="D12" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7206,18 +7357,18 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>287</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7225,13 +7376,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7239,13 +7390,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -7275,8 +7426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7292,7 +7443,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7300,7 +7451,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7316,7 +7467,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -7324,7 +7475,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7335,7 +7486,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7343,13 +7494,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>42</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7357,18 +7508,18 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7385,71 +7536,71 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>284</v>
+        <v>302</v>
       </c>
       <c r="D12" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>220</v>
+        <v>303</v>
       </c>
       <c r="D13" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>298</v>
+        <v>273</v>
       </c>
       <c r="D14" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>224</v>
+      <c r="B15" s="6" t="s">
+        <v>305</v>
       </c>
       <c r="D15" t="s">
-        <v>225</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
       <c r="D16" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>227</v>
+        <v>306</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -7471,62 +7622,62 @@
         <v>4</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>232</v>
+        <v>307</v>
       </c>
       <c r="D23" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="D24" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>237</v>
+        <v>308</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -7545,7 +7696,7 @@
     </row>
     <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -7553,7 +7704,7 @@
     </row>
     <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>261</v>
+        <v>238</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -7564,13 +7715,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7578,7 +7729,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>262</v>
+        <v>239</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -7589,13 +7740,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7603,13 +7754,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7617,12 +7768,12 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>271</v>
+        <v>310</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7630,7 +7781,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -7644,13 +7795,13 @@
         <v>4</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -7658,21 +7809,21 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7680,13 +7831,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="4:4" ht="19.149999999999999" x14ac:dyDescent="0.25">
@@ -7701,10 +7852,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7728,7 +7879,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7744,150 +7895,145 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>95</v>
+        <v>312</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
       <c r="D16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add comment for coop computer ch.0 win10(ja)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{832CDF93-F4DF-4A2C-97C1-6C7A0FC49667}"/>
+  <xr:revisionPtr revIDLastSave="130" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E788221-88C9-4860-B3F8-15D0E4659EBB}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="2835" windowWidth="18225" windowHeight="11873" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4170" yWindow="-11625" windowWidth="18225" windowHeight="11880" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="319">
   <si>
     <t>header1</t>
   </si>
@@ -51,10 +51,6 @@
   </si>
   <si>
     <t>fresta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Windowsで使用する言語を選びます。「日本語」をクリックしてください。
-  </t>
   </si>
   <si>
     <t>chartn</t>
@@ -3441,34 +3437,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Surfaceの電源を初めて入れて、デスクトップ画面が表示されるまでの設定内容について説明します。一番重要なのは、普段利用するユーザ名とパスワードを作成するところ。あとはだいたい言われるままにしていけば大丈夫です。 すでにデスクトップが表示されている方はこの章をスキップして次の「パソコンのスペック確認」へ進んでください。 Windows10はバージョン番号が同じでもバリエーションがあったり、出荷時期によって違いがあります。以下の手順にある画面がそもそも表示されなかったり、表示される表現が少し異なることもありますが、あわてないでください。</t>
-    <rPh sb="177" eb="179">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="180" eb="181">
-      <t>オナ</t>
-    </rPh>
-    <rPh sb="205" eb="206">
-      <t>チガ</t>
-    </rPh>
-    <rPh sb="228" eb="230">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="238" eb="240">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="243" eb="245">
-      <t>ヒョウゲン</t>
-    </rPh>
-    <rPh sb="246" eb="247">
-      <t>スコ</t>
-    </rPh>
-    <rPh sb="248" eb="249">
-      <t>コト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Windows Update を使って、WindowsとOfficeがつねに最新版で使えるように設定します。
 さらに、Defenderでのフルスキャン（全てのファイルに対するウィルスチェック）のやり方を確認しておきます。
 &lt;ul&gt;&lt;li&gt;&lt;a href="#windows_update"&gt;Windows Updateの設定&lt;/a&gt;
@@ -4036,41 +4004,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;strong&gt;※ 生協推奨PCを購入した方は、引き渡されたPCと一緒に提供されたマニュアルおよび動画に従って初期設定を行ってから、このテキストの次の章（第１章）からはじめてください。&lt;/strong&gt; 
-&lt;p&gt;購入したばかりの Windows 10 の電源を入れて、使い始められるようになるまでに必要な設定作業を説明します。</t>
-    <rPh sb="10" eb="12">
-      <t>セイキョウ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>スイショウ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>コウニュウ</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>カタ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>テイキョウ</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>ドウガ</t>
-    </rPh>
-    <rPh sb="52" eb="53">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="55" eb="59">
-      <t>ショキセッテイ</t>
-    </rPh>
-    <rPh sb="60" eb="61">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="79" eb="80">
-      <t>ショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">自分のパソコンの基本的なスペックを確認しておきましょう。CPUの型式、OSのビット数、記憶容量など。 </t>
     <phoneticPr fontId="1"/>
   </si>
@@ -4295,25 +4228,6 @@
     </rPh>
     <rPh sb="199" eb="201">
       <t>ヒロダイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">「詳細情報」という名前のウィンドウが開きます。中にPCに関する情報がたくさん表示されています。
-「Wind+B13owsの仕様」をみると「エディション」のところに「Windows 10 Pro」とありますね。これがOSの種類です。「バージョン」のところには詳細なバージョン番号（いつの時点のOSか）が書かれています。&lt;span class="check"&gt;check-1&lt;span&gt;&lt;/span&gt;
-&lt;/span&gt;
-その上の方に「デバイスの仕様」がありますね。ここの「システムの種類」を見ると、OSのビット数がわかります。&amp;quot;64ビットオペレーティングシステム&amp;quot; とあります。この場合は64ビットですね。二進法で64桁のデータを一度に処理できるOSであるということを示しています。&lt;span class="check"&gt;check-2&lt;span&gt;&lt;/span&gt;
-&lt;/span&gt;
-その上に「実装RAM」と書かれたところがあります。ここを見ると、主記憶装置（メインメモリ）の容量がわかります。この場合は8GB（ギガバイト）ですね。この容量が大きいほど、大量のデータを一括して扱えたり、多くのプログラムを同時に動作させたりすることがスムーズにできるようになります。
-  </t>
-    <rPh sb="1" eb="3">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="299" eb="301">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="456" eb="458">
-      <t>バアイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5175,6 +5089,97 @@
     <t xml:space="preserve">広島大学では履修登録、成績確認、各種通知は「Myもみじ」を利用して行います。「Myもみじ」へログインしてみましょう。
 まず「Myもみじへログイン」をクリックしてください。
    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">「詳細情報」という名前のウィンドウが開きます。中にPCに関する情報がたくさん表示されています。
+「Windowsの仕様」をみると「エディション」のところに「Windows 10 Pro」とありますね。これがOSの種類です。「バージョン」のところには詳細なバージョン番号（いつの時点のOSか）が書かれています。&lt;span class="check"&gt;check-1&lt;span&gt;&lt;/span&gt;
+&lt;/span&gt;
+その上の方に「デバイスの仕様」がありますね。ここの「システムの種類」を見ると、OSのビット数がわかります。&amp;quot;64ビットオペレーティングシステム&amp;quot; とあります。この場合は64ビットですね。二進法で64桁のデータを一度に処理できるOSであるということを示しています。&lt;span class="check"&gt;check-2&lt;span&gt;&lt;/span&gt;
+&lt;/span&gt;
+その上に「実装RAM」と書かれたところがあります。ここを見ると、主記憶装置（メインメモリ）の容量がわかります。この場合は8GB（ギガバイト）ですね。この容量が大きいほど、大量のデータを一括して扱えたり、多くのプログラムを同時に動作させたりすることがスムーズにできるようになります。
+  </t>
+    <rPh sb="1" eb="3">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="295" eb="297">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="452" eb="454">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Windowsで使用する言語を選びます。「日本語」をクリックしてください。
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;strong&gt;※ 生協推奨PCを購入した方は、引き渡されたPCと一緒に生協から提供されたマニュアルおよび動画 に従って初期設定をを行い、このテキストは次の章（第１章）からはじめてください。&lt;/strong&gt;</t>
+    <rPh sb="36" eb="38">
+      <t>セイキョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;strong&gt;※ 生協推奨PCを購入した方は、引き渡されたPCと一緒に生協から提供されたマニュアルおよび動画に従って初期設定を行ってから、このテキストの次の章（第１章）からはじめてください。&lt;/strong&gt; 
+&lt;p&gt;購入したばかりの Windows 10 の電源を入れて、使い始められるようになるまでに必要な設定作業を説明します。</t>
+    <rPh sb="10" eb="12">
+      <t>セイキョウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>スイショウ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>コウニュウ</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>セイキョウ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>ドウガ</t>
+    </rPh>
+    <rPh sb="56" eb="57">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="59" eb="63">
+      <t>ショキセッテイ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="83" eb="84">
+      <t>ショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Surfaceの電源を初めて入れて、デスクトップ画面が表示されるまでの設定内容について説明します。一番重要なのは、普段利用するユーザ名とパスワードを作成するところ。あとはだいたい言われるままにしていけば大丈夫です。 すでにデスクトップが表示されている方はこの章をスキップして次の「パソコンのスペック確認」へ進んでください。 Windows10はバージョン番号が同じでもバリエーションがあったり、出荷時期によって違いがあります。以下の手順にある画面の表現がテキストと少し異なったり、そもそも表示されなかったりすることもありますが、あわてないでください。</t>
+    <rPh sb="177" eb="179">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="180" eb="181">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="205" eb="206">
+      <t>チガ</t>
+    </rPh>
+    <rPh sb="224" eb="226">
+      <t>ヒョウゲン</t>
+    </rPh>
+    <rPh sb="232" eb="233">
+      <t>スコ</t>
+    </rPh>
+    <rPh sb="234" eb="235">
+      <t>コト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -5619,7 +5624,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5635,7 +5640,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -5643,7 +5648,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -5657,7 +5662,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5691,10 +5696,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5702,7 +5707,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5718,17 +5723,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5736,30 +5741,30 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5801,7 +5806,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5809,7 +5814,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5825,22 +5830,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5848,7 +5853,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -5859,72 +5864,72 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="102" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D16" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D18" t="s">
         <v>205</v>
-      </c>
-      <c r="D18" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -5935,216 +5940,216 @@
     </row>
     <row r="27" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
         <v>137</v>
-      </c>
-      <c r="C29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
         <v>143</v>
-      </c>
-      <c r="C38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="102" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -6156,10 +6161,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="19.149999999999999" x14ac:dyDescent="0.25"/>
@@ -6176,7 +6181,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s" ph="1">
-        <v>270</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6184,7 +6189,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s" ph="1">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6200,7 +6205,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
@@ -6208,7 +6213,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>237</v>
+        <v>318</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6217,237 +6222,242 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s" ph="1">
-        <v>4</v>
-      </c>
+    <row r="7" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s" ph="1">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s" ph="1">
+        <v>315</v>
+      </c>
+      <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
-      <c r="C7" t="s" ph="1">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s" ph="1">
+      <c r="D8" t="s" ph="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="57.4" ph="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s" ph="1">
+        <v>129</v>
+      </c>
+      <c r="C9" t="s" ph="1">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s" ph="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="s" ph="1">
+        <v>127</v>
+      </c>
+      <c r="C10" t="s" ph="1">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s" ph="1">
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="57.4" ph="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s" ph="1">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s" ph="1">
-        <v>130</v>
-      </c>
-      <c r="C8" t="s" ph="1">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s" ph="1">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s" ph="1">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s" ph="1">
-        <v>128</v>
-      </c>
-      <c r="C9" t="s" ph="1">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s" ph="1">
+    <row r="11" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s" ph="1">
+        <v>68</v>
+      </c>
+      <c r="D11" t="s" ph="1">
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s" ph="1">
-        <v>69</v>
-      </c>
-      <c r="D10" t="s" ph="1">
+    <row r="12" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s" ph="1">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s" ph="1">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s" ph="1">
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s" ph="1">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s" ph="1">
-        <v>61</v>
-      </c>
-      <c r="C11" t="s" ph="1">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s" ph="1">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="133.9" ph="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s" ph="1">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s" ph="1">
-        <v>105</v>
-      </c>
-      <c r="C12" t="s" ph="1">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s" ph="1">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="133.9" ph="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s" ph="1">
+        <v>4</v>
+      </c>
       <c r="B13" s="1" t="s" ph="1">
         <v>104</v>
       </c>
+      <c r="C13" t="s" ph="1">
+        <v>7</v>
+      </c>
       <c r="D13" t="s" ph="1">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s" ph="1">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="D14" t="s" ph="1">
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="114.75" ph="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s" ph="1">
-        <v>4</v>
-      </c>
+    <row r="15" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s" ph="1">
+        <v>128</v>
+      </c>
+      <c r="D15" t="s" ph="1">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="114.75" ph="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s" ph="1">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s" ph="1">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s" ph="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="95.65" ph="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s" ph="1">
+        <v>105</v>
+      </c>
+      <c r="C17" t="s" ph="1">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s" ph="1">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s" ph="1">
+        <v>106</v>
+      </c>
+      <c r="C18" t="s" ph="1">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s" ph="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s" ph="1">
         <v>62</v>
       </c>
-      <c r="C15" t="s" ph="1">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s" ph="1">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="95.65" ph="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s" ph="1">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s" ph="1">
-        <v>106</v>
-      </c>
-      <c r="C16" t="s" ph="1">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s" ph="1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s" ph="1">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s" ph="1">
-        <v>107</v>
-      </c>
-      <c r="C17" t="s" ph="1">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s" ph="1">
+      <c r="D19" t="s" ph="1">
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s" ph="1">
-        <v>63</v>
-      </c>
-      <c r="D18" t="s" ph="1">
+    <row r="20" spans="1:4" ht="114.75" ph="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s" ph="1">
+        <v>80</v>
+      </c>
+      <c r="C20" t="s" ph="1">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s" ph="1">
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="114.75" ph="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s" ph="1">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s" ph="1">
+    <row r="21" spans="1:4" ph="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s" ph="1">
+        <v>171</v>
+      </c>
+      <c r="C21" t="s" ph="1">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s" ph="1">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="57.4" ph="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s" ph="1">
+        <v>172</v>
+      </c>
+      <c r="D22" t="s" ph="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="95.65" ph="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s" ph="1">
+        <v>173</v>
+      </c>
+      <c r="C23" t="s" ph="1">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s" ph="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="133.9" ph="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="s" ph="1">
         <v>81</v>
       </c>
-      <c r="C19" t="s" ph="1">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s" ph="1">
+      <c r="C24" t="s" ph="1">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s" ph="1">
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s" ph="1">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s" ph="1">
-        <v>172</v>
-      </c>
-      <c r="C20" t="s" ph="1">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s" ph="1">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="57.4" ph="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s" ph="1">
-        <v>173</v>
-      </c>
-      <c r="D21" t="s" ph="1">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="95.65" ph="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s" ph="1">
-        <v>4</v>
-      </c>
-      <c r="B22" s="1" t="s" ph="1">
-        <v>174</v>
-      </c>
-      <c r="C22" t="s" ph="1">
-        <v>8</v>
-      </c>
-      <c r="D22" t="s" ph="1">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="133.9" ph="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s" ph="1">
-        <v>4</v>
-      </c>
-      <c r="B23" s="1" t="s" ph="1">
+    <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s" ph="1">
+        <v>125</v>
+      </c>
+      <c r="C25" t="s" ph="1">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s" ph="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1" t="s" ph="1">
         <v>82</v>
       </c>
-      <c r="C23" t="s" ph="1">
-        <v>8</v>
-      </c>
-      <c r="D23" t="s" ph="1">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ph="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s" ph="1">
-        <v>126</v>
-      </c>
-      <c r="C24" t="s" ph="1">
-        <v>8</v>
-      </c>
-      <c r="D24" t="s" ph="1">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s" ph="1">
-        <v>4</v>
-      </c>
-      <c r="B25" s="1" t="s" ph="1">
-        <v>83</v>
-      </c>
-      <c r="C25" t="s" ph="1">
-        <v>8</v>
-      </c>
-      <c r="D25" t="s" ph="1">
-        <v>70</v>
+      <c r="C26" t="s" ph="1">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s" ph="1">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -6461,8 +6471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6478,7 +6488,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6486,7 +6496,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6502,7 +6512,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
@@ -6510,7 +6520,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6524,27 +6534,27 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="178.5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -6552,13 +6562,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
@@ -6566,21 +6576,21 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -6594,13 +6604,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6608,13 +6618,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6622,13 +6632,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6636,13 +6646,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -6673,7 +6683,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6681,7 +6691,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6697,7 +6707,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6705,7 +6715,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6716,17 +6726,17 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6734,13 +6744,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6748,13 +6758,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6762,13 +6772,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6776,13 +6786,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6790,18 +6800,18 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -6809,13 +6819,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -6823,13 +6833,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
@@ -6837,13 +6847,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -6851,13 +6861,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6865,13 +6875,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6879,13 +6889,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -6916,7 +6926,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6924,7 +6934,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6940,7 +6950,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -6948,7 +6958,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6959,70 +6969,70 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D9" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D13" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -7030,50 +7040,50 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D17" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D18" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D19" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D20" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D21" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -7104,7 +7114,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7112,7 +7122,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7128,7 +7138,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -7139,7 +7149,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7150,20 +7160,20 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7171,13 +7181,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>184</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
@@ -7185,18 +7195,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7204,7 +7214,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7215,7 +7225,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7226,7 +7236,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7259,7 +7269,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7267,7 +7277,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7283,7 +7293,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7291,7 +7301,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7302,12 +7312,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7315,18 +7325,18 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7334,21 +7344,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D12" t="s">
         <v>193</v>
-      </c>
-      <c r="D12" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7356,18 +7366,18 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>195</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7375,13 +7385,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>197</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7389,13 +7399,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -7425,7 +7435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
@@ -7442,7 +7452,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7450,7 +7460,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7466,7 +7476,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -7474,7 +7484,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7485,7 +7495,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7493,13 +7503,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7507,18 +7517,18 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -7537,69 +7547,69 @@
     </row>
     <row r="12" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D15" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -7621,29 +7631,29 @@
         <v>4</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7651,13 +7661,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -7665,18 +7675,18 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -7695,7 +7705,7 @@
     </row>
     <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -7703,7 +7713,7 @@
     </row>
     <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -7714,13 +7724,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7728,7 +7738,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -7739,13 +7749,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7753,13 +7763,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7767,12 +7777,12 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7780,7 +7790,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -7794,13 +7804,13 @@
         <v>4</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -7808,21 +7818,21 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7830,13 +7840,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
         <v>52</v>
-      </c>
-      <c r="C41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="49" spans="4:4" ht="19.149999999999999" x14ac:dyDescent="0.25">
@@ -7870,7 +7880,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7878,7 +7888,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7894,12 +7904,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7907,13 +7917,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
@@ -7921,13 +7931,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7935,13 +7945,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7949,13 +7959,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7963,13 +7973,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7977,13 +7987,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7991,29 +8001,29 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -8027,13 +8037,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix some word win10(ja)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E788221-88C9-4860-B3F8-15D0E4659EBB}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85BE829F-4769-44E0-99DA-1629A629D974}"/>
   <bookViews>
-    <workbookView xWindow="4170" yWindow="-11625" windowWidth="18225" windowHeight="11880" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="-14595" windowWidth="18225" windowHeight="11880" tabRatio="782" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -367,45 +367,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Microsoft Teams について。最近のWindows10パソコンでは、サインイン時にMicrosoft Teams が自動的に起動します。これはMicrosoftが提供しているグループチャットアプリで、広大メールアドレスとパスワードでサインインして使うことができます。
-詳細はメディアセンターWebサイトの&lt;a href="https://www.media.hiroshima-u.ac.jp/services/communication/teams/"&gt;「Microsft Teams」&lt;/a&gt;で。
-また、使わない場合は画面左下のウィンドウアイコンから「設定」→「アプリ」→「スタートアップ」と進んでTeamsのスイッチを「オフ」にすると、自動起動を止めることができます。</t>
-    <rPh sb="21" eb="23">
-      <t>サイキン</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>トキ</t>
-    </rPh>
-    <rPh sb="64" eb="67">
-      <t>ジドウテキ</t>
-    </rPh>
-    <rPh sb="68" eb="70">
-      <t>キドウ</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>テイキョウ</t>
-    </rPh>
-    <rPh sb="106" eb="108">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="129" eb="130">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="140" eb="142">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="260" eb="261">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="264" eb="266">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="304" eb="305">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">「このアカウントのセキュリティの質問」を作成するように促されます。これは、パスワードを忘れてしまった時に、代わりになる質問を入れておく機能です。
 しかしこのPCに触れる人なら誰でもこの質問を使ってログインできてしまうので、あなたのPCが乗っ取られる危険性を大きくするものです。あまり良い機能ではありません。
 何か記入をしないと次に進めないので、あえて質問とは関係のない答を入れるのがおススメです。
@@ -563,22 +524,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;h2&gt;広島大学学生向けOffice365ProPlusのインストール&lt;/h2&gt;</t>
-    <rPh sb="4" eb="6">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>ム</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win10-4-23.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1140,68 +1085,6 @@
     </rPh>
     <rPh sb="64" eb="66">
       <t>フヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>包括ライセンスでMicrosoft Office365 Pro Plusをインストールした場合は、Microsoft Teamsは既にインストールされている筈です。検索ウィンドウで「Teams」を検索すれば出てくる筈です。
-もし別途Officeを購入したため、Microsoft Teamsがまだ入っていないという場合は、https://www.microsoft.com/ja-jp/microsoft-teams/download-app からダウンロードしてインストールしてください(Office365と違ってアカウントにサインインしなくてもダウンロードできます)。また、iOS機器(iPhone, iPad)やAndroid機器でも動きますが、ここではPCでの確認手順を説明します。</t>
-    <rPh sb="0" eb="2">
-      <t>ホウカツ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="65" eb="66">
-      <t>スデ</t>
-    </rPh>
-    <rPh sb="78" eb="79">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="82" eb="84">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="98" eb="100">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="103" eb="104">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="107" eb="108">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="114" eb="116">
-      <t>ベット</t>
-    </rPh>
-    <rPh sb="123" eb="125">
-      <t>コウニュウ</t>
-    </rPh>
-    <rPh sb="148" eb="149">
-      <t>ハイ</t>
-    </rPh>
-    <rPh sb="157" eb="159">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="255" eb="256">
-      <t>チガ</t>
-    </rPh>
-    <rPh sb="292" eb="294">
-      <t>キキ</t>
-    </rPh>
-    <rPh sb="316" eb="318">
-      <t>キキ</t>
-    </rPh>
-    <rPh sb="320" eb="321">
-      <t>ウゴ</t>
-    </rPh>
-    <rPh sb="334" eb="336">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="336" eb="338">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="339" eb="341">
-      <t>セツメイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -3101,179 +2984,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ここでは、&lt;strong&gt;まだOfficeがインストールされていないPCに&lt;/strong&gt;広島大学の提供するOffice365ProPlusをダウンロードしてインストールする方法を説明します。</t>
-    <rPh sb="46" eb="48">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="51" eb="53">
-      <t>テイキョウ</t>
-    </rPh>
-    <rPh sb="88" eb="90">
-      <t>ホウホウ</t>
-    </rPh>
-    <rPh sb="91" eb="93">
-      <t>セツメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>広島大学では、マイクロソフト社との包括ライセンス契約（Microsoft Enrollment for Education Solutions）を結んでいます。これによって広島大学の学生は広島大学が定める利用要領に基づいて、いくつかのマイクロソフト社製ソフトウェア製品（Microsoft Office等）を無償で利用することができます。
-Microsoft Office については、広島大学の学生は個人所有のPCで５台まで無償で利用することができます。
-ただしこのOffice 365アプリはマイクロソフトのサーバに登録されている広島大学のアカウントに関係づけられており、卒業（もしくは退学）後は利用できなくなってしまいますので、ご注意ください。
-※ 「Office 365 Proplus」は現在「Microsoft 365 Apps for Enterprise」に改称されていますが、Office 365 アプリとしての位置づけには変更ありません。以下このテキストでは「Office365ProPlus」のままで説明します。</t>
-    <rPh sb="0" eb="2">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>シャ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ホウカツ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ケイヤク</t>
-    </rPh>
-    <rPh sb="73" eb="74">
-      <t>ムス</t>
-    </rPh>
-    <rPh sb="86" eb="88">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="88" eb="90">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="91" eb="93">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="94" eb="96">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="96" eb="98">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="99" eb="100">
-      <t>サダ</t>
-    </rPh>
-    <rPh sb="102" eb="104">
-      <t>リヨウ</t>
-    </rPh>
-    <rPh sb="104" eb="106">
-      <t>ヨウリョウ</t>
-    </rPh>
-    <rPh sb="107" eb="108">
-      <t>モト</t>
-    </rPh>
-    <rPh sb="124" eb="125">
-      <t>シャ</t>
-    </rPh>
-    <rPh sb="125" eb="126">
-      <t>セイ</t>
-    </rPh>
-    <rPh sb="132" eb="134">
-      <t>セイヒン</t>
-    </rPh>
-    <rPh sb="151" eb="152">
-      <t>トウ</t>
-    </rPh>
-    <rPh sb="154" eb="156">
-      <t>ムショウ</t>
-    </rPh>
-    <rPh sb="157" eb="159">
-      <t>リヨウ</t>
-    </rPh>
-    <rPh sb="429" eb="431">
-      <t>イカ</t>
-    </rPh>
-    <rPh sb="461" eb="463">
-      <t>セツメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>ch5-download-from-portal-office365.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>あとは画面の指示に従ってインストーラーを保存し、そのインストーラーを起動するとOffice365ProPlusがインストールされます。利用規約に同意し、ライセンス認証のために広大メールアドレスを再度入力してしばらく待つとインストール完了です。
-&lt;p class="spl"&gt;※この方法でインストールしたOfficeは広大メールアドレスによってライセンス認証されているので、すぐに使うことができます。ただしこの章の最初に書いたように、&lt;strong&gt;広島大学を卒業した後は利用できなくなります&lt;/strong&gt;ので注意してください。&lt;/p&gt;</t>
-    <rPh sb="3" eb="5">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>シジ</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>キドウ</t>
-    </rPh>
-    <rPh sb="81" eb="83">
-      <t>ニンショウ</t>
-    </rPh>
-    <rPh sb="87" eb="89">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="97" eb="99">
-      <t>サイド</t>
-    </rPh>
-    <rPh sb="99" eb="101">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="107" eb="108">
-      <t>マ</t>
-    </rPh>
-    <rPh sb="116" eb="118">
-      <t>カンリョウ</t>
-    </rPh>
-    <rPh sb="140" eb="142">
-      <t>ホウホウ</t>
-    </rPh>
-    <rPh sb="158" eb="160">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="176" eb="178">
-      <t>ニンショウ</t>
-    </rPh>
-    <rPh sb="189" eb="190">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="204" eb="205">
-      <t>ショウ</t>
-    </rPh>
-    <rPh sb="206" eb="208">
-      <t>サイショ</t>
-    </rPh>
-    <rPh sb="209" eb="210">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="224" eb="226">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="226" eb="228">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="229" eb="231">
-      <t>ソツギョウ</t>
-    </rPh>
-    <rPh sb="233" eb="234">
-      <t>アト</t>
-    </rPh>
-    <rPh sb="235" eb="237">
-      <t>リヨウ</t>
-    </rPh>
-    <rPh sb="256" eb="258">
-      <t>チュウイ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -3572,36 +3283,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Office365のインストール手順、Microsoft Teamsの使い方</t>
-    <rPh sb="16" eb="18">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>カタ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;ul&gt;
-&lt;li&gt;&lt;a href="#office365"&gt;Office365のインストール&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;&lt;a href="#teams"&gt;Teamsの使い方&lt;/a&gt;&lt;/li&gt;
-&lt;/ul&gt;</t>
-    <rPh sb="83" eb="84">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="85" eb="86">
-      <t>カタ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h2&gt;&lt;a name="office365"&gt;Office365のインストール&lt;/a&gt;&lt;/h2&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;h2&gt;&lt;a name="teams"&gt;Teamsの使い方&lt;/a&gt;&lt;/h2&gt;</t>
     <rPh sb="26" eb="27">
       <t>ツカ</t>
@@ -4050,16 +3731,6 @@
     </rPh>
     <rPh sb="284" eb="285">
       <t>ト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">この章から、テキストにあるリンク（URL）をクリックしてWebブラウザを使うと作業しやすい場面が多くなります。
-できれば作業しているPCでこのテキストを見ながら作業しましょう。ネットワークに接続していればできるはずです。
-&lt;a href="https://riise.hiroshima-u.ac.jp/fresta/2022/"&gt;https://riise.hiroshima-u.ac.jp/fresta/2022/&lt;/a&gt;
-</t>
-    <rPh sb="2" eb="3">
-      <t>ショウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4347,53 +4018,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Googleのダウンロードページにジャンプしました。Google Chromeのブラウザ内部のデータをGoogleに送信しても良いかという許可チェックボックスがありますが、このチェックを外してダウンロードを行います。
-※ Edgeを使って作業している場合、右上に「EdgeのほうがChromeより良い」という旨の広告メッセージが出ますが、いまは無視してください。</t>
-    <rPh sb="44" eb="46">
-      <t>ナイブ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>ソウシン</t>
-    </rPh>
-    <rPh sb="63" eb="64">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="69" eb="71">
-      <t>キョカ</t>
-    </rPh>
-    <rPh sb="93" eb="94">
-      <t>ハズ</t>
-    </rPh>
-    <rPh sb="103" eb="104">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="116" eb="117">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="119" eb="121">
-      <t>サギョウ</t>
-    </rPh>
-    <rPh sb="125" eb="127">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="128" eb="130">
-      <t>ミギウエ</t>
-    </rPh>
-    <rPh sb="148" eb="149">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="154" eb="155">
-      <t>ムネ</t>
-    </rPh>
-    <rPh sb="164" eb="165">
-      <t>デ</t>
-    </rPh>
-    <rPh sb="172" eb="174">
-      <t>ムシ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>広大moodleの「コースツリー」の中の「MFA設定ガイド」をクリックすると、コースのトップページが表示されます。少し下の方にスクロールして表示される「広大IDとIMCアカウントの概要」を、まず読んでください。</t>
     <rPh sb="0" eb="2">
       <t>ヒロダイ</t>
@@ -4427,138 +4051,6 @@
     </rPh>
     <rPh sb="97" eb="98">
       <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ログインしたら、この画面（ダッシュボード）が出ます。&lt;span class="check"&gt;check-8&lt;/span&gt;
-真ん中に見える「コースツリー」に、あなたがアクセスできるコースが表示されています。これらは、あなたの履修課目に関する授業支援や、広島大学において自習すべき教材などのコースです。（この図は在学生向けの一例で、新入生に表示されるものとは異なります）
-新入生向けに共通で表示されるものを簡単に説明すると：
-&lt;dl&gt;
-&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
-&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届」を提出する必要があります。このコースでは、点検届が提出できます。&lt;strong&gt;このテキストによる設定・点検を済ませたあと、できるだけ早くにこのコースを開いて点検届を提出してください。&lt;/strong&gt;&lt;/dd&gt;
-&lt;dt&gt;MFA設定ガイド&lt;/dt&gt;
-&lt;dd&gt;広島大学ではパスワード窃取・アカウント乗っ取りの防止策として、広大IDを持つ全ての構成員に対しIMCアカウントおよび広大IDの多要素認証（MFA）設定を義務付けています。この「MFA設定ガイド」で、広島大学でMFA設定を行うための手順を説明しています&lt;/dd&gt; &lt;/dl&gt;
-</t>
-    <rPh sb="65" eb="66">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="111" eb="113">
-      <t>リシュウ</t>
-    </rPh>
-    <rPh sb="113" eb="115">
-      <t>カモク</t>
-    </rPh>
-    <rPh sb="116" eb="117">
-      <t>カン</t>
-    </rPh>
-    <rPh sb="119" eb="121">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="121" eb="123">
-      <t>シエン</t>
-    </rPh>
-    <rPh sb="125" eb="127">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="127" eb="129">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="133" eb="135">
-      <t>ジシュウ</t>
-    </rPh>
-    <rPh sb="138" eb="140">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="157" eb="158">
-      <t>ム</t>
-    </rPh>
-    <rPh sb="184" eb="187">
-      <t>シンニュウセイ</t>
-    </rPh>
-    <rPh sb="187" eb="188">
-      <t>ム</t>
-    </rPh>
-    <rPh sb="190" eb="192">
-      <t>キョウツウ</t>
-    </rPh>
-    <rPh sb="193" eb="195">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="340" eb="342">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="343" eb="345">
-      <t>テンケン</t>
-    </rPh>
-    <rPh sb="346" eb="347">
-      <t>ス</t>
-    </rPh>
-    <rPh sb="358" eb="359">
-      <t>ハヤ</t>
-    </rPh>
-    <rPh sb="367" eb="368">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="405" eb="407">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="420" eb="424">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="431" eb="433">
-      <t>セッシュ</t>
-    </rPh>
-    <rPh sb="439" eb="440">
-      <t>ノ</t>
-    </rPh>
-    <rPh sb="441" eb="442">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="451" eb="453">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="456" eb="457">
-      <t>モ</t>
-    </rPh>
-    <rPh sb="458" eb="459">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="461" eb="464">
-      <t>コウセイイン</t>
-    </rPh>
-    <rPh sb="465" eb="466">
-      <t>タイ</t>
-    </rPh>
-    <rPh sb="478" eb="480">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="483" eb="488">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="493" eb="495">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="496" eb="499">
-      <t>ギムヅ</t>
-    </rPh>
-    <rPh sb="511" eb="513">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="519" eb="523">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="527" eb="529">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="530" eb="531">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="535" eb="537">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="538" eb="540">
-      <t>セツメイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -4964,41 +4456,6 @@
     </rPh>
     <rPh sb="40" eb="42">
       <t>テイシュツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>IMCアカウントを「@hiroshima-u.ac.jp」つきで入力し、さらにパスワードも入力します。このサイトはMicrosoftのサイトなので、「@hiroshima-u.ac.jp」がついていないと貴方の学生番号がどの大学のものか判らないため、「@hiroshima-u.ac.jp」を加える必要があります。
-※ 学外からのアクセスの場合は、ここで多要素認証（MFA）の認証手続きが入ります</t>
-    <rPh sb="32" eb="34">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="102" eb="104">
-      <t>アナタ</t>
-    </rPh>
-    <rPh sb="105" eb="107">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="107" eb="109">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="112" eb="114">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="118" eb="119">
-      <t>ワカ</t>
-    </rPh>
-    <rPh sb="146" eb="147">
-      <t>クワ</t>
-    </rPh>
-    <rPh sb="149" eb="151">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="170" eb="172">
-      <t>バアイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5178,6 +4635,594 @@
     </rPh>
     <rPh sb="234" eb="235">
       <t>コト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">この章から、テキストにあるリンク（URL）をクリックしてWebブラウザを使うと作業しやすい場面が多くなります。
+できれば作業しているPCでこのテキストを見ながら作業しましょう。ネットワークに接続していればできるはずです。
+&lt;a href="https://www.riise.hiroshima-u.ac.jp/fresta/2022/" target="_blank" rel="noreferrer"&gt;https://www.riise.hiroshima-u.ac.jp/fresta/2022/&lt;/a&gt;
+</t>
+    <rPh sb="2" eb="3">
+      <t>ショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Googleのダウンロードページにジャンプしました。Google Chromeのブラウザ内部のデータをGoogleに送信しても良いかという許可チェックボックスがありますが、このチェックを外してダウンロードを行います。
+※ Edgeを使って作業している場合、右上に「EdgeのほうがChromeより良いですよ」という旨の広告メッセージが出ますが、いまは無視してください。</t>
+    <rPh sb="44" eb="46">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>ソウシン</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>キョカ</t>
+    </rPh>
+    <rPh sb="93" eb="94">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="103" eb="104">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="116" eb="117">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="119" eb="121">
+      <t>サギョウ</t>
+    </rPh>
+    <rPh sb="125" eb="127">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="128" eb="130">
+      <t>ミギウエ</t>
+    </rPh>
+    <rPh sb="148" eb="149">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="157" eb="158">
+      <t>ムネ</t>
+    </rPh>
+    <rPh sb="167" eb="168">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="175" eb="177">
+      <t>ムシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ログインしたら、この画面（ダッシュボード）が出ます。&lt;span class="check"&gt;check-8&lt;/span&gt;
+真ん中に見える「コースツリー」に、あなたがアクセスできるコースが表示されています。これらは、あなたの履修課目に関する授業支援や、広島大学において自習すべき教材などのコースです。（この図は在学生向けの一例で、新入生に表示されるものとは異なります）
+新入生向けに共通で表示されるものを簡単に説明すると：
+&lt;dl&gt;
+&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
+&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届」を提出する必要があります。このコースでは、点検届が提出できます。&lt;strong&gt;このテキストによる設定・点検を済ませたあと、できるだけ早くにこのコースを開いて点検届を提出してください。&lt;/strong&gt;&lt;/dd&gt;
+&lt;dt&gt;MFA設定ガイド&lt;/dt&gt;
+&lt;dd&gt;広島大学ではパスワード窃取によるアカウント乗っ取りの防止策として、広大IDを持つ全ての構成員に対しIMCアカウントおよび広大IDの多要素認証（MFA）設定を義務付けています。この「MFA設定ガイド」で、広島大学でMFA設定を行うための手順を説明しています&lt;/dd&gt; &lt;/dl&gt;
+</t>
+    <rPh sb="65" eb="66">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="111" eb="113">
+      <t>リシュウ</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>カモク</t>
+    </rPh>
+    <rPh sb="116" eb="117">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="119" eb="121">
+      <t>ジュギョウ</t>
+    </rPh>
+    <rPh sb="121" eb="123">
+      <t>シエン</t>
+    </rPh>
+    <rPh sb="125" eb="127">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="127" eb="129">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="133" eb="135">
+      <t>ジシュウ</t>
+    </rPh>
+    <rPh sb="138" eb="140">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="157" eb="158">
+      <t>ム</t>
+    </rPh>
+    <rPh sb="184" eb="187">
+      <t>シンニュウセイ</t>
+    </rPh>
+    <rPh sb="187" eb="188">
+      <t>ム</t>
+    </rPh>
+    <rPh sb="190" eb="192">
+      <t>キョウツウ</t>
+    </rPh>
+    <rPh sb="193" eb="195">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="340" eb="342">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="343" eb="345">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="346" eb="347">
+      <t>ス</t>
+    </rPh>
+    <rPh sb="358" eb="359">
+      <t>ハヤ</t>
+    </rPh>
+    <rPh sb="367" eb="368">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="405" eb="407">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="420" eb="424">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="431" eb="433">
+      <t>セッシュ</t>
+    </rPh>
+    <rPh sb="441" eb="442">
+      <t>ノ</t>
+    </rPh>
+    <rPh sb="443" eb="444">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="453" eb="455">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="458" eb="459">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="460" eb="461">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="463" eb="466">
+      <t>コウセイイン</t>
+    </rPh>
+    <rPh sb="467" eb="468">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="480" eb="482">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="485" eb="490">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="495" eb="497">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="498" eb="501">
+      <t>ギムヅ</t>
+    </rPh>
+    <rPh sb="513" eb="515">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="521" eb="525">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="529" eb="531">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="532" eb="533">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="537" eb="539">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="540" eb="542">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Microsoft Teams について。最近のWindows10パソコンでは、サインイン時にMicrosoft Teams が自動的に起動します。これはMicrosoftが提供しているグループチャットアプリで、広大メールアドレスとパスワードでサインインして使うことができます。COVID-19の影響もあって広島大学でもTeamsを使ってリモートで行う授業が多くなりました。
+このテキストの後ろにある付録でひととおり説明しています。さらに詳細はメディアセンターWebサイトの&lt;a href="https://www.media.hiroshima-u.ac.jp/services/communication/teams/"&gt;「Microsoft Teams」&lt;/a&gt;で。
+※ 使わない場合は画面左下のウィンドウアイコンから「設定」→「アプリ」→「スタートアップ」と進んでTeamsのスイッチを「オフ」にすると、自動起動を止めることができます。</t>
+    <rPh sb="21" eb="23">
+      <t>サイキン</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="64" eb="67">
+      <t>ジドウテキ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="106" eb="108">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="129" eb="130">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="148" eb="150">
+      <t>エイキョウ</t>
+    </rPh>
+    <rPh sb="154" eb="158">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="166" eb="167">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="176" eb="178">
+      <t>ジュギョウ</t>
+    </rPh>
+    <rPh sb="179" eb="180">
+      <t>オオ</t>
+    </rPh>
+    <rPh sb="219" eb="221">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="339" eb="340">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="343" eb="345">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="383" eb="384">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ここでは、&lt;strong&gt;まだOfficeがインストールされていないPCに&lt;/strong&gt;広島大学の提供するMicrosoft 365 Apps for enterpriseをダウンロードしてインストールする方法を説明します。</t>
+    <rPh sb="46" eb="48">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="105" eb="107">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="108" eb="110">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2&gt;広島大学学生向けMicrosoft 365 Apps for enterpriseのインストール&lt;/h2&gt;</t>
+    <rPh sb="4" eb="6">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ム</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>あとは画面の指示に従ってインストーラーを保存し、そのインストーラーを起動するとMicrosoft 365 Apps for enterpriseがインストールされます。利用規約に同意し、ライセンス認証のために広大メールアドレスを再度入力してしばらく待つとインストール完了です。
+&lt;p class="spl"&gt;※この方法でインストールしたOfficeは広大メールアドレスによってライセンス認証されているので、すぐに使うことができます。ただしこの章の最初に書いたように、&lt;strong&gt;広島大学を卒業した後は利用できなくなります&lt;/strong&gt;ので注意してください。&lt;/p&gt;</t>
+    <rPh sb="3" eb="5">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>シジ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ホゾン</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>キドウ</t>
+    </rPh>
+    <rPh sb="98" eb="100">
+      <t>ニンショウ</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="114" eb="116">
+      <t>サイド</t>
+    </rPh>
+    <rPh sb="116" eb="118">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="124" eb="125">
+      <t>マ</t>
+    </rPh>
+    <rPh sb="133" eb="135">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="157" eb="159">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="175" eb="177">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="193" eb="195">
+      <t>ニンショウ</t>
+    </rPh>
+    <rPh sb="206" eb="207">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="221" eb="222">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="223" eb="225">
+      <t>サイショ</t>
+    </rPh>
+    <rPh sb="226" eb="227">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="241" eb="243">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="243" eb="245">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="246" eb="248">
+      <t>ソツギョウ</t>
+    </rPh>
+    <rPh sb="250" eb="251">
+      <t>アト</t>
+    </rPh>
+    <rPh sb="252" eb="254">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="273" eb="275">
+      <t>チュウイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>包括ライセンスでMicrosoft 365 Apps for enterpriseをインストールした場合は、Microsoft Teamsは既にインストールされている筈です。検索ウィンドウで「Teams」を検索すれば出てくる筈です。
+もし別途Officeを購入したため、Microsoft Teamsがまだ入っていないという場合は、https://www.microsoft.com/ja-jp/microsoft-teams/download-app からダウンロードしてインストールしてください(Office365と違ってアカウントにサインインしなくてもダウンロードできます)。また、iOS機器(iPhone, iPad)やAndroid機器でも動きますが、ここではPCでの確認手順を説明します。</t>
+    <rPh sb="0" eb="2">
+      <t>ホウカツ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="70" eb="71">
+      <t>スデ</t>
+    </rPh>
+    <rPh sb="83" eb="84">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="87" eb="89">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="103" eb="105">
+      <t>ケンサク</t>
+    </rPh>
+    <rPh sb="108" eb="109">
+      <t>デ</t>
+    </rPh>
+    <rPh sb="112" eb="113">
+      <t>ハズ</t>
+    </rPh>
+    <rPh sb="119" eb="121">
+      <t>ベット</t>
+    </rPh>
+    <rPh sb="128" eb="130">
+      <t>コウニュウ</t>
+    </rPh>
+    <rPh sb="153" eb="154">
+      <t>ハイ</t>
+    </rPh>
+    <rPh sb="162" eb="164">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="260" eb="261">
+      <t>チガ</t>
+    </rPh>
+    <rPh sb="297" eb="299">
+      <t>キキ</t>
+    </rPh>
+    <rPh sb="321" eb="323">
+      <t>キキ</t>
+    </rPh>
+    <rPh sb="325" eb="326">
+      <t>ウゴ</t>
+    </rPh>
+    <rPh sb="339" eb="341">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="341" eb="343">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="344" eb="346">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>（付録）Office365アプリのインストール手順、Microsoft Teamsの使い方</t>
+    <rPh sb="1" eb="3">
+      <t>フロク</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;ul&gt;
+&lt;li&gt;&lt;a href="#office365"&gt;Office365アプリのインストール&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#teams"&gt;Teamsの使い方&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
+    <rPh sb="86" eb="87">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="88" eb="89">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2&gt;&lt;a name="office365"&gt;Office365アプリのインストール&lt;/a&gt;&lt;/h2&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広島大学では、マイクロソフト社との包括ライセンス契約（Microsoft Enrollment for Education Solutions）を結んでいます。これによって広島大学の学生は広島大学が定める利用要領に基づいて、いくつかのマイクロソフト社製ソフトウェア製品（Microsoft Office等）を無償で利用することができます。
+Microsoft Office については、広島大学の学生は個人所有のPCで５台まで無償で利用することができます。
+ただしこのOffice 365アプリはマイクロソフトのサーバに登録されている広島大学のアカウントに関係づけられており、卒業（もしくは退学）後は利用できなくなってしまいますので、ご注意ください。
+&lt;p class="spl"&gt;※ 「Microsoft 365 Apps for enterprise」は以前「Office 365 ProPlus」だったものが2020年に改称されたものです。このため関連する説明の中で「Office 365 ProPlus」の呼称が残っている場合があります。Office365アプリとしての位置づけは変わりませんので、適当に読み替えてください。&lt;/p&gt;</t>
+    <rPh sb="0" eb="2">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>シャ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ホウカツ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ケイヤク</t>
+    </rPh>
+    <rPh sb="73" eb="74">
+      <t>ムス</t>
+    </rPh>
+    <rPh sb="86" eb="88">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="88" eb="90">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="91" eb="93">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="96" eb="98">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="99" eb="100">
+      <t>サダ</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="104" eb="106">
+      <t>ヨウリョウ</t>
+    </rPh>
+    <rPh sb="107" eb="108">
+      <t>モト</t>
+    </rPh>
+    <rPh sb="124" eb="125">
+      <t>シャ</t>
+    </rPh>
+    <rPh sb="125" eb="126">
+      <t>セイ</t>
+    </rPh>
+    <rPh sb="132" eb="134">
+      <t>セイヒン</t>
+    </rPh>
+    <rPh sb="151" eb="152">
+      <t>トウ</t>
+    </rPh>
+    <rPh sb="154" eb="156">
+      <t>ムショウ</t>
+    </rPh>
+    <rPh sb="157" eb="159">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="379" eb="381">
+      <t>イゼン</t>
+    </rPh>
+    <rPh sb="411" eb="412">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="427" eb="429">
+      <t>カンレン</t>
+    </rPh>
+    <rPh sb="431" eb="433">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="434" eb="435">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="457" eb="459">
+      <t>コショウ</t>
+    </rPh>
+    <rPh sb="460" eb="461">
+      <t>ノコ</t>
+    </rPh>
+    <rPh sb="465" eb="467">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="503" eb="505">
+      <t>テキトウ</t>
+    </rPh>
+    <rPh sb="506" eb="507">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="508" eb="509">
+      <t>カ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IMCアカウントを「@hiroshima-u.ac.jp」つきで入力し、さらにパスワードも入力します。このサイトはMicrosoftのサイトなので、「@hiroshima-u.ac.jp」がついていないと貴方の学生番号がどの大学のものか判らないため、「@hiroshima-u.ac.jp」を加える必要があります。
+※ 学外からのアクセスの場合は、ここで多要素認証（MFA）の認証手続きが入ります。</t>
+    <rPh sb="32" eb="34">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="102" eb="104">
+      <t>アナタ</t>
+    </rPh>
+    <rPh sb="105" eb="107">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="107" eb="109">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="112" eb="114">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="118" eb="119">
+      <t>ワカ</t>
+    </rPh>
+    <rPh sb="146" eb="147">
+      <t>クワ</t>
+    </rPh>
+    <rPh sb="149" eb="151">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="170" eb="172">
+      <t>バアイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5624,7 +5669,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5640,7 +5685,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -5648,7 +5693,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -5662,7 +5707,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5683,7 +5728,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5696,10 +5741,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5723,17 +5768,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5741,30 +5786,30 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="D9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5789,8 +5834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392D1BFF-FF5C-4A7E-8C9C-E750AF0FFFAF}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5806,7 +5851,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5814,7 +5859,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5830,22 +5875,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>244</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>245</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>246</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5853,7 +5898,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>226</v>
+        <v>310</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -5867,69 +5912,69 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="102" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>227</v>
+        <v>317</v>
       </c>
       <c r="D14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>93</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="D16" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
       <c r="D17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D18" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="D19" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>229</v>
+        <v>312</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -5940,216 +5985,216 @@
     </row>
     <row r="27" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>130</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C29" t="s">
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
       </c>
       <c r="D38" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="102" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C41" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D41" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -6163,7 +6208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -6181,7 +6226,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s" ph="1">
-        <v>317</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6189,7 +6234,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s" ph="1">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6205,7 +6250,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s" ph="1">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
@@ -6213,7 +6258,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6224,7 +6269,7 @@
     </row>
     <row r="7" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s" ph="1">
-        <v>316</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -6232,13 +6277,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="57.4" ph="1" x14ac:dyDescent="0.25">
@@ -6246,7 +6291,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s" ph="1">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>7</v>
@@ -6260,13 +6305,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s" ph="1">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -6274,7 +6319,7 @@
         <v>68</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -6288,7 +6333,7 @@
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="133.9" ph="1" x14ac:dyDescent="0.25">
@@ -6296,29 +6341,29 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s" ph="1">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s" ph="1">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s" ph="1">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="114.75" ph="1" x14ac:dyDescent="0.25">
@@ -6332,7 +6377,7 @@
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="95.65" ph="1" x14ac:dyDescent="0.25">
@@ -6340,13 +6385,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s" ph="1">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
@@ -6354,13 +6399,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s" ph="1">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6368,7 +6413,7 @@
         <v>62</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="114.75" ph="1" x14ac:dyDescent="0.25">
@@ -6376,13 +6421,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s" ph="1">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6390,18 +6435,18 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s" ph="1">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="57.4" ph="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s" ph="1">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D22" t="s" ph="1">
         <v>76</v>
@@ -6412,7 +6457,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s" ph="1">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
@@ -6426,24 +6471,24 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s" ph="1">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s" ph="1">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -6451,7 +6496,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s" ph="1">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
@@ -6488,7 +6533,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6496,7 +6541,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6512,7 +6557,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
@@ -6520,7 +6565,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6548,7 +6593,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -6576,7 +6621,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -6590,7 +6635,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -6604,7 +6649,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -6632,7 +6677,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6646,7 +6691,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -6683,7 +6728,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6691,7 +6736,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6707,7 +6752,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6715,7 +6760,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6731,7 +6776,7 @@
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6800,7 +6845,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6819,7 +6864,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -6833,7 +6878,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -6847,7 +6892,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -6875,7 +6920,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -6889,13 +6934,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -6910,7 +6955,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView topLeftCell="A17" zoomScale="118" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6926,7 +6971,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6934,7 +6979,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6950,7 +6995,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -6958,7 +7003,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6974,65 +7019,65 @@
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="D9" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="D10" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="D11" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="D12" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="D13" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>271</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -7040,42 +7085,42 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>290</v>
+        <v>307</v>
       </c>
       <c r="D17" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="D18" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="D19" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="D20" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="D21" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7083,7 +7128,7 @@
         <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -7097,8 +7142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475A5B02-452F-483B-8907-D83726E9A70E}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7114,7 +7159,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7122,7 +7167,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7138,7 +7183,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -7149,7 +7194,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7165,15 +7210,15 @@
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="D9" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7181,13 +7226,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
@@ -7195,18 +7240,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>292</v>
+        <v>308</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7214,7 +7259,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7225,7 +7270,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7236,7 +7281,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7252,8 +7297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DD8924-3FAE-44AB-A508-09E9136389D4}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7269,7 +7314,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7277,7 +7322,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7293,7 +7338,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7301,7 +7346,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7312,12 +7357,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7325,7 +7370,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -7336,7 +7381,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7344,21 +7389,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D12" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7366,18 +7411,18 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7385,13 +7430,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7399,13 +7444,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -7435,8 +7480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7460,7 +7505,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7476,7 +7521,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="255" x14ac:dyDescent="0.25">
@@ -7484,7 +7529,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7517,13 +7562,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -7547,53 +7592,53 @@
     </row>
     <row r="12" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="D12" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="D13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="D14" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="D15" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="D16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -7604,12 +7649,12 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -7631,29 +7676,29 @@
         <v>4</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="D23" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="D24" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7661,7 +7706,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -7675,7 +7720,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -7705,7 +7750,7 @@
     </row>
     <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -7713,7 +7758,7 @@
     </row>
     <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -7724,7 +7769,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -7738,7 +7783,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -7749,7 +7794,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
@@ -7763,7 +7808,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -7777,12 +7822,12 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7790,7 +7835,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
@@ -7827,9 +7872,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>79</v>
+        <v>309</v>
       </c>
       <c r="D40" t="s" ph="1">
         <v>65</v>
@@ -7864,7 +7909,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7888,7 +7933,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7904,12 +7949,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7917,7 +7962,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -7931,7 +7976,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -7945,7 +7990,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -7959,7 +8004,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7987,7 +8032,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -8012,7 +8057,7 @@
     </row>
     <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
         <v>59</v>
@@ -8023,7 +8068,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -8037,7 +8082,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
fix win10_en to match win10(ja)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85BE829F-4769-44E0-99DA-1629A629D974}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B503AD35-5481-4A0C-9774-19FCE6485A0E}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="-14595" windowWidth="18225" windowHeight="11880" tabRatio="782" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13365" yWindow="-15225" windowWidth="18225" windowHeight="11880" tabRatio="782" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="318">
   <si>
     <t>header1</t>
   </si>
@@ -4901,22 +4901,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>&lt;h2&gt;広島大学学生向けMicrosoft 365 Apps for enterpriseのインストール&lt;/h2&gt;</t>
-    <rPh sb="4" eb="6">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>ム</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>あとは画面の指示に従ってインストーラーを保存し、そのインストーラーを起動するとMicrosoft 365 Apps for enterpriseがインストールされます。利用規約に同意し、ライセンス認証のために広大メールアドレスを再度入力してしばらく待つとインストール完了です。
 &lt;p class="spl"&gt;※この方法でインストールしたOfficeは広大メールアドレスによってライセンス認証されているので、すぐに使うことができます。ただしこの章の最初に書いたように、&lt;strong&gt;広島大学を卒業した後は利用できなくなります&lt;/strong&gt;ので注意してください。&lt;/p&gt;</t>
     <rPh sb="3" eb="5">
@@ -5052,35 +5036,6 @@
     </rPh>
     <rPh sb="344" eb="346">
       <t>セツメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>（付録）Office365アプリのインストール手順、Microsoft Teamsの使い方</t>
-    <rPh sb="1" eb="3">
-      <t>フロク</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="42" eb="43">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="44" eb="45">
-      <t>カタ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;ul&gt;
-&lt;li&gt;&lt;a href="#office365"&gt;Office365アプリのインストール&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;&lt;a href="#teams"&gt;Teamsの使い方&lt;/a&gt;&lt;/li&gt;
-&lt;/ul&gt;</t>
-    <rPh sb="86" eb="87">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="88" eb="89">
-      <t>カタ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5223,6 +5178,39 @@
     </rPh>
     <rPh sb="170" eb="172">
       <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Office365アプリのインストール手順、Microsoft Teamsの使い方
+&lt;ul&gt;
+&lt;li&gt;&lt;a href="#office365"&gt;Office365アプリのインストール&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#teams"&gt;Teamsの使い方&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
+    <rPh sb="19" eb="21">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>カタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3&gt;広島大学学生向けMicrosoft 365 Apps for enterpriseのインストール&lt;/h3&gt;</t>
+    <rPh sb="4" eb="6">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ガクセイ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ム</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5832,10 +5820,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392D1BFF-FF5C-4A7E-8C9C-E750AF0FFFAF}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5878,322 +5866,317 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>315</v>
+      <c r="D9" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="D13" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D16" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="D17" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D18" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="D19" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>313</v>
+        <v>162</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>133</v>
+        <v>164</v>
       </c>
       <c r="C29" t="s">
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>162</v>
+        <v>108</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>108</v>
+        <v>159</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" ht="51" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="102" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>155</v>
       </c>
       <c r="D38" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="51" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="102" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C41" t="s">
-        <v>155</v>
+        <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C45" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C46" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C47" t="s">
-        <v>7</v>
-      </c>
-      <c r="D47" t="s">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix checklist numbers win10en/11en
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="170" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{799866B6-E4FE-44B5-BDF8-C1C7ADF06D8D}"/>
+  <xr:revisionPtr revIDLastSave="171" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B3BCF49-B728-4EC2-9DBA-D6D28FC824D3}"/>
   <bookViews>
-    <workbookView xWindow="1298" yWindow="765" windowWidth="18225" windowHeight="11873" tabRatio="782" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10275" yWindow="-13845" windowWidth="18225" windowHeight="11880" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -6194,24 +6194,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="19.149999999999999" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1" phonetic="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1" phonetic="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1" phonetic="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1" phonetic="1"/>
     <col min="5" max="16384" width="8.796875" phonetic="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="57.4" ph="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s" ph="1">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s" ph="1">
+      <c r="B1" s="1" t="s">
         <v>302</v>
       </c>
     </row>
@@ -6219,7 +6219,7 @@
       <c r="A2" t="s" ph="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s" ph="1">
+      <c r="B2" s="1" t="s">
         <v>172</v>
       </c>
     </row>
@@ -6227,7 +6227,7 @@
       <c r="A3" t="s" ph="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s" ph="1">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -6235,7 +6235,7 @@
       <c r="A4" t="s" ph="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s" ph="1">
+      <c r="B4" s="1" t="s">
         <v>217</v>
       </c>
     </row>
@@ -6243,7 +6243,7 @@
       <c r="A6" t="s" ph="1">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s" ph="1">
+      <c r="B6" s="1" t="s">
         <v>303</v>
       </c>
       <c r="C6" t="s" ph="1">
@@ -6254,15 +6254,15 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s" ph="1">
+      <c r="B7" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s" ph="1">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="s" ph="1">
+      <c r="B8" s="1" t="s">
         <v>300</v>
       </c>
       <c r="C8" t="s" ph="1">
@@ -6272,11 +6272,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="57.4" ph="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s" ph="1">
         <v>4</v>
       </c>
-      <c r="B9" s="1" t="s" ph="1">
+      <c r="B9" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C9" t="s" ph="1">
@@ -6286,11 +6286,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s" ph="1">
         <v>4</v>
       </c>
-      <c r="B10" s="1" t="s" ph="1">
+      <c r="B10" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C10" t="s" ph="1">
@@ -6300,19 +6300,19 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s" ph="1">
+    <row r="11" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D11" t="s" ph="1">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s" ph="1">
         <v>4</v>
       </c>
-      <c r="B12" s="1" t="s" ph="1">
+      <c r="B12" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C12" t="s" ph="1">
@@ -6322,11 +6322,11 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="133.9" ph="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="89.25" ph="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s" ph="1">
         <v>4</v>
       </c>
-      <c r="B13" s="1" t="s" ph="1">
+      <c r="B13" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C13" t="s" ph="1">
@@ -6336,27 +6336,27 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s" ph="1">
+    <row r="14" spans="1:4" ht="51" ph="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>101</v>
       </c>
       <c r="D14" t="s" ph="1">
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s" ph="1">
+    <row r="15" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>126</v>
       </c>
       <c r="D15" t="s" ph="1">
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="114.75" ph="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s" ph="1">
         <v>4</v>
       </c>
-      <c r="B16" s="1" t="s" ph="1">
+      <c r="B16" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C16" t="s" ph="1">
@@ -6366,11 +6366,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="95.65" ph="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="63.75" ph="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s" ph="1">
         <v>4</v>
       </c>
-      <c r="B17" s="1" t="s" ph="1">
+      <c r="B17" s="1" t="s">
         <v>103</v>
       </c>
       <c r="C17" t="s" ph="1">
@@ -6380,11 +6380,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="51" ph="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s" ph="1">
         <v>4</v>
       </c>
-      <c r="B18" s="1" t="s" ph="1">
+      <c r="B18" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C18" t="s" ph="1">
@@ -6395,18 +6395,18 @@
       </c>
     </row>
     <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s" ph="1">
+      <c r="B19" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D19" t="s" ph="1">
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="114.75" ph="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s" ph="1">
         <v>4</v>
       </c>
-      <c r="B20" s="1" t="s" ph="1">
+      <c r="B20" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C20" t="s" ph="1">
@@ -6420,7 +6420,7 @@
       <c r="A21" t="s" ph="1">
         <v>4</v>
       </c>
-      <c r="B21" s="1" t="s" ph="1">
+      <c r="B21" s="1" t="s">
         <v>168</v>
       </c>
       <c r="C21" t="s" ph="1">
@@ -6430,19 +6430,19 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="57.4" ph="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s" ph="1">
+    <row r="22" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>169</v>
       </c>
       <c r="D22" t="s" ph="1">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="95.65" ph="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="63.75" ph="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s" ph="1">
         <v>4</v>
       </c>
-      <c r="B23" s="1" t="s" ph="1">
+      <c r="B23" s="1" t="s">
         <v>170</v>
       </c>
       <c r="C23" t="s" ph="1">
@@ -6452,11 +6452,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="133.9" ph="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="89.25" ph="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s" ph="1">
         <v>4</v>
       </c>
-      <c r="B24" s="1" t="s" ph="1">
+      <c r="B24" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C24" t="s" ph="1">
@@ -6467,7 +6467,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s" ph="1">
+      <c r="B25" s="1" t="s">
         <v>123</v>
       </c>
       <c r="C25" t="s" ph="1">
@@ -6477,11 +6477,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s" ph="1">
         <v>4</v>
       </c>
-      <c r="B26" s="1" t="s" ph="1">
+      <c r="B26" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C26" t="s" ph="1">
@@ -7128,8 +7128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475A5B02-452F-483B-8907-D83726E9A70E}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="90" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add access to Bb9 with myMOMIJI win10(ja)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="171" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B3BCF49-B728-4EC2-9DBA-D6D28FC824D3}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{039F8D5A-2470-4B72-9E4F-885A6E3B2BBF}"/>
   <bookViews>
-    <workbookView xWindow="10275" yWindow="-13845" windowWidth="18225" windowHeight="11880" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3600" yWindow="-15450" windowWidth="18225" windowHeight="11880" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="321">
   <si>
     <t>header1</t>
   </si>
@@ -3009,34 +3009,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">Myもみじのトップページに表示されている時間割の中に「大学教育入門」のリンクがあるはずです。
-これをクリックするとBb9の「大学教育入門」コースに直接アクセスできます。
-&lt;font color="red"&gt;※ 画面イメージ未撮影&lt;/font&gt;
-  </t>
-    <rPh sb="13" eb="15">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="20" eb="23">
-      <t>ジカンワリ</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="27" eb="33">
-      <t>ダイガクキョウイクニュウモン</t>
-    </rPh>
-    <rPh sb="62" eb="68">
-      <t>ダイガクキョウイクニュウモン</t>
-    </rPh>
-    <rPh sb="73" eb="75">
-      <t>チョクセツ</t>
-    </rPh>
-    <rPh sb="111" eb="114">
-      <t>ミサツエイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">Bb9の「大学教育入門」コースのトップページが表示されます。ここで「大学教育入門」の教材の閲覧およびダウンロードや、課題の提出などができます。
 「大学教育入門」は、大学で学ぶにあたり必要な事柄や、広島大学特有の事情について学習する授業です。全学部生必修です。このコースでは、授業の各週で使う資料をダウンロードしたり、確認テストを受験したりします。
 &lt;font color="red"&gt;※ 画面イメージ未撮影&lt;/font&gt;
@@ -5214,6 +5186,64 @@
     </rPh>
     <rPh sb="35" eb="37">
       <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mymomiji-intro.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mymomiji-topintro.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Myもみじのトップページに表示されている時間割の中に「大学教育入門」のリンクがあるはずです。
+これをクリックして「大学教育入門」の詳細画面に移動します。
+&lt;font color="red"&gt;※ 画面はイメージです&lt;/font&gt;
+  </t>
+    <rPh sb="13" eb="15">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="20" eb="23">
+      <t>ジカンワリ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="27" eb="33">
+      <t>ダイガクキョウイクニュウモン</t>
+    </rPh>
+    <rPh sb="57" eb="63">
+      <t>ダイガクキョウイクニュウモン</t>
+    </rPh>
+    <rPh sb="65" eb="69">
+      <t>ショウサイガメン</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>イドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「大学教育入門」の詳細画面の中に「Bb9へ」というリンクがあるはずです。
+これをクリックするとBb9の「大学教育入門」コースに直接アクセスできます。
+&lt;font color="red"&gt;※ 画面はイメージです&lt;/font&gt;
+  </t>
+    <rPh sb="1" eb="7">
+      <t>ダイガクキョウイクニュウモン</t>
+    </rPh>
+    <rPh sb="9" eb="13">
+      <t>ショウサイガメン</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="52" eb="58">
+      <t>ダイガクキョウイクニュウモン</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>チョクセツ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5660,7 +5690,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5777,12 +5807,12 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D9" t="s">
         <v>178</v>
@@ -5790,7 +5820,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5842,7 +5872,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5850,7 +5880,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5866,12 +5896,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5881,7 +5911,7 @@
     </row>
     <row r="9" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D9" t="s">
         <v>92</v>
@@ -5889,7 +5919,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5897,7 +5927,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -5908,20 +5938,20 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D13" t="s">
         <v>242</v>
-      </c>
-      <c r="D13" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D14" t="s">
         <v>199</v>
@@ -5937,7 +5967,7 @@
     </row>
     <row r="16" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D16" t="s">
         <v>221</v>
@@ -5945,17 +5975,17 @@
     </row>
     <row r="17" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -5971,7 +6001,7 @@
     </row>
     <row r="24" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -6194,7 +6224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -6212,7 +6242,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6244,7 +6274,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6255,7 +6285,7 @@
     </row>
     <row r="7" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -6263,7 +6293,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
@@ -6519,7 +6549,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6551,7 +6581,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6579,7 +6609,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -6663,7 +6693,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6677,7 +6707,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -6746,7 +6776,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6831,7 +6861,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6850,7 +6880,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -6864,7 +6894,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -6989,7 +7019,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7010,42 +7040,42 @@
     </row>
     <row r="9" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D10" t="s">
         <v>246</v>
-      </c>
-      <c r="D10" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D11" t="s">
         <v>248</v>
-      </c>
-      <c r="D11" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D12" t="s">
         <v>250</v>
-      </c>
-      <c r="D12" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -7055,12 +7085,12 @@
     </row>
     <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D16" t="s">
         <v>94</v>
@@ -7071,42 +7101,42 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D18" t="s">
         <v>261</v>
-      </c>
-      <c r="D18" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D19" t="s">
         <v>263</v>
-      </c>
-      <c r="D19" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D20" t="s">
         <v>265</v>
-      </c>
-      <c r="D20" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D21" t="s">
         <v>267</v>
-      </c>
-      <c r="D21" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7114,7 +7144,7 @@
         <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -7145,7 +7175,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7153,7 +7183,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7180,7 +7210,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7201,7 +7231,7 @@
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D9" t="s">
         <v>178</v>
@@ -7226,7 +7256,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7245,7 +7275,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7256,7 +7286,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7343,12 +7373,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7367,7 +7397,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7375,13 +7405,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7408,7 +7438,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7464,10 +7494,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7515,7 +7545,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7548,7 +7578,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -7578,15 +7608,15 @@
     </row>
     <row r="12" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D13" t="s">
         <v>199</v>
@@ -7594,7 +7624,7 @@
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D14" t="s">
         <v>201</v>
@@ -7602,15 +7632,15 @@
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D16" t="s">
         <v>202</v>
@@ -7618,7 +7648,7 @@
     </row>
     <row r="17" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -7640,7 +7670,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -7662,7 +7692,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -7673,7 +7703,7 @@
     </row>
     <row r="23" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D23" t="s">
         <v>180</v>
@@ -7681,10 +7711,10 @@
     </row>
     <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D24" t="s">
         <v>238</v>
-      </c>
-      <c r="D24" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7692,7 +7722,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -7706,7 +7736,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -7744,144 +7774,158 @@
     </row>
     <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="1" t="s">
+    <row r="35" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
       <c r="B36" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="1" t="s">
+    <row r="38" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C37" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="C38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="102" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="102" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="D40" t="s" ph="1">
+    <row r="41" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D41" t="s" ph="1">
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="1" t="s">
+    <row r="42" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>7</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="4:4" ht="19.149999999999999" x14ac:dyDescent="0.25">
-      <c r="D49" ph="1"/>
+    <row r="50" spans="4:4" ht="19.149999999999999" x14ac:dyDescent="0.25">
+      <c r="D50" ph="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -7940,7 +7984,7 @@
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7962,7 +8006,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
fix a pic win10(ja)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="181" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{039F8D5A-2470-4B72-9E4F-885A6E3B2BBF}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB265E06-2CE5-4403-9690-C96C3928FA3D}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="-15450" windowWidth="18225" windowHeight="11880" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5190,10 +5190,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>mymomiji-intro.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>mymomiji-topintro.svg</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -5245,6 +5241,10 @@
     <rPh sb="63" eb="65">
       <t>チョクセツ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mymomiji-intro.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -7497,7 +7497,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7774,24 +7774,24 @@
     </row>
     <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
         <v>320</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix some typo win10(ja)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="245" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37DF3C40-B0E1-4D5E-B33D-58F854E61A02}"/>
+  <xr:revisionPtr revIDLastSave="250" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13BDF525-CA85-4750-B63A-2A047CD77C2F}"/>
   <bookViews>
-    <workbookView xWindow="1508" yWindow="405" windowWidth="19860" windowHeight="11880" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="203" yWindow="4320" windowWidth="19860" windowHeight="11880" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="331">
   <si>
     <t>header1</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>win10-5-09.svg</t>
-  </si>
-  <si>
-    <t>電子メールやクラウドストレージが使えるOffice365、オンライン履修登録などをおこなう「もみじ」、オンライン学習支援システムのBb9など、大学で提供されているネットワークサービスを使えるように設定します。</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;h2&gt;&lt;a name="momiji"&gt;&lt;/a&gt;もみじ (広大学生用ポータルサイト)&lt;/h2&gt; </t>
@@ -4001,27 +3998,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">この実習では、このままで次の「Bb9」の使い方に進みます。
-※ Myもみじの閲覧が済んだら、できるだけ画面右上の「ログアウト」をクリックするようにしましょう。
-  </t>
-    <rPh sb="2" eb="4">
-      <t>ジッシュウ</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="22" eb="23">
-      <t>カタ</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;strong&gt;※ ここまでの実習の中で、広島大学には２つのオンライン学習支援システム「広大moodle」「Bb9」があることに気づかれたと思います。
 広島大学では今年度「広大moodle」「Bb9」の２つのオンライン学習支援システムを併用します。来年度からは「広大moodle」に一本化する予定です。
 しばらく面倒をおかけしますが、ご了解ください。&lt;/strong&gt;</t>
@@ -4924,56 +4900,6 @@
   </si>
   <si>
     <t>mymomiji-topintro.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Myもみじのトップページに表示されている時間割の中に「大学教育入門」のリンクがあるはずです。
-これをクリックして「大学教育入門」の詳細画面に移動します。
-&lt;font color="red"&gt;※ 画面はイメージです&lt;/font&gt;
-  </t>
-    <rPh sb="13" eb="15">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="20" eb="23">
-      <t>ジカンワリ</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="27" eb="33">
-      <t>ダイガクキョウイクニュウモン</t>
-    </rPh>
-    <rPh sb="57" eb="63">
-      <t>ダイガクキョウイクニュウモン</t>
-    </rPh>
-    <rPh sb="65" eb="69">
-      <t>ショウサイガメン</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>イドウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">「大学教育入門」の詳細画面の中に「Bb9へ」というリンクがあるはずです。
-これをクリックするとBb9の「大学教育入門」コースに直接アクセスできます。
-&lt;font color="red"&gt;※ 画面はイメージです&lt;/font&gt;
-  </t>
-    <rPh sb="1" eb="7">
-      <t>ダイガクキョウイクニュウモン</t>
-    </rPh>
-    <rPh sb="9" eb="13">
-      <t>ショウサイガメン</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="52" eb="58">
-      <t>ダイガクキョウイクニュウモン</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>チョクセツ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5284,20 +5210,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">メディアセンタのMicrosoft 365ポータルサイト&lt;a href="https://www.media.hiroshima-u.ac.jp/services/webmail-portal/" target="_blank" rel="noreferrer"&gt;https://www.media.hiroshima-u.ac.jp/services/webmail-portal/&lt;/a&gt;にジャンプします。水色の「Microsoft365ポータル」を押すと&lt;a href="https://portal.office.com/" target="_blank" rel="noreferrer"&gt;https://portal.office.com/&lt;/a&gt;に移動します。
-※ </t>
-    <rPh sb="205" eb="207">
-      <t>ミズイロ</t>
-    </rPh>
-    <rPh sb="227" eb="228">
-      <t>オ</t>
-    </rPh>
-    <rPh sb="331" eb="333">
-      <t>イドウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>もみじトップページの右側にある「Webメール」バナーをクリックしましょう。</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -5401,6 +5313,85 @@
     <rPh sb="96" eb="98">
       <t>キョウザイ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">この実習では、このまま引き続き次の「Bb9」の使い方に進みます。
+※ Myもみじの閲覧が済んだら、できるだけ画面右上の「ログアウト」をクリックするようにしましょう。
+  </t>
+    <rPh sb="2" eb="4">
+      <t>ジッシュウ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ヒ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ツヅ</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「大学教育入門」の詳細画面の中に「Bb9へ」というリンクがあるはずです。
+これをクリックするとBb9の「大学教育入門」コースに直接アクセスできます。
+  </t>
+    <rPh sb="1" eb="7">
+      <t>ダイガクキョウイクニュウモン</t>
+    </rPh>
+    <rPh sb="9" eb="13">
+      <t>ショウサイガメン</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="52" eb="58">
+      <t>ダイガクキョウイクニュウモン</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>チョクセツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Myもみじのトップページに表示されている時間割の中に「大学教育入門」のリンクがあるはずです。
+これをクリックして「大学教育入門」の詳細画面に移動します。
+  </t>
+    <rPh sb="13" eb="15">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="20" eb="23">
+      <t>ジカンワリ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="27" eb="33">
+      <t>ダイガクキョウイクニュウモン</t>
+    </rPh>
+    <rPh sb="57" eb="63">
+      <t>ダイガクキョウイクニュウモン</t>
+    </rPh>
+    <rPh sb="65" eb="69">
+      <t>ショウサイガメン</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>イドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>電子メールやクラウドストレージが使えるOffice365、オンライン履修登録などをおこなう「もみじ」、オンライン学習支援システムのBb9など、大学で提供されているネットワークサービスを使えるようにしましょう。</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5846,7 +5837,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5862,7 +5853,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -5870,7 +5861,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -5884,7 +5875,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5918,10 +5909,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5929,7 +5920,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5945,17 +5936,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5963,30 +5954,30 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -6028,7 +6019,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6036,7 +6027,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6052,12 +6043,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6067,15 +6058,15 @@
     </row>
     <row r="9" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6083,7 +6074,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -6094,59 +6085,59 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D13" t="s">
         <v>232</v>
-      </c>
-      <c r="D13" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D15" t="s">
         <v>195</v>
-      </c>
-      <c r="D15" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -6157,216 +6148,216 @@
     </row>
     <row r="24" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C27" t="s">
         <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C29" t="s">
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="102" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -6398,7 +6389,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6406,7 +6397,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6422,7 +6413,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
@@ -6430,7 +6421,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6441,7 +6432,7 @@
     </row>
     <row r="7" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -6449,13 +6440,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -6463,13 +6454,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -6477,21 +6468,21 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -6499,13 +6490,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="89.25" ph="1" x14ac:dyDescent="0.25">
@@ -6513,29 +6504,29 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" ph="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
@@ -6543,13 +6534,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="63.75" ph="1" x14ac:dyDescent="0.25">
@@ -6557,13 +6548,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="51" ph="1" x14ac:dyDescent="0.25">
@@ -6571,21 +6562,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
@@ -6593,13 +6584,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6607,21 +6598,21 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="63.75" ph="1" x14ac:dyDescent="0.25">
@@ -6629,13 +6620,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="89.25" ph="1" x14ac:dyDescent="0.25">
@@ -6643,24 +6634,24 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -6668,13 +6659,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -6705,7 +6696,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6713,7 +6704,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6729,7 +6720,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
@@ -6737,7 +6728,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6751,7 +6742,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -6765,7 +6756,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -6779,7 +6770,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -6793,7 +6784,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -6807,7 +6798,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -6821,7 +6812,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -6835,7 +6826,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6849,7 +6840,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6863,7 +6854,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -6900,7 +6891,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6908,7 +6899,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6924,7 +6915,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6932,7 +6923,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6948,7 +6939,7 @@
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6995,7 +6986,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7003,13 +6994,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -7017,7 +7008,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7036,13 +7027,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7050,13 +7041,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
@@ -7064,7 +7055,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -7078,7 +7069,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -7092,13 +7083,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -7106,13 +7097,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -7143,7 +7134,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7151,7 +7142,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7167,7 +7158,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7175,7 +7166,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7191,65 +7182,65 @@
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D10" t="s">
         <v>236</v>
-      </c>
-      <c r="D10" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D11" t="s">
         <v>238</v>
-      </c>
-      <c r="D11" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D12" t="s">
         <v>240</v>
-      </c>
-      <c r="D12" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -7257,50 +7248,50 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="D18" t="s">
         <v>251</v>
-      </c>
-      <c r="D18" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D19" t="s">
         <v>253</v>
-      </c>
-      <c r="D19" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D20" t="s">
         <v>255</v>
-      </c>
-      <c r="D20" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D21" t="s">
         <v>257</v>
-      </c>
-      <c r="D21" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -7331,7 +7322,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7339,7 +7330,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7355,7 +7346,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7363,7 +7354,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7374,12 +7365,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7387,7 +7378,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -7398,7 +7389,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7406,21 +7397,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D12" t="s">
         <v>184</v>
-      </c>
-      <c r="D12" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7428,18 +7419,18 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>186</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7447,13 +7438,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>188</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7461,13 +7452,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -7514,7 +7505,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7522,7 +7513,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7538,7 +7529,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -7549,7 +7540,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7565,12 +7556,12 @@
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -7578,29 +7569,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7608,29 +7599,29 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D14" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="D15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7638,13 +7629,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
         <v>176</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
@@ -7652,18 +7643,18 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7671,7 +7662,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -7682,7 +7673,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -7693,7 +7684,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -7709,8 +7700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7726,7 +7717,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7734,7 +7725,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7750,7 +7741,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="216.75" x14ac:dyDescent="0.25">
@@ -7758,7 +7749,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7769,7 +7760,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7777,18 +7768,18 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -7796,80 +7787,80 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>323</v>
+        <v>231</v>
       </c>
       <c r="D11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -7891,29 +7882,29 @@
         <v>4</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D23" t="s">
         <v>228</v>
-      </c>
-      <c r="D23" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7921,13 +7912,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -7935,18 +7926,18 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>275</v>
+        <v>327</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -7965,7 +7956,7 @@
     </row>
     <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -7973,24 +7964,24 @@
     </row>
     <row r="29" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>304</v>
+        <v>329</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>305</v>
+        <v>328</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7998,13 +7989,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -8012,7 +8003,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C32" t="s">
         <v>4</v>
@@ -8023,32 +8014,32 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D34" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -8056,13 +8047,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -8070,13 +8061,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -8084,12 +8075,12 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -8097,7 +8088,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -8111,13 +8102,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -8125,21 +8116,21 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -8147,13 +8138,13 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="4:4" ht="19.149999999999999" x14ac:dyDescent="0.25">
@@ -8195,7 +8186,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8211,12 +8202,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -8224,7 +8215,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -8238,7 +8229,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -8252,7 +8243,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -8266,7 +8257,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -8294,7 +8285,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -8308,7 +8299,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -8319,10 +8310,10 @@
     </row>
     <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -8330,7 +8321,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -8344,7 +8335,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
access bb9 by MyMOMIJI Win10(ja)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="250" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13BDF525-CA85-4750-B63A-2A047CD77C2F}"/>
+  <xr:revisionPtr revIDLastSave="266" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6D94B2B-9BE0-402F-8317-6060C59D2F97}"/>
   <bookViews>
-    <workbookView xWindow="203" yWindow="4320" windowWidth="19860" windowHeight="11880" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3863" yWindow="1508" windowWidth="18225" windowHeight="11872" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="324">
   <si>
     <t>header1</t>
   </si>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>win10-6-16.svg</t>
-  </si>
-  <si>
-    <t>win10-6-17.svg</t>
   </si>
   <si>
     <t>win10-6-25.svg</t>
@@ -3987,17 +3984,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check-13&lt;/span&gt;
-これを「Myもみじのトップページ」と呼ぶことにしましょう。
-履修登録をしたり、成績を確認することができます。
-また「掲示」では、授業や学部からの連絡が表示されます。
-  </t>
-    <rPh sb="70" eb="71">
-      <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;strong&gt;※ ここまでの実習の中で、広島大学には２つのオンライン学習支援システム「広大moodle」「Bb9」があることに気づかれたと思います。
 広島大学では今年度「広大moodle」「Bb9」の２つのオンライン学習支援システムを併用します。来年度からは「広大moodle」に一本化する予定です。
 しばらく面倒をおかけしますが、ご了解ください。&lt;/strong&gt;</t>
@@ -5218,131 +5204,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">自分の履修科目についての「Bb9」のコース全体を見ることもできます。もみじTOPページに戻って、今度は「Bb9/moodle」のバナーをクリックしましょう。
-&lt;strong&gt;※ 学外にいる場合はこの方法での「Bb9」へのログインはできません。次の次の項目まで飛んでください。&lt;/strong&gt;
-</t>
-    <rPh sb="0" eb="2">
-      <t>ジブン</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>リシュウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>カモク</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ゼンタイ</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="89" eb="91">
-      <t>ガクガイ</t>
-    </rPh>
-    <rPh sb="94" eb="96">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="99" eb="101">
-      <t>ホウホウ</t>
-    </rPh>
-    <rPh sb="121" eb="122">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="123" eb="124">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="125" eb="127">
-      <t>コウモク</t>
-    </rPh>
-    <rPh sb="129" eb="130">
-      <t>ト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>オンライン学習支援システムのページの右側にある「bb9」のバナーをクリックします。</t>
-    <rPh sb="5" eb="9">
-      <t>ガクシュウシエン</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>ミギガワ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>lms-bb9.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">するとログイン画面が開きます。
-「ユーザ名」には広大ID（学生番号と同じ）を、「パスワード」には広大パスワードを入力してください。
-入力したら「ログイン」をクリックします。
-   </t>
-  </si>
-  <si>
-    <t>win10-6-15.svg</t>
-  </si>
-  <si>
-    <t>Bb9にログインしたら、この画面が出ます。
-真ん中の「コース一覧」に、あなたがアクセスできるコースが表示されています。
-これらは、あなたの履修課目に関する授業支援や、広島大学において自習すべき教材などのコースです。</t>
-    <rPh sb="69" eb="71">
-      <t>リシュウ</t>
-    </rPh>
-    <rPh sb="71" eb="73">
-      <t>カモク</t>
-    </rPh>
-    <rPh sb="74" eb="75">
-      <t>カン</t>
-    </rPh>
-    <rPh sb="77" eb="79">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="79" eb="81">
-      <t>シエン</t>
-    </rPh>
-    <rPh sb="83" eb="85">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="85" eb="87">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="91" eb="93">
-      <t>ジシュウ</t>
-    </rPh>
-    <rPh sb="96" eb="98">
-      <t>キョウザイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">この実習では、このまま引き続き次の「Bb9」の使い方に進みます。
-※ Myもみじの閲覧が済んだら、できるだけ画面右上の「ログアウト」をクリックするようにしましょう。
-  </t>
-    <rPh sb="2" eb="4">
-      <t>ジッシュウ</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>ヒ</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>ツヅ</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>カタ</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">「大学教育入門」の詳細画面の中に「Bb9へ」というリンクがあるはずです。
 これをクリックするとBb9の「大学教育入門」コースに直接アクセスできます。
   </t>
@@ -5392,6 +5253,43 @@
   </si>
   <si>
     <t>電子メールやクラウドストレージが使えるOffice365、オンライン履修登録などをおこなう「もみじ」、オンライン学習支援システムのBb9など、大学で提供されているネットワークサービスを使えるようにしましょう。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+各システムの閲覧が済んだら、できるだけ「サインアウト」「ログアウト」するようにしましょう。多くの場合、画面右上にあるアイコンからログアウトできます。
+※ 図は「Myもみじ」でのログアウト方法の例
+  </t>
+    <rPh sb="1" eb="2">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>エツラン</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ス</t>
+    </rPh>
+    <rPh sb="78" eb="79">
+      <t>ズ</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="97" eb="98">
+      <t>レイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check-13&lt;/span&gt;
+これを「Myもみじのトップページ」と呼ぶことにしましょう。
+履修登録をしたり、成績を確認することができます。
+また「掲示」では、授業や学部からの連絡が表示されます。
+このまま引き続いて、次の「Bb9」の使い方に進みましょう。
+  </t>
+    <rPh sb="70" eb="71">
+      <t>ヨ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5837,7 +5735,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5853,7 +5751,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -5861,7 +5759,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -5875,7 +5773,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5909,10 +5807,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5920,7 +5818,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5936,17 +5834,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5954,30 +5852,30 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -6019,7 +5917,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6027,7 +5925,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6043,12 +5941,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6058,15 +5956,15 @@
     </row>
     <row r="9" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6074,7 +5972,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -6085,59 +5983,59 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D13" t="s">
         <v>231</v>
-      </c>
-      <c r="D13" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" t="s">
         <v>194</v>
-      </c>
-      <c r="D15" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -6148,216 +6046,216 @@
     </row>
     <row r="24" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C27" t="s">
         <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C29" t="s">
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
       </c>
       <c r="D30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
       </c>
       <c r="D32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="102" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -6389,7 +6287,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6397,7 +6295,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6413,7 +6311,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
@@ -6421,7 +6319,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6432,7 +6330,7 @@
     </row>
     <row r="7" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -6440,13 +6338,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
@@ -6454,13 +6352,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -6468,21 +6366,21 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -6490,13 +6388,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="89.25" ph="1" x14ac:dyDescent="0.25">
@@ -6504,29 +6402,29 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" ph="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
@@ -6534,13 +6432,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="63.75" ph="1" x14ac:dyDescent="0.25">
@@ -6548,13 +6446,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="51" ph="1" x14ac:dyDescent="0.25">
@@ -6562,21 +6460,21 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="76.5" ph="1" x14ac:dyDescent="0.25">
@@ -6584,13 +6482,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6598,21 +6496,21 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="38.25" ph="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="63.75" ph="1" x14ac:dyDescent="0.25">
@@ -6620,13 +6518,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="89.25" ph="1" x14ac:dyDescent="0.25">
@@ -6634,24 +6532,24 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -6659,13 +6557,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -6696,7 +6594,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6704,7 +6602,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6720,7 +6618,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
@@ -6728,7 +6626,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6742,7 +6640,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -6756,7 +6654,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -6770,7 +6668,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -6784,7 +6682,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -6798,7 +6696,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -6812,7 +6710,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -6826,7 +6724,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -6840,7 +6738,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6854,7 +6752,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -6891,7 +6789,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6899,7 +6797,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6915,7 +6813,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -6923,7 +6821,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6939,7 +6837,7 @@
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6986,7 +6884,7 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6994,13 +6892,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -7008,7 +6906,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7027,13 +6925,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7041,13 +6939,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
@@ -7055,7 +6953,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -7069,7 +6967,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -7083,13 +6981,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -7097,13 +6995,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -7134,7 +7032,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7142,7 +7040,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7158,7 +7056,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7166,7 +7064,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7182,65 +7080,65 @@
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D10" t="s">
         <v>235</v>
-      </c>
-      <c r="D10" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D11" t="s">
         <v>237</v>
-      </c>
-      <c r="D11" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D12" t="s">
         <v>239</v>
-      </c>
-      <c r="D12" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -7248,50 +7146,50 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D18" t="s">
         <v>250</v>
-      </c>
-      <c r="D18" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D19" t="s">
         <v>252</v>
-      </c>
-      <c r="D19" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D20" t="s">
         <v>254</v>
-      </c>
-      <c r="D20" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D21" t="s">
         <v>256</v>
-      </c>
-      <c r="D21" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -7322,7 +7220,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7330,7 +7228,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7346,7 +7244,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7354,7 +7252,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7365,12 +7263,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7378,7 +7276,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -7389,7 +7287,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7397,21 +7295,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D12" t="s">
         <v>183</v>
-      </c>
-      <c r="D12" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7419,18 +7317,18 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>185</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7438,13 +7336,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>187</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7452,13 +7350,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -7505,7 +7403,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7513,7 +7411,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7529,7 +7427,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -7540,7 +7438,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7556,7 +7454,7 @@
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -7569,7 +7467,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7580,18 +7478,18 @@
     </row>
     <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7599,29 +7497,29 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D14" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7629,13 +7527,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
         <v>175</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
@@ -7643,18 +7541,18 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7662,7 +7560,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -7673,7 +7571,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -7684,7 +7582,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -7698,10 +7596,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7717,7 +7615,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7725,7 +7623,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7741,7 +7639,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="216.75" x14ac:dyDescent="0.25">
@@ -7749,7 +7647,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7768,13 +7666,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -7787,64 +7685,64 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D11" t="s">
         <v>231</v>
-      </c>
-      <c r="D11" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -7855,12 +7753,12 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -7882,273 +7780,201 @@
         <v>4</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D23" t="s">
         <v>227</v>
       </c>
-      <c r="D23" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" ht="102" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
       <c r="B34" s="1" t="s">
-        <v>322</v>
+        <v>213</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
-        <v>324</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="102" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>217</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C37" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D37" t="s" ph="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C40" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="102" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D43" t="s" ph="1">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="D38" t="s">
         <v>47</v>
       </c>
-      <c r="C44" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="4:4" ht="19.149999999999999" x14ac:dyDescent="0.25">
-      <c r="D52" ph="1"/>
+    </row>
+    <row r="46" spans="1:4" ht="19.149999999999999" x14ac:dyDescent="0.25">
+      <c r="D46" ph="1"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" ph="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -8186,7 +8012,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8202,12 +8028,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -8215,7 +8041,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -8229,7 +8055,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -8243,7 +8069,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -8257,7 +8083,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -8285,7 +8111,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -8299,7 +8125,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -8310,10 +8136,10 @@
     </row>
     <row r="14" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -8321,7 +8147,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -8335,7 +8161,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
add pics mfa setting win10(ja)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="266" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6D94B2B-9BE0-402F-8317-6060C59D2F97}"/>
+  <xr:revisionPtr revIDLastSave="299" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1206303D-6F12-4615-BFE1-42C9817EA973}"/>
   <bookViews>
-    <workbookView xWindow="3863" yWindow="1508" windowWidth="18225" windowHeight="11872" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5018" yWindow="1260" windowWidth="18225" windowHeight="11873" tabRatio="782" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="331">
   <si>
     <t>header1</t>
   </si>
@@ -2334,50 +2334,12 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>moodle-top.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;h2&gt;&lt;a name="mfa"&gt;&lt;/a&gt;多要素認証(MFA)の設定&lt;/h2&gt; </t>
     <rPh sb="22" eb="27">
       <t>タヨウソニンショウ</t>
     </rPh>
     <rPh sb="33" eb="35">
       <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>下の方にある「広大IDのMFA設定」の説明に従って広大IDの多要素認証（MFA）設定を行ってください。&lt;span class="check"&gt;check-10&lt;/span&gt;</t>
-    <rPh sb="0" eb="1">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="22" eb="23">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="30" eb="35">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="43" eb="44">
-      <t>オコナ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -3011,34 +2973,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>さらに下の方にある「IMCアカウントのMFA設定」の説明に従ってIMCアカウントの多要素認証（MFA）設定を行ってください。&lt;span class="check"&gt;check-9&lt;/span&gt;</t>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="41" eb="46">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="51" eb="53">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="54" eb="55">
-      <t>オコナ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win10ja-search-excel.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -3777,43 +3711,6 @@
   </t>
     <rPh sb="72" eb="73">
       <t>タモ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>広大moodleの「コースツリー」の中の「MFA設定ガイド」をクリックすると、コースのトップページが表示されます。少し下の方にスクロールして表示される「広大IDとIMCアカウントの概要」を、まず読んでください。</t>
-    <rPh sb="0" eb="2">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="50" eb="52">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="57" eb="58">
-      <t>スコ</t>
-    </rPh>
-    <rPh sb="59" eb="60">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="61" eb="62">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="76" eb="78">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="90" eb="92">
-      <t>ガイヨウ</t>
-    </rPh>
-    <rPh sb="97" eb="98">
-      <t>ヨ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5290,6 +5187,185 @@
     <rPh sb="70" eb="71">
       <t>ヨ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>さらに下の方にある「IMCアカウントのMFA設定」をクリックしてIMCアカウントのMFA設定教材を表示しましょう。</t>
+    <rPh sb="3" eb="4">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広大moodleの「コースツリー」の中の「MFA設定ガイド」をクリックすると、コースのトップページが表示されます。まず「コメントシート」欄に表示される説明を読みましょう。</t>
+    <rPh sb="0" eb="2">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="68" eb="69">
+      <t>ラン</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="75" eb="77">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="78" eb="79">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>moodle-mfa-hirodai,png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>さらに下の方にある「広大IDのMFA設定」をクリックしてIMCアカウントのMFA設定教材を表示しましょう。</t>
+    <rPh sb="3" eb="4">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>教材の下の方にある「広大IDのMFA利用設定実習」をクリックして、説明に従ってIMCアカウントの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check-10&lt;/span&gt;</t>
+    <rPh sb="0" eb="2">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="48" eb="53">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="74" eb="77">
+      <t>カクコウモク</t>
+    </rPh>
+    <rPh sb="78" eb="80">
+      <t>シリョウ</t>
+    </rPh>
+    <rPh sb="81" eb="82">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>教材の下の方にある「IMCアカウントのMFA利用設定実習」をクリックして、説明に従ってIMCアカウントの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check-9&lt;/span&gt;</t>
+    <rPh sb="0" eb="2">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="52" eb="57">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="65" eb="66">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="78" eb="81">
+      <t>カクコウモク</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>シリョウ</t>
+    </rPh>
+    <rPh sb="85" eb="86">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>moodle-dashboard-ja.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>moodle-mfa-imc,svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>moodle-mfa-top.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>moodle-mfaimc-below.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>moodle-mfahirodai-below.svg</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5735,7 +5811,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5773,7 +5849,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -5810,7 +5886,7 @@
         <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5834,17 +5910,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5852,12 +5928,12 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D9" t="s">
         <v>173</v>
@@ -5865,17 +5941,17 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="165.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -5917,7 +5993,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5925,7 +6001,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5941,12 +6017,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5956,7 +6032,7 @@
     </row>
     <row r="9" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D9" t="s">
         <v>87</v>
@@ -5964,7 +6040,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -5972,7 +6048,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -5983,54 +6059,54 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D13" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="D14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6046,7 +6122,7 @@
     </row>
     <row r="24" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -6287,7 +6363,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6311,7 +6387,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
@@ -6319,7 +6395,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6330,7 +6406,7 @@
     </row>
     <row r="7" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -6338,7 +6414,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
@@ -6594,7 +6670,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6626,7 +6702,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6654,7 +6730,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -6738,7 +6814,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6752,7 +6828,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -6821,7 +6897,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6837,7 +6913,7 @@
     </row>
     <row r="8" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -6906,7 +6982,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6925,7 +7001,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -6939,7 +7015,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -7056,7 +7132,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7064,7 +7140,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7085,42 +7161,42 @@
     </row>
     <row r="9" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D9" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D10" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D11" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D13" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -7130,12 +7206,12 @@
     </row>
     <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D16" t="s">
         <v>89</v>
@@ -7146,42 +7222,42 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D17" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D18" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D19" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D20" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D21" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7189,7 +7265,7 @@
         <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -7228,7 +7304,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7244,7 +7320,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7252,7 +7328,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7263,12 +7339,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7287,7 +7363,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7295,21 +7371,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7317,18 +7393,18 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7336,13 +7412,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7350,13 +7426,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -7384,10 +7460,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475A5B02-452F-483B-8907-D83726E9A70E}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="90" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7403,7 +7479,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7411,7 +7487,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7427,7 +7503,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -7438,7 +7514,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7454,7 +7530,7 @@
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -7467,7 +7543,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7478,18 +7554,18 @@
     </row>
     <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7497,26 +7573,26 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D14" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D15" t="s">
         <v>173</v>
@@ -7541,18 +7617,18 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>176</v>
+        <v>326</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7560,21 +7636,21 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>265</v>
+        <v>321</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
+      <c r="D19" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
+        <v>320</v>
+      </c>
+      <c r="D20" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7582,10 +7658,35 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>178</v>
+        <v>325</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D22" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -7598,8 +7699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7615,7 +7716,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7623,7 +7724,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7639,7 +7740,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="216.75" x14ac:dyDescent="0.25">
@@ -7647,7 +7748,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7666,13 +7767,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -7685,64 +7786,64 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D11" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D14" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.25">
@@ -7753,12 +7854,12 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -7780,18 +7881,18 @@
         <v>4</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D22" t="s">
         <v>175</v>
@@ -7799,10 +7900,10 @@
     </row>
     <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D23" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -7810,13 +7911,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -7826,7 +7927,7 @@
     </row>
     <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -7834,24 +7935,24 @@
     </row>
     <row r="27" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -7859,7 +7960,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -7873,7 +7974,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -7884,7 +7985,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -7898,12 +7999,12 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7911,7 +8012,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -7950,7 +8051,7 @@
     </row>
     <row r="37" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D37" t="s" ph="1">
         <v>60</v>
@@ -7973,7 +8074,7 @@
     <row r="46" spans="1:4" ht="19.149999999999999" x14ac:dyDescent="0.25">
       <c r="D46" ph="1"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:4" ht="19.149999999999999" x14ac:dyDescent="0.25">
       <c r="D51" ph="1"/>
     </row>
   </sheetData>
@@ -8012,7 +8113,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8028,12 +8129,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -8055,7 +8156,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
add pics setup MFA win10en
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="304" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65EA2C1C-6794-4F04-A5C9-072E94B45EC7}"/>
+  <xr:revisionPtr revIDLastSave="307" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF90C1A5-EB37-4667-821D-BCBF4F57B3E8}"/>
   <bookViews>
-    <workbookView xWindow="5018" yWindow="1260" windowWidth="18225" windowHeight="11873" tabRatio="782" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="772" yWindow="1350" windowWidth="18225" windowHeight="11873" tabRatio="782" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -5212,31 +5212,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>さらに下の方にある「広大IDのMFA設定」をクリックしてIMCアカウントのMFA設定教材を表示しましょう。</t>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="42" eb="44">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>教材の下の方にある「IMCアカウントのMFA利用設定実習」をクリックして、説明に従ってIMCアカウントの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check-9&lt;/span&gt;</t>
     <rPh sb="0" eb="2">
       <t>キョウザイ</t>
@@ -5297,10 +5272,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>moodle-mfa-hirodai.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>広大moodleの「コースツリー」の中の「MFA設定ガイド」をクリックすると、コースのトップページが表示されます。まず「コメントシート」欄に表示される説明を読んでください。</t>
     <rPh sb="0" eb="2">
       <t>ヒロダイ</t>
@@ -5329,7 +5300,39 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>教材の下の方にある「広大IDのMFA利用設定実習」をクリックして、説明に従ってIMCアカウントの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check-10&lt;/span&gt;
+    <t>moodle-mfa-hirodai.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>さらに下の方にある「広大IDのMFA設定」をクリックして広大IDのMFA設定教材を表示しましょう。</t>
+    <rPh sb="3" eb="4">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>教材の下の方にある「広大IDのMFA利用設定実習」をクリックして、説明に従って広大IDの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check-10&lt;/span&gt;
 ※ 学外から設定する場合は第６章に説明のある「VPN」を使います。もしVPNの使用が難しい場合は、残りの設定はあとで学内ネットワークに接続してから行いましょう。</t>
     <rPh sb="0" eb="2">
       <t>キョウザイ</t>
@@ -5346,58 +5349,61 @@
     <rPh sb="36" eb="37">
       <t>シタガ</t>
     </rPh>
-    <rPh sb="48" eb="53">
+    <rPh sb="39" eb="41">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="44" eb="49">
       <t>タヨウソニンショウ</t>
     </rPh>
-    <rPh sb="58" eb="60">
+    <rPh sb="54" eb="56">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="61" eb="62">
+    <rPh sb="57" eb="58">
       <t>スス</t>
     </rPh>
-    <rPh sb="68" eb="70">
+    <rPh sb="64" eb="66">
       <t>ショウサイ</t>
     </rPh>
-    <rPh sb="74" eb="77">
+    <rPh sb="70" eb="73">
       <t>カクコウモク</t>
     </rPh>
-    <rPh sb="78" eb="80">
+    <rPh sb="74" eb="76">
       <t>シリョウ</t>
     </rPh>
-    <rPh sb="81" eb="82">
+    <rPh sb="77" eb="78">
       <t>ミ</t>
     </rPh>
+    <rPh sb="122" eb="124">
+      <t>ガクガイ</t>
+    </rPh>
     <rPh sb="126" eb="128">
-      <t>ガクガイ</t>
+      <t>セッテイ</t>
     </rPh>
     <rPh sb="130" eb="132">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="159" eb="161">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="162" eb="163">
+      <t>ムズカ</t>
+    </rPh>
+    <rPh sb="165" eb="167">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="169" eb="170">
+      <t>ノコ</t>
+    </rPh>
+    <rPh sb="172" eb="174">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="134" eb="136">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="163" eb="165">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="166" eb="167">
-      <t>ムズカ</t>
-    </rPh>
-    <rPh sb="169" eb="171">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="173" eb="174">
-      <t>ノコ</t>
-    </rPh>
-    <rPh sb="176" eb="178">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="182" eb="184">
+    <rPh sb="178" eb="180">
       <t>ガクナイ</t>
     </rPh>
-    <rPh sb="191" eb="193">
+    <rPh sb="187" eb="189">
       <t>セツゾク</t>
     </rPh>
-    <rPh sb="197" eb="198">
+    <rPh sb="193" eb="194">
       <t>オコナ</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -7314,7 +7320,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7657,7 +7663,7 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -7670,13 +7676,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -7684,7 +7690,7 @@
         <v>320</v>
       </c>
       <c r="D20" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7692,18 +7698,18 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="D22" t="s">
         <v>328</v>
@@ -7720,7 +7726,7 @@
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change usage Bb9 win11(ja)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/kishiba_hiroshima-u_ac_jp/Documents/Documents/fresta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="309" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F16965D-7E9C-4724-ABA2-933AE406A1E3}"/>
+  <xr:revisionPtr revIDLastSave="314" documentId="13_ncr:1_{BE7D8B25-C639-442F-BD93-EA6719E39471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B10B987C-8E81-4094-9346-D468ABFAC619}"/>
   <bookViews>
-    <workbookView xWindow="5452" yWindow="1155" windowWidth="18226" windowHeight="11873" tabRatio="782" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="405" yWindow="-15450" windowWidth="17520" windowHeight="11595" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="332">
   <si>
     <t>header1</t>
   </si>
@@ -2871,10 +2871,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">&lt;h2&gt;&lt;a name="omake"&gt;&lt;/a&gt;おまけ&lt;/h2&gt; </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">ここから先は補足情報であり、この実習で設定する必要はありません。後日必要に応じて行ってください。
  </t>
     <rPh sb="4" eb="5">
@@ -4765,10 +4761,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>mymomiji-intro.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win10-6-11a.svg</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -4833,57 +4825,6 @@
     </rPh>
     <rPh sb="79" eb="80">
       <t>オコナ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>広島大学の学生用ポータルサイト「もみじ」を確認してから、オンライン学習支援システムの広大moodleにログインして広島大学で必要な多要素認証（MFA）の設定をしましょう。
- &lt;ul&gt;
-&lt;li&gt;&lt;a href="#momiji"&gt;もみじ（広大学生用ポータルサイト）&lt;/a&gt;
-&lt;/li&gt;
-&lt;li&gt;&lt;a href="#moodle"&gt;広大moodleにログインする&lt;/a&gt;
-&lt;/li&gt;
-&lt;li&gt;&lt;a href="#mfa"&gt;多要素認証(MFA)の設定&lt;/a&gt;
-&lt;/li&gt;
- &lt;/ul&gt;</t>
-    <rPh sb="0" eb="4">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="5" eb="8">
-      <t>ガクセイヨウ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="42" eb="44">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="57" eb="61">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="62" eb="64">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="65" eb="70">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="76" eb="78">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="118" eb="120">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="120" eb="123">
-      <t>ガクセイヨウ</t>
-    </rPh>
-    <rPh sb="164" eb="166">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="209" eb="214">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="220" eb="222">
-      <t>セッテイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5017,6 +4958,384 @@
     </rPh>
     <rPh sb="5" eb="6">
       <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>もみじトップページの右側にある「Webメール」バナーをクリックしましょう。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>momiji-webmail.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「大学教育入門」の詳細画面の中に「Bb9へ」というリンクがあるはずです。
+これをクリックするとBb9の「大学教育入門」コースに直接アクセスできます。
+  </t>
+    <rPh sb="1" eb="7">
+      <t>ダイガクキョウイクニュウモン</t>
+    </rPh>
+    <rPh sb="9" eb="13">
+      <t>ショウサイガメン</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="52" eb="58">
+      <t>ダイガクキョウイクニュウモン</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>チョクセツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Myもみじのトップページに表示されている時間割の中に「大学教育入門」のリンクがあるはずです。
+これをクリックして「大学教育入門」の詳細画面に移動します。
+  </t>
+    <rPh sb="13" eb="15">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="20" eb="23">
+      <t>ジカンワリ</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="27" eb="33">
+      <t>ダイガクキョウイクニュウモン</t>
+    </rPh>
+    <rPh sb="57" eb="63">
+      <t>ダイガクキョウイクニュウモン</t>
+    </rPh>
+    <rPh sb="65" eb="69">
+      <t>ショウサイガメン</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>イドウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+各システムの閲覧が済んだら、できるだけ「サインアウト」「ログアウト」するようにしましょう。多くの場合、画面右上にあるアイコンからログアウトできます。
+※ 図は「Myもみじ」でのログアウト方法の例
+  </t>
+    <rPh sb="1" eb="2">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>エツラン</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ス</t>
+    </rPh>
+    <rPh sb="78" eb="79">
+      <t>ズ</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="97" eb="98">
+      <t>レイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check-13&lt;/span&gt;
+これを「Myもみじのトップページ」と呼ぶことにしましょう。
+履修登録をしたり、成績を確認することができます。
+また「掲示」では、授業や学部からの連絡が表示されます。
+このまま引き続いて、次の「Bb9」の使い方に進みましょう。
+  </t>
+    <rPh sb="70" eb="71">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>さらに下の方にある「IMCアカウントのMFA設定」をクリックしてIMCアカウントのMFA設定教材を表示しましょう。</t>
+    <rPh sb="3" eb="4">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>教材の下の方にある「IMCアカウントのMFA利用設定実習」をクリックして、説明に従ってIMCアカウントの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check-9&lt;/span&gt;</t>
+    <rPh sb="0" eb="2">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="52" eb="57">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="65" eb="66">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="78" eb="81">
+      <t>カクコウモク</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>シリョウ</t>
+    </rPh>
+    <rPh sb="85" eb="86">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>moodle-dashboard-ja.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>moodle-mfa-top.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>moodle-mfaimc-below.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>moodle-mfahirodai-below.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>moodle-mfa-imc.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広大moodleの「コースツリー」の中の「MFA設定ガイド」をクリックすると、コースのトップページが表示されます。まず「コメントシート」欄に表示される説明を読んでください。</t>
+    <rPh sb="0" eb="2">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="50" eb="52">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="68" eb="69">
+      <t>ラン</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="75" eb="77">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="78" eb="79">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>moodle-mfa-hirodai.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>さらに下の方にある「広大IDのMFA設定」をクリックして広大IDのMFA設定教材を表示しましょう。</t>
+    <rPh sb="3" eb="4">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>教材の下の方にある「広大IDのMFA利用設定実習」をクリックして、説明に従って広大IDの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check-10&lt;/span&gt;
+※ 学外から設定する場合は第６章に説明のある「VPN」を使います。もしVPNの使用が難しい場合は、残りの設定はあとで学内ネットワークに接続してから行いましょう。</t>
+    <rPh sb="0" eb="2">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="44" eb="49">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="57" eb="58">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="70" eb="73">
+      <t>カクコウモク</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>シリョウ</t>
+    </rPh>
+    <rPh sb="77" eb="78">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="122" eb="124">
+      <t>ガクガイ</t>
+    </rPh>
+    <rPh sb="126" eb="128">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="130" eb="132">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="159" eb="161">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="162" eb="163">
+      <t>ムズカ</t>
+    </rPh>
+    <rPh sb="165" eb="167">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="169" eb="170">
+      <t>ノコ</t>
+    </rPh>
+    <rPh sb="172" eb="174">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="178" eb="180">
+      <t>ガクナイ</t>
+    </rPh>
+    <rPh sb="187" eb="189">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="193" eb="194">
+      <t>オコナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>電子メールやクラウドストレージが使えるOffice365、オンライン履修登録などをおこなう「Myもみじ」、オンライン学習支援システムのBb9など、大学で提供されているネットワークサービスを使えるようにしましょう。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>もみじトップページの「Bb9/moodle」バナー、または次のリンクから広島大学オンライン学習支援システム（広大moodle）にアクセスしてください。
+&lt;a href="https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/"&gt;https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/&lt;/a&gt;
+「広大IDでログイン」をクリックしてログインしましょう。</t>
+    <rPh sb="29" eb="30">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="36" eb="40">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="45" eb="49">
+      <t>ガクシュウシエン</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="195" eb="197">
+      <t>ヒロダイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「Moodle」は、オープンソースで提供されているオンライン学習支援システムです。広島大学ではMoodleを広大IDでログインして利用できるようにしており、これを「広大moodle」と呼んでいます。
+ここに授業で使う資料が掲載されたり、テストを受けたり、課題を提出したりすることがあります。
+</t>
+    <rPh sb="18" eb="20">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>ガクシュウ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>シエン</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="65" eb="67">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="92" eb="93">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>mymomiji-intro.svg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h2&gt;&lt;a name="appendix"&gt;&lt;/a&gt;補足情報&lt;/h2&gt; </t>
+    <rPh sb="27" eb="29">
+      <t>ホソク</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ジョウホウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5031,7 +5350,7 @@
 &lt;/li&gt;
 &lt;li&gt;&lt;a href="#bb9"&gt;Bb9 (学習支援システム )&lt;/a&gt;
 &lt;/li&gt;
-&lt;li&gt;&lt;a href="#omake"&gt;おまけ&lt;/a&gt;
+&lt;li&gt;&lt;a href="#appendix"&gt;補足情報&lt;/a&gt;
 &lt;/li&gt;
 &lt;ul&gt; &lt;/ul&gt;
 &lt;/ul&gt;
@@ -5069,342 +5388,59 @@
     <rPh sb="193" eb="194">
       <t>カマ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>もみじトップページの右側にある「Webメール」バナーをクリックしましょう。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>momiji-webmail.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">「大学教育入門」の詳細画面の中に「Bb9へ」というリンクがあるはずです。
-これをクリックするとBb9の「大学教育入門」コースに直接アクセスできます。
-  </t>
-    <rPh sb="1" eb="7">
-      <t>ダイガクキョウイクニュウモン</t>
-    </rPh>
-    <rPh sb="9" eb="13">
-      <t>ショウサイガメン</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="52" eb="58">
-      <t>ダイガクキョウイクニュウモン</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>チョクセツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Myもみじのトップページに表示されている時間割の中に「大学教育入門」のリンクがあるはずです。
-これをクリックして「大学教育入門」の詳細画面に移動します。
-  </t>
-    <rPh sb="13" eb="15">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="20" eb="23">
-      <t>ジカンワリ</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="27" eb="33">
-      <t>ダイガクキョウイクニュウモン</t>
-    </rPh>
-    <rPh sb="57" eb="63">
-      <t>ダイガクキョウイクニュウモン</t>
-    </rPh>
-    <rPh sb="65" eb="69">
-      <t>ショウサイガメン</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>イドウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">
-各システムの閲覧が済んだら、できるだけ「サインアウト」「ログアウト」するようにしましょう。多くの場合、画面右上にあるアイコンからログアウトできます。
-※ 図は「Myもみじ」でのログアウト方法の例
-  </t>
-    <rPh sb="1" eb="2">
-      <t>カク</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>エツラン</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>ス</t>
-    </rPh>
-    <rPh sb="78" eb="79">
-      <t>ズ</t>
-    </rPh>
-    <rPh sb="94" eb="96">
-      <t>ホウホウ</t>
-    </rPh>
-    <rPh sb="97" eb="98">
-      <t>レイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check-13&lt;/span&gt;
-これを「Myもみじのトップページ」と呼ぶことにしましょう。
-履修登録をしたり、成績を確認することができます。
-また「掲示」では、授業や学部からの連絡が表示されます。
-このまま引き続いて、次の「Bb9」の使い方に進みましょう。
-  </t>
-    <rPh sb="70" eb="71">
-      <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>さらに下の方にある「IMCアカウントのMFA設定」をクリックしてIMCアカウントのMFA設定教材を表示しましょう。</t>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
+    <rPh sb="425" eb="429">
+      <t>ホソクジョウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>広島大学の学生用ポータルサイト「もみじ」を確認してから、オンライン学習支援システムの広大moodleにログインして広島大学で必要な多要素認証（MFA）の設定をしましょう。
+ &lt;ul&gt;
+&lt;li&gt;&lt;a href="#momiji"&gt;もみじ（広大学生用ポータルサイト）&lt;/a&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;a href="#moodle"&gt;広大moodle（オンライン学習支援システム）にログインする&lt;/a&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;a href="#mfa"&gt;多要素認証(MFA)の設定&lt;/a&gt;
+&lt;/li&gt;
+ &lt;/ul&gt;</t>
+    <rPh sb="0" eb="4">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="5" eb="8">
+      <t>ガクセイヨウ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="57" eb="61">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="65" eb="70">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="44" eb="46">
+    <rPh sb="118" eb="120">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="120" eb="123">
+      <t>ガクセイヨウ</t>
+    </rPh>
+    <rPh sb="164" eb="166">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="224" eb="229">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="235" eb="237">
       <t>セッテイ</t>
-    </rPh>
-    <rPh sb="46" eb="48">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>教材の下の方にある「IMCアカウントのMFA利用設定実習」をクリックして、説明に従ってIMCアカウントの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check-9&lt;/span&gt;</t>
-    <rPh sb="0" eb="2">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="40" eb="41">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="52" eb="57">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="62" eb="64">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="65" eb="66">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="78" eb="81">
-      <t>カクコウモク</t>
-    </rPh>
-    <rPh sb="82" eb="84">
-      <t>シリョウ</t>
-    </rPh>
-    <rPh sb="85" eb="86">
-      <t>ミ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-dashboard-ja.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-mfa-top.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-mfaimc-below.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-mfahirodai-below.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-mfa-imc.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>広大moodleの「コースツリー」の中の「MFA設定ガイド」をクリックすると、コースのトップページが表示されます。まず「コメントシート」欄に表示される説明を読んでください。</t>
-    <rPh sb="0" eb="2">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="50" eb="52">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="68" eb="69">
-      <t>ラン</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="75" eb="77">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="78" eb="79">
-      <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-mfa-hirodai.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>さらに下の方にある「広大IDのMFA設定」をクリックして広大IDのMFA設定教材を表示しましょう。</t>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>教材の下の方にある「広大IDのMFA利用設定実習」をクリックして、説明に従って広大IDの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check-10&lt;/span&gt;
-※ 学外から設定する場合は第６章に説明のある「VPN」を使います。もしVPNの使用が難しい場合は、残りの設定はあとで学内ネットワークに接続してから行いましょう。</t>
-    <rPh sb="0" eb="2">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="44" eb="49">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="54" eb="56">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="57" eb="58">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="70" eb="73">
-      <t>カクコウモク</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>シリョウ</t>
-    </rPh>
-    <rPh sb="77" eb="78">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="122" eb="124">
-      <t>ガクガイ</t>
-    </rPh>
-    <rPh sb="126" eb="128">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="130" eb="132">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="159" eb="161">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="162" eb="163">
-      <t>ムズカ</t>
-    </rPh>
-    <rPh sb="165" eb="167">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="169" eb="170">
-      <t>ノコ</t>
-    </rPh>
-    <rPh sb="172" eb="174">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="178" eb="180">
-      <t>ガクナイ</t>
-    </rPh>
-    <rPh sb="187" eb="189">
-      <t>セツゾク</t>
-    </rPh>
-    <rPh sb="193" eb="194">
-      <t>オコナ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>電子メールやクラウドストレージが使えるOffice365、オンライン履修登録などをおこなう「Myもみじ」、オンライン学習支援システムのBb9など、大学で提供されているネットワークサービスを使えるようにしましょう。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>もみじトップページの「Bb9/moodle」バナー、または次のリンクから広島大学オンライン学習支援システム（広大moodle）にアクセスしてください。
-&lt;a href="https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/"&gt;https://moodle.vle.hiroshima-u.ac.jp/local/hulogin/&lt;/a&gt;
-「広大IDでログイン」をクリックしてログインしましょう。</t>
-    <rPh sb="29" eb="30">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="36" eb="40">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="45" eb="49">
-      <t>ガクシュウシエン</t>
-    </rPh>
-    <rPh sb="54" eb="56">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="195" eb="197">
-      <t>ヒロダイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5851,7 +5887,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5909,7 +5945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02489F37-694A-4583-9CE4-9D6A1DDB1F5F}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -5968,12 +6004,12 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D9" t="s">
         <v>173</v>
@@ -5981,7 +6017,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -6033,7 +6069,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6041,7 +6077,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -6057,12 +6093,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -6072,7 +6108,7 @@
     </row>
     <row r="9" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D9" t="s">
         <v>87</v>
@@ -6080,7 +6116,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -6088,7 +6124,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -6099,20 +6135,20 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D13" t="s">
         <v>227</v>
-      </c>
-      <c r="D13" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D14" t="s">
         <v>190</v>
@@ -6128,25 +6164,25 @@
     </row>
     <row r="16" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -6162,7 +6198,7 @@
     </row>
     <row r="24" spans="2:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -6403,7 +6439,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.25">
@@ -6435,7 +6471,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6446,7 +6482,7 @@
     </row>
     <row r="7" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" ph="1" x14ac:dyDescent="0.25">
@@ -6454,7 +6490,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
@@ -6710,7 +6746,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6742,7 +6778,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6770,7 +6806,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -6854,7 +6890,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -6868,7 +6904,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -6937,7 +6973,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7022,7 +7058,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7041,7 +7077,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -7055,7 +7091,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -7180,7 +7216,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7201,42 +7237,42 @@
     </row>
     <row r="9" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D10" t="s">
         <v>231</v>
-      </c>
-      <c r="D10" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D11" t="s">
         <v>233</v>
-      </c>
-      <c r="D11" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D12" t="s">
         <v>235</v>
-      </c>
-      <c r="D12" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -7246,12 +7282,12 @@
     </row>
     <row r="15" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D16" t="s">
         <v>89</v>
@@ -7262,42 +7298,42 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D18" t="s">
         <v>246</v>
-      </c>
-      <c r="D18" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D19" t="s">
         <v>248</v>
-      </c>
-      <c r="D19" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D20" t="s">
         <v>250</v>
-      </c>
-      <c r="D20" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D21" t="s">
         <v>252</v>
-      </c>
-      <c r="D21" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7305,7 +7341,7 @@
         <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -7319,8 +7355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DD8924-3FAE-44AB-A508-09E9136389D4}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7360,7 +7396,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
@@ -7379,12 +7415,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="127.5" x14ac:dyDescent="0.25">
@@ -7403,7 +7439,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -7411,13 +7447,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
@@ -7444,7 +7480,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -7500,10 +7536,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475A5B02-452F-483B-8907-D83726E9A70E}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7519,7 +7555,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7527,7 +7563,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7543,7 +7579,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -7554,7 +7590,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>301</v>
+        <v>331</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7583,7 +7619,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -7594,7 +7630,7 @@
     </row>
     <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -7605,128 +7641,139 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D15" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="D14" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="1:4" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
+    <row r="18" spans="1:4" ht="191.25" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D21" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+    <row r="22" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
         <v>318</v>
       </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D23" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="51" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
         <v>319</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="D22" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -7739,8 +7786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -7756,7 +7803,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -7788,7 +7835,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>311</v>
+        <v>330</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7807,7 +7854,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -7826,26 +7873,26 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D11" t="s">
         <v>227</v>
-      </c>
-      <c r="D11" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D12" t="s">
         <v>190</v>
@@ -7853,7 +7900,7 @@
     </row>
     <row r="13" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D13" t="s">
         <v>192</v>
@@ -7861,15 +7908,15 @@
     </row>
     <row r="14" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D15" t="s">
         <v>193</v>
@@ -7877,7 +7924,7 @@
     </row>
     <row r="16" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -7899,7 +7946,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -7921,7 +7968,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -7932,7 +7979,7 @@
     </row>
     <row r="22" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D22" t="s">
         <v>175</v>
@@ -7940,10 +7987,10 @@
     </row>
     <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D23" t="s">
         <v>223</v>
-      </c>
-      <c r="D23" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -7951,13 +7998,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -7967,7 +8014,7 @@
     </row>
     <row r="26" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -7975,24 +8022,24 @@
     </row>
     <row r="27" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="51" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>295</v>
+        <v>328</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
@@ -8000,7 +8047,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -8014,7 +8061,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C30" t="s">
         <v>4</v>
@@ -8025,7 +8072,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -8039,12 +8086,12 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>210</v>
+        <v>329</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
@@ -8052,7 +8099,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
@@ -8091,7 +8138,7 @@
     </row>
     <row r="37" spans="1:4" ht="89.25" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D37" t="s" ph="1">
         <v>60</v>
@@ -8128,8 +8175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -8174,7 +8221,7 @@
     </row>
     <row r="6" spans="1:4" ht="38.25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="63.75" x14ac:dyDescent="0.25">
@@ -8196,7 +8243,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
win10ja: fix check number
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20407"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE4BE6A-EF2B-4667-B1AE-CFBE252566C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7FC5A7-F7D2-49B9-9B25-9348A2092664}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="21600" windowHeight="11592" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="-15096" windowWidth="21600" windowHeight="11592" tabRatio="782" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="353">
   <si>
     <t>header1</t>
   </si>
@@ -5197,373 +5197,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">「詳細情報」という名前のウィンドウが開きます。中にPCに関する情報がたくさん表示されています。
-「Windowsの仕様」をみると「エディション」のところに「Windows 10 Pro」とありますね。これがOSの種類です。「バージョン」のところには詳細なバージョン番号（いつの時点のOSか）が書かれています。&lt;span class="check"&gt;check 1
-&lt;/span&gt;
-その上の方に「デバイスの仕様」がありますね。ここの「システムの種類」を見ると、OSのビット数がわかります。&amp;quot;64ビットオペレーティングシステム&amp;quot; とあります。この場合は64ビットですね。二進法で64桁のデータを一度に処理できるOSであるということを示しています。&lt;span class="check"&gt;check 2&lt;/span&gt;
-その上に「実装RAM」と書かれたところがあります。ここを見ると、主記憶装置（メインメモリ）の容量がわかります。この場合は8GB（ギガバイト）ですね。この容量が大きいほど、大量のデータを一括して扱えたり、多くのプログラムを同時に動作させたりすることがスムーズにできるようになります。
-  </t>
-    <rPh sb="1" eb="3">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="282" eb="284">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="425" eb="427">
-      <t>バアイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ウィルス対策ソフトのDefenderを含めて、Windows基本システムは定期的に自動更新されます。
-このウィンドウの上の方で更新状況が確認できます。&lt;span class="check"&gt;check 3&lt;/span&gt;&lt;span class="check"&gt;check 5&lt;/span&gt;
-さらに、Officeも自動更新するように設定しましょう。「詳細オプション」をクリックしてください。
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Defenderでは、ウイルスやスパイウェアその他の悪意を持つプログラム全般を「脅威」とし、それらを判別するルールを保存したファイルを「脅威の定義」と呼んでいます。
-「ウイルスと脅威の防止の更新」の下に、前回いつ「脅威の定義」が更新されたかが書かれています。&lt;span class="check"&gt;check 4&lt;/span&gt;&lt;span class="check"&gt;check 5&lt;/span&gt;
-&lt;p class="spl"&gt;※ここで「他のプログラム（ウィルスバスター、マカフィーリブセーフなど）が有効になっている」という旨の表示がされた場合、ウィルス対策はその表示されたプログラムが行っています。その場合はこの下の項目は飛ばして、別途そのプログラムの「利用期限」と「更新方法」「フルスキャンの実施方法」を確認してください。とくに「利用期限」が切れてウィルス対策に穴ができることがないよう注意してください。あとで Defender の利用に戻すこともできます。&lt;/p&gt;
-脅威の定義を新しくするには「ウイルスと脅威の防止の更新」をクリックします。
-  </t>
-    <rPh sb="248" eb="250">
-      <t>ユウコウ</t>
-    </rPh>
-    <rPh sb="260" eb="261">
-      <t>ムネ</t>
-    </rPh>
-    <rPh sb="275" eb="277">
-      <t>タイサク</t>
-    </rPh>
-    <rPh sb="280" eb="282">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="291" eb="292">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="300" eb="302">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="305" eb="306">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="307" eb="309">
-      <t>コウモク</t>
-    </rPh>
-    <rPh sb="310" eb="311">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="315" eb="317">
-      <t>ベット</t>
-    </rPh>
-    <rPh sb="326" eb="328">
-      <t>リヨウ</t>
-    </rPh>
-    <rPh sb="328" eb="330">
-      <t>キゲン</t>
-    </rPh>
-    <rPh sb="333" eb="335">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="335" eb="337">
-      <t>ホウホウ</t>
-    </rPh>
-    <rPh sb="346" eb="348">
-      <t>ジッシ</t>
-    </rPh>
-    <rPh sb="348" eb="350">
-      <t>ホウホウ</t>
-    </rPh>
-    <rPh sb="352" eb="354">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="365" eb="367">
-      <t>リヨウ</t>
-    </rPh>
-    <rPh sb="367" eb="369">
-      <t>キゲン</t>
-    </rPh>
-    <rPh sb="371" eb="372">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="378" eb="380">
-      <t>タイサク</t>
-    </rPh>
-    <rPh sb="381" eb="382">
-      <t>アナ</t>
-    </rPh>
-    <rPh sb="393" eb="395">
-      <t>チュウイ</t>
-    </rPh>
-    <rPh sb="416" eb="418">
-      <t>リヨウ</t>
-    </rPh>
-    <rPh sb="419" eb="420">
-      <t>モド</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">三種類の高度なスキャンがありますね。「フルスキャン」を選んで下の「今すぐスキャン」ボタンを押すと、フルスキャンが実施されます。&lt;span class="check"&gt;check 6&lt;/span&gt;
-フルスキャンの実施には数時間（新品のPCでも３０分程度）かかります。時間の余裕のあるときにできるだけ早く実施してください。
-右上の×をクリックして、ウィンドウを閉じましょう。
-  </t>
-    <rPh sb="114" eb="116">
-      <t>シンピン</t>
-    </rPh>
-    <rPh sb="123" eb="124">
-      <t>フン</t>
-    </rPh>
-    <rPh sb="124" eb="126">
-      <t>テイド</t>
-    </rPh>
-    <rPh sb="133" eb="135">
-      <t>ジカン</t>
-    </rPh>
-    <rPh sb="136" eb="138">
-      <t>ヨユウ</t>
-    </rPh>
-    <rPh sb="161" eb="163">
-      <t>ミギウエ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>「ライセンス契約に同意します」で「同意する」をクリックします。
-&lt;p class="spl"&gt;※本来は「利用許諾契約書を読む」で契約事項を読んでから同意するものです。「ファイル」→「アカウント」→「Excelのバージョン情報」と辿ればいつでも読めるので、時間のある時に読んでおいてください。&lt;/p&gt;
-これでOfficeを使用するための準備が完了しました。&lt;span class="check"&gt;check 12&lt;/span&gt;
-&lt;strong&gt;広島大学のOffice365アカウントは卒業などで学籍を失うと無くなってしまうので、Office365がインストールされたままでも卒業後は使えなくなります。&lt;/strong&gt;
-以上でこの章の作業は終了です。</t>
-    <rPh sb="6" eb="8">
-      <t>ケイヤク</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ドウイ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ドウイ</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>ホンライ</t>
-    </rPh>
-    <rPh sb="52" eb="54">
-      <t>リヨウ</t>
-    </rPh>
-    <rPh sb="54" eb="56">
-      <t>キョダク</t>
-    </rPh>
-    <rPh sb="56" eb="59">
-      <t>ケイヤクショ</t>
-    </rPh>
-    <rPh sb="60" eb="61">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>ケイヤク</t>
-    </rPh>
-    <rPh sb="66" eb="68">
-      <t>ジコウ</t>
-    </rPh>
-    <rPh sb="69" eb="70">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>ドウイ</t>
-    </rPh>
-    <rPh sb="110" eb="112">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="114" eb="115">
-      <t>タド</t>
-    </rPh>
-    <rPh sb="121" eb="122">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="127" eb="129">
-      <t>ジカン</t>
-    </rPh>
-    <rPh sb="132" eb="133">
-      <t>トキ</t>
-    </rPh>
-    <rPh sb="134" eb="135">
-      <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ログインしたら、この画面（ダッシュボード）が出ます。&lt;span class="check"&gt;check 8&lt;/span&gt;
-真ん中に見える「コースツリー」に、あなたがアクセスできるコースが表示されています。これらは、あなたの履修課目に関する授業支援や、広島大学において自習すべき教材などのコースです。（この図は在学生向けの一例で、新入生に表示されるものとは異なります）
-新入生向けに共通で表示されるものを簡単に説明すると：
-&lt;dl&gt;
-&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
-&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届」を提出する必要があります。このコースでは、点検届が提出できます。&lt;strong&gt;このテキストによる設定・点検を済ませたあと、できるだけ早くにこのコースを開いて点検届を提出してください。&lt;/strong&gt;&lt;/dd&gt;
-&lt;dt&gt;MFA設定ガイド&lt;/dt&gt;
-&lt;dd&gt;広島大学ではパスワード窃取によるアカウント乗っ取りの防止策として、広大IDを持つ全ての構成員に対しIMCアカウントおよび広大IDの多要素認証（MFA）設定を義務付けています。この「MFA設定ガイド」で、広島大学でMFA設定を行うための手順を説明しています&lt;/dd&gt; &lt;/dl&gt;
-</t>
-    <rPh sb="65" eb="66">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="111" eb="113">
-      <t>リシュウ</t>
-    </rPh>
-    <rPh sb="113" eb="115">
-      <t>カモク</t>
-    </rPh>
-    <rPh sb="116" eb="117">
-      <t>カン</t>
-    </rPh>
-    <rPh sb="119" eb="121">
-      <t>ジュギョウ</t>
-    </rPh>
-    <rPh sb="121" eb="123">
-      <t>シエン</t>
-    </rPh>
-    <rPh sb="125" eb="127">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="127" eb="129">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="133" eb="135">
-      <t>ジシュウ</t>
-    </rPh>
-    <rPh sb="138" eb="140">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="157" eb="158">
-      <t>ム</t>
-    </rPh>
-    <rPh sb="184" eb="187">
-      <t>シンニュウセイ</t>
-    </rPh>
-    <rPh sb="187" eb="188">
-      <t>ム</t>
-    </rPh>
-    <rPh sb="190" eb="192">
-      <t>キョウツウ</t>
-    </rPh>
-    <rPh sb="193" eb="195">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="340" eb="342">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="343" eb="345">
-      <t>テンケン</t>
-    </rPh>
-    <rPh sb="346" eb="347">
-      <t>ス</t>
-    </rPh>
-    <rPh sb="358" eb="359">
-      <t>ハヤ</t>
-    </rPh>
-    <rPh sb="367" eb="368">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="405" eb="407">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="420" eb="424">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="431" eb="433">
-      <t>セッシュ</t>
-    </rPh>
-    <rPh sb="441" eb="442">
-      <t>ノ</t>
-    </rPh>
-    <rPh sb="443" eb="444">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="453" eb="455">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="458" eb="459">
-      <t>モ</t>
-    </rPh>
-    <rPh sb="460" eb="461">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="463" eb="466">
-      <t>コウセイイン</t>
-    </rPh>
-    <rPh sb="467" eb="468">
-      <t>タイ</t>
-    </rPh>
-    <rPh sb="480" eb="482">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="485" eb="490">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="495" eb="497">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="498" eb="501">
-      <t>ギムヅ</t>
-    </rPh>
-    <rPh sb="513" eb="515">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="521" eb="525">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="529" eb="531">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="532" eb="533">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="537" eb="539">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="540" eb="542">
-      <t>セツメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>教材の下の方にある「IMCアカウントのMFA利用設定実習」をクリックして、説明に従ってIMCアカウントの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check 9&lt;/span&gt;</t>
-    <rPh sb="0" eb="2">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="40" eb="41">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="52" eb="57">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="62" eb="64">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="65" eb="66">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="78" eb="81">
-      <t>カクコウモク</t>
-    </rPh>
-    <rPh sb="82" eb="84">
-      <t>シリョウ</t>
-    </rPh>
-    <rPh sb="85" eb="86">
-      <t>ミ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">教材の下の方にある「広大IDのMFA利用設定実習」をクリックして、説明に従って広大IDの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check 10&lt;/span&gt;
 </t>
     <rPh sb="0" eb="2">
@@ -5618,13 +5251,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">この画面になったら「接続」をクリックしてください。
-これで接続の設定が完了しました。
-接続が完了すると「接続済み」と表示されます。&lt;span class="check"&gt;check 14&lt;/span&gt;
-   </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Outlook for Webのページが開き、新着メールを確認することができます。大学からのメール連絡は広大メールに来ますので、常にメールチェックするようにしてください。&lt;span class="check"&gt;check 11&lt;/span&gt;</t>
     <rPh sb="20" eb="21">
       <t>ヒラ</t>
@@ -5649,93 +5275,6 @@
     </rPh>
     <rPh sb="64" eb="65">
       <t>ツネ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>デスクトップにPDFファイルのアイコンが現れたら、ダブルクリックしてその内容を表示します。
-この内容の、「ID」と「回復キー」の両方が途切れずちゃんと読めるようにスマートフォンや携帯電話などで写真を撮っておきます。あるいは、このPDFファイルを外付けのUSBフラッシュメモリにコピーするなどしてもかまいません。
-数日の間に必要になることはないでしょうが4年間の間、あるいは卒業後にPCが故障したりするとこのキーが必要になる場合があります。紛失した場合はこの手順を再度実施してキーを確保してください。&lt;span class="check"&gt;check 7&lt;/span&gt;</t>
-    <rPh sb="20" eb="21">
-      <t>アラワ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="48" eb="50">
-      <t>ナイヨウ</t>
-    </rPh>
-    <rPh sb="58" eb="60">
-      <t>カイフク</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>リョウホウ</t>
-    </rPh>
-    <rPh sb="67" eb="69">
-      <t>トギ</t>
-    </rPh>
-    <rPh sb="75" eb="76">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="89" eb="91">
-      <t>ケイタイ</t>
-    </rPh>
-    <rPh sb="91" eb="93">
-      <t>デンワ</t>
-    </rPh>
-    <rPh sb="96" eb="98">
-      <t>シャシン</t>
-    </rPh>
-    <rPh sb="99" eb="100">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="156" eb="158">
-      <t>スウジツ</t>
-    </rPh>
-    <rPh sb="159" eb="160">
-      <t>アイダ</t>
-    </rPh>
-    <rPh sb="161" eb="163">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="177" eb="179">
-      <t>ネンカン</t>
-    </rPh>
-    <rPh sb="180" eb="181">
-      <t>アイダ</t>
-    </rPh>
-    <rPh sb="186" eb="189">
-      <t>ソツギョウゴ</t>
-    </rPh>
-    <rPh sb="193" eb="195">
-      <t>コショウ</t>
-    </rPh>
-    <rPh sb="206" eb="208">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="211" eb="213">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="219" eb="221">
-      <t>フンシツ</t>
-    </rPh>
-    <rPh sb="223" eb="225">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="228" eb="230">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="231" eb="233">
-      <t>サイド</t>
-    </rPh>
-    <rPh sb="233" eb="235">
-      <t>ジッシ</t>
-    </rPh>
-    <rPh sb="240" eb="242">
-      <t>カクホ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5918,6 +5457,398 @@
     <rPh sb="132" eb="134">
       <t>リョウキン</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">「詳細情報」という名前のウィンドウが開きます。中にPCに関する情報がたくさん表示されています。
+「Windowsの仕様」をみると「エディション」のところに「Windows 10 Pro」とありますね。これがOSの種類です。「バージョン」のところには詳細なバージョン番号（いつの時点のOSか）が書かれています。&lt;span class="check"&gt;check 1
+&lt;/span&gt;
+その上に「実装RAM」と書かれたところがあります。ここを見ると、主記憶装置（メインメモリ）の容量がわかります。この場合は8GB（ギガバイト）ですね。この容量が大きいほど、大量のデータを一括して扱えたり、多くのプログラムを同時に動作させたりすることがスムーズにできるようになります。
+  </t>
+    <rPh sb="1" eb="3">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="248" eb="250">
+      <t>バアイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ウィルス対策ソフトのDefenderを含めて、Windows基本システムは定期的に自動更新されます。
+このウィンドウの上の方で更新状況が確認できます。&lt;span class="check"&gt;check 2&lt;/span&gt;&lt;span class="check"&gt;check 4&lt;/span&gt;
+さらに、Officeも自動更新するように設定しましょう。「詳細オプション」をクリックしてください。
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Defenderでは、ウイルスやスパイウェアその他の悪意を持つプログラム全般を「脅威」とし、それらを判別するルールを保存したファイルを「脅威の定義」と呼んでいます。
+「ウイルスと脅威の防止の更新」の下に、前回いつ「脅威の定義」が更新されたかが書かれています。&lt;span class="check"&gt;check 3&lt;/span&gt;&lt;span class="check"&gt;check 4&lt;/span&gt;
+&lt;p class="spl"&gt;※ここで「他のプログラム（ウィルスバスター、マカフィーリブセーフなど）が有効になっている」という旨の表示がされた場合、ウィルス対策はその表示されたプログラムが行っています。その場合はこの下の項目は飛ばして、別途そのプログラムの「利用期限」と「更新方法」「フルスキャンの実施方法」を確認してください。とくに「利用期限」が切れてウィルス対策に穴ができることがないよう注意してください。あとで Defender の利用に戻すこともできます。&lt;/p&gt;
+脅威の定義を新しくするには「ウイルスと脅威の防止の更新」をクリックします。
+  </t>
+    <rPh sb="248" eb="250">
+      <t>ユウコウ</t>
+    </rPh>
+    <rPh sb="260" eb="261">
+      <t>ムネ</t>
+    </rPh>
+    <rPh sb="275" eb="277">
+      <t>タイサク</t>
+    </rPh>
+    <rPh sb="280" eb="282">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="291" eb="292">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="300" eb="302">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="305" eb="306">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="307" eb="309">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="310" eb="311">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="315" eb="317">
+      <t>ベット</t>
+    </rPh>
+    <rPh sb="326" eb="328">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="328" eb="330">
+      <t>キゲン</t>
+    </rPh>
+    <rPh sb="333" eb="335">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="335" eb="337">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="346" eb="348">
+      <t>ジッシ</t>
+    </rPh>
+    <rPh sb="348" eb="350">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="352" eb="354">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="365" eb="367">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="367" eb="369">
+      <t>キゲン</t>
+    </rPh>
+    <rPh sb="371" eb="372">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="378" eb="380">
+      <t>タイサク</t>
+    </rPh>
+    <rPh sb="381" eb="382">
+      <t>アナ</t>
+    </rPh>
+    <rPh sb="393" eb="395">
+      <t>チュウイ</t>
+    </rPh>
+    <rPh sb="416" eb="418">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="419" eb="420">
+      <t>モド</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">三種類の高度なスキャンがありますね。「フルスキャン」を選んで下の「今すぐスキャン」ボタンを押すと、フルスキャンが実施されます。&lt;span class="check"&gt;check 5&lt;/span&gt;
+フルスキャンの実施には数時間（新品のPCでも３０分程度）かかります。時間の余裕のあるときにできるだけ早く実施してください。
+右上の×をクリックして、ウィンドウを閉じましょう。
+  </t>
+    <rPh sb="114" eb="116">
+      <t>シンピン</t>
+    </rPh>
+    <rPh sb="123" eb="124">
+      <t>フン</t>
+    </rPh>
+    <rPh sb="124" eb="126">
+      <t>テイド</t>
+    </rPh>
+    <rPh sb="133" eb="135">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="136" eb="138">
+      <t>ヨユウ</t>
+    </rPh>
+    <rPh sb="161" eb="163">
+      <t>ミギウエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>デスクトップにPDFファイルのアイコンが現れたことを確認しておきます。</t>
+    <rPh sb="20" eb="21">
+      <t>アラワ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BitLocker鍵を出力したPDFをダブルクリックしてその内容を表示します。
+この内容の、「ID」と「回復キー」の両方が途切れずちゃんと読めるようにスマートフォンや携帯電話などで写真を撮っておきます。
+数日の間に必要になることはないでしょうが4年間の間、あるいは卒業後にPCが故障したりするとこのキーが必要になる場合があります。紛失した場合はこの手順を再度実施してキーを確保してください。&lt;span class="check"&gt;check 6&lt;/span&gt;</t>
+    <rPh sb="9" eb="10">
+      <t>カギ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>シュツリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「ライセンス契約に同意します」で「同意する」をクリックします。
+&lt;p class="spl"&gt;※本来は「利用許諾契約書を読む」で契約事項を読んでから同意するものです。「ファイル」→「アカウント」→「Excelのバージョン情報」と辿ればいつでも読めるので、時間のある時に読んでおいてください。&lt;/p&gt;
+これでOfficeを使用するための準備が完了しました。&lt;span class="check"&gt;check 11&lt;/span&gt;
+&lt;strong&gt;広島大学のOffice365アカウントは卒業などで学籍を失うと無くなってしまうので、Office365がインストールされたままでも卒業後は使えなくなります。&lt;/strong&gt;
+以上でこの章の作業は終了です。</t>
+    <rPh sb="6" eb="8">
+      <t>ケイヤク</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ドウイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ドウイ</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ホンライ</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>キョダク</t>
+    </rPh>
+    <rPh sb="56" eb="59">
+      <t>ケイヤクショ</t>
+    </rPh>
+    <rPh sb="60" eb="61">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>ケイヤク</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>ジコウ</t>
+    </rPh>
+    <rPh sb="69" eb="70">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>ドウイ</t>
+    </rPh>
+    <rPh sb="110" eb="112">
+      <t>ジョウホウ</t>
+    </rPh>
+    <rPh sb="114" eb="115">
+      <t>タド</t>
+    </rPh>
+    <rPh sb="121" eb="122">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="127" eb="129">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="132" eb="133">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="134" eb="135">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ログインしたら、この画面（ダッシュボード）が出ます。&lt;span class="check"&gt;check 7&lt;/span&gt;
+真ん中に見える「コースツリー」に、あなたがアクセスできるコースが表示されています。これらは、あなたの履修課目に関する授業支援や、広島大学において自習すべき教材などのコースです。（この図は在学生向けの一例で、新入生に表示されるものとは異なります）
+新入生向けに共通で表示されるものを簡単に説明すると：
+&lt;dl&gt;
+&lt;dt&gt;ノートパソコン点検届&lt;/dt&gt;
+&lt;dd&gt;あなたの必携PCが、きちんと大学で使える状態になっているか確認するため、大学に「ノートパソコン点検届」を提出する必要があります。このコースでは、点検届が提出できます。&lt;strong&gt;このテキストによる設定・点検を済ませたあと、できるだけ早くにこのコースを開いて点検届を提出してください。&lt;/strong&gt;&lt;/dd&gt;
+&lt;dt&gt;MFA設定ガイド&lt;/dt&gt;
+&lt;dd&gt;広島大学ではパスワード窃取によるアカウント乗っ取りの防止策として、広大IDを持つ全ての構成員に対しIMCアカウントおよび広大IDの多要素認証（MFA）設定を義務付けています。この「MFA設定ガイド」で、広島大学でMFA設定を行うための手順を説明しています&lt;/dd&gt; &lt;/dl&gt;
+</t>
+    <rPh sb="65" eb="66">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="111" eb="113">
+      <t>リシュウ</t>
+    </rPh>
+    <rPh sb="113" eb="115">
+      <t>カモク</t>
+    </rPh>
+    <rPh sb="116" eb="117">
+      <t>カン</t>
+    </rPh>
+    <rPh sb="119" eb="121">
+      <t>ジュギョウ</t>
+    </rPh>
+    <rPh sb="121" eb="123">
+      <t>シエン</t>
+    </rPh>
+    <rPh sb="125" eb="127">
+      <t>ヒロシマ</t>
+    </rPh>
+    <rPh sb="127" eb="129">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="133" eb="135">
+      <t>ジシュウ</t>
+    </rPh>
+    <rPh sb="138" eb="140">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="157" eb="158">
+      <t>ム</t>
+    </rPh>
+    <rPh sb="184" eb="187">
+      <t>シンニュウセイ</t>
+    </rPh>
+    <rPh sb="187" eb="188">
+      <t>ム</t>
+    </rPh>
+    <rPh sb="190" eb="192">
+      <t>キョウツウ</t>
+    </rPh>
+    <rPh sb="193" eb="195">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="340" eb="342">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="343" eb="345">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="346" eb="347">
+      <t>ス</t>
+    </rPh>
+    <rPh sb="358" eb="359">
+      <t>ハヤ</t>
+    </rPh>
+    <rPh sb="367" eb="368">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="405" eb="407">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="420" eb="424">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="431" eb="433">
+      <t>セッシュ</t>
+    </rPh>
+    <rPh sb="441" eb="442">
+      <t>ノ</t>
+    </rPh>
+    <rPh sb="443" eb="444">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="453" eb="455">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="458" eb="459">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="460" eb="461">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="463" eb="466">
+      <t>コウセイイン</t>
+    </rPh>
+    <rPh sb="467" eb="468">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="480" eb="482">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="485" eb="490">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="495" eb="497">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="498" eb="501">
+      <t>ギムヅ</t>
+    </rPh>
+    <rPh sb="513" eb="515">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="521" eb="525">
+      <t>ヒロシマダイガク</t>
+    </rPh>
+    <rPh sb="529" eb="531">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="532" eb="533">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="537" eb="539">
+      <t>テジュン</t>
+    </rPh>
+    <rPh sb="540" eb="542">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>教材の下の方にある「IMCアカウントのMFA利用設定実習」をクリックして、説明に従ってIMCアカウントの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check 8&lt;/span&gt;</t>
+    <rPh sb="0" eb="2">
+      <t>キョウザイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>セツメイ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="52" eb="57">
+      <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="65" eb="66">
+      <t>スス</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>ショウサイ</t>
+    </rPh>
+    <rPh sb="78" eb="81">
+      <t>カクコウモク</t>
+    </rPh>
+    <rPh sb="82" eb="84">
+      <t>シリョウ</t>
+    </rPh>
+    <rPh sb="85" eb="86">
+      <t>ミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">この画面になったら「接続」をクリックしてください。
+これで接続の設定が完了しました。
+接続が完了すると「接続済み」と表示されます。&lt;span class="check"&gt;check 13&lt;/span&gt;
+   </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6477,7 +6408,7 @@
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="D9" t="s">
         <v>147</v>
@@ -7272,12 +7203,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>324</v>
+        <v>343</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -7395,8 +7326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7515,7 +7446,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>325</v>
+        <v>344</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7576,7 +7507,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>326</v>
+        <v>345</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -7618,7 +7549,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>327</v>
+        <v>346</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -7696,9 +7627,9 @@
         <v>287</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="D33" t="s">
         <v>288</v>
@@ -7774,10 +7705,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43F54BA-B356-43A4-B76F-707ED0C70724}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="C18" zoomScale="118" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A18" zoomScale="118" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7953,6 +7884,11 @@
         <v>214</v>
       </c>
     </row>
+    <row r="23" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7964,8 +7900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DD8924-3FAE-44AB-A508-09E9136389D4}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8043,7 +7979,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -8111,7 +8047,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>328</v>
+        <v>349</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -8147,8 +8083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475A5B02-452F-483B-8907-D83726E9A70E}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A16" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8269,13 +8205,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8313,7 +8249,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>329</v>
+        <v>350</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -8354,7 +8290,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>330</v>
+        <v>351</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -8376,7 +8312,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -8396,8 +8332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="B15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8413,7 +8349,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8445,7 +8381,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8464,7 +8400,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -8526,7 +8462,7 @@
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="D15" t="s">
         <v>165</v>
@@ -8545,7 +8481,7 @@
     </row>
     <row r="17" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -8608,7 +8544,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -8655,7 +8591,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
@@ -8721,8 +8657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8792,7 +8728,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8814,13 +8750,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8834,7 +8770,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8842,13 +8778,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8856,13 +8792,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>333</v>
+        <v>352</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8892,7 +8828,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
test to embed YouTube video
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2025_01\fresta2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9532F1C-1FA1-4985-8B44-997CC7651307}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EE9D13-879C-4E8E-8423-68274A266367}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="21600" windowHeight="11592" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="-15096" windowWidth="21600" windowHeight="11592" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -3583,28 +3583,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Surfaceの電源を初めて入れて、デスクトップ画面が表示されるまでの設定内容について説明します。一番重要なのは、普段利用するユーザ名とパスワードを作成するところ。あとはだいたい言われるままにしていけば大丈夫です。 すでにデスクトップが表示されている方はこの章をスキップして次の「パソコンのスペック確認」へ進んでください。 Windows10はバージョン番号が同じでもバリエーションがあったり、出荷時期によって違いがあります。以下の手順にある画面の表現がテキストと少し異なったり、そもそも表示されなかったりすることもありますが、あわてないでください。</t>
-    <rPh sb="177" eb="179">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="180" eb="181">
-      <t>オナ</t>
-    </rPh>
-    <rPh sb="205" eb="206">
-      <t>チガ</t>
-    </rPh>
-    <rPh sb="224" eb="226">
-      <t>ヒョウゲン</t>
-    </rPh>
-    <rPh sb="232" eb="233">
-      <t>スコ</t>
-    </rPh>
-    <rPh sb="234" eb="235">
-      <t>コト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Googleのダウンロードページにジャンプしました。Google Chromeのブラウザ内部のデータをGoogleに送信しても良いかという許可チェックボックスがありますが、このチェックを外してダウンロードを行います。
 ※ Edgeを使って作業している場合、右上に「EdgeのほうがChromeより良いですよ」という旨の広告メッセージが出ますが、いまは無視してください。</t>
     <rPh sb="44" eb="46">
@@ -5847,6 +5825,37 @@
   <si>
     <t>ここには私物MSアカウントよりは多くのデータを置いておくことができます。
 スマホ用のOneDriveアプリもありますので、外出先でもデータを取り出すことがあれば、活用してください。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Surfaceの電源を初めて入れて、デスクトップ画面が表示されるまでの設定内容について説明します。一番重要なのは、普段利用するユーザ名とパスワードを作成するところ。あとはだいたい言われるままにしていけば大丈夫です。 すでにデスクトップが表示されている方はこの章をスキップして次の「パソコンのスペック確認」へ進んでください。 Windows10はバージョン番号が同じでもバリエーションがあったり、出荷時期によって違いがあります。以下の手順にある画面の表現がテキストと少し異なったり、そもそも表示されなかったりすることもありますが、あわてないでください。
+&lt;p&gt;
+    &lt;iframe width="640" height="360"
+            src="https://www.youtube.com/embed/bq4XJSPEoDA"
+            title="YouTube Embedding Test"
+            frameborder="3"
+            allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share"
+            referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;
+    &lt;/iframe&gt;
+&lt;/p&gt;</t>
+    <rPh sb="177" eb="179">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="180" eb="181">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="205" eb="206">
+      <t>チガ</t>
+    </rPh>
+    <rPh sb="224" eb="226">
+      <t>ヒョウゲン</t>
+    </rPh>
+    <rPh sb="232" eb="233">
+      <t>スコ</t>
+    </rPh>
+    <rPh sb="234" eb="235">
+      <t>コト</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6284,7 +6293,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6300,7 +6309,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6308,7 +6317,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6383,7 +6392,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6406,7 +6415,7 @@
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D9" t="s">
         <v>147</v>
@@ -6417,7 +6426,7 @@
         <v>231</v>
       </c>
       <c r="D10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6493,12 +6502,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -6508,7 +6517,7 @@
     </row>
     <row r="9" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D9" t="s">
         <v>69</v>
@@ -6516,7 +6525,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6524,7 +6533,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -6535,7 +6544,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -6548,7 +6557,7 @@
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D14" t="s">
         <v>162</v>
@@ -6567,12 +6576,12 @@
         <v>232</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
@@ -6598,7 +6607,7 @@
     </row>
     <row r="24" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
@@ -6821,8 +6830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -6863,15 +6872,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="187.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>238</v>
+        <v>352</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -7170,7 +7179,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
@@ -7206,7 +7215,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -7341,7 +7350,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7349,7 +7358,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7365,7 +7374,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7373,7 +7382,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7444,7 +7453,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7505,7 +7514,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -7547,7 +7556,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -7558,7 +7567,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -7566,76 +7575,76 @@
     </row>
     <row r="25" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D26" t="s">
         <v>276</v>
-      </c>
-      <c r="D26" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D28" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D29" t="s">
         <v>280</v>
-      </c>
-      <c r="D29" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D30" t="s">
         <v>282</v>
-      </c>
-      <c r="D30" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="D31" t="s">
         <v>284</v>
-      </c>
-      <c r="D31" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D32" t="s">
         <v>286</v>
-      </c>
-      <c r="D32" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D33" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
@@ -7643,7 +7652,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
@@ -7651,47 +7660,47 @@
     </row>
     <row r="38" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="D38" t="s">
         <v>291</v>
-      </c>
-      <c r="D38" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D40" t="s">
         <v>293</v>
-      </c>
-      <c r="D40" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="D41" t="s">
         <v>295</v>
-      </c>
-      <c r="D41" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="D42" t="s">
         <v>297</v>
-      </c>
-      <c r="D42" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="D43" t="s">
         <v>299</v>
-      </c>
-      <c r="D43" t="s">
-        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -7746,7 +7755,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7820,7 +7829,7 @@
     </row>
     <row r="15" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7836,7 +7845,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D17" t="s">
         <v>205</v>
@@ -7884,7 +7893,7 @@
     </row>
     <row r="23" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -7939,7 +7948,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7977,7 +7986,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -8045,7 +8054,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -8098,7 +8107,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8106,7 +8115,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8122,7 +8131,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -8133,7 +8142,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8162,7 +8171,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -8173,7 +8182,7 @@
     </row>
     <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -8184,7 +8193,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8192,7 +8201,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -8203,26 +8212,26 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>327</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D16" t="s">
         <v>147</v>
@@ -8247,13 +8256,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -8266,21 +8275,21 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8288,21 +8297,21 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D23" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8310,13 +8319,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -8330,7 +8339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -8347,7 +8356,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8371,7 +8380,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
@@ -8379,7 +8388,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8398,7 +8407,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -8417,13 +8426,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>258</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8460,7 +8469,7 @@
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D15" t="s">
         <v>165</v>
@@ -8479,7 +8488,7 @@
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -8542,13 +8551,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8556,7 +8565,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -8567,7 +8576,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8589,7 +8598,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
@@ -8612,7 +8621,7 @@
     </row>
     <row r="30" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D30" t="s" ph="1">
         <v>47</v>
@@ -8623,7 +8632,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
@@ -8696,7 +8705,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8709,7 +8718,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -8726,7 +8735,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8748,13 +8757,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8768,7 +8777,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8776,13 +8785,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8790,13 +8799,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8826,7 +8835,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
win10.xlsx: revert youtube link (for testing)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2025_01\fresta2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D37E7CD-532E-4A7A-824C-DBE7F122B962}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF6A61A-13C6-427E-AC35-BECD60CC8AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="21600" windowHeight="11592" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="353">
   <si>
     <t>header1</t>
   </si>
@@ -5843,21 +5843,9 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>chartn</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;strong&gt;※ 生協推奨PCを購入した方は、引き渡されたPCと一緒に生協から提供されたマニュアルおよび動画 に従って初期設定をを行い、このテキストは次の章（第１章）からはじめてください。(2025-01-10)&lt;/strong&gt;</t>
     <rPh sb="36" eb="38">
       <t>セイキョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>YouTube動画
-    &lt;iframe width="640" height="360"  src="https://www.youtube.com/embed/bq4XJSPEoDA" title="YouTube Embedding Test" frameborder="3" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen&gt;&lt;/iframe&gt;</t>
-    <rPh sb="7" eb="9">
-      <t>ドウガ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -5957,9 +5945,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5997,9 +5985,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6032,26 +6020,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6084,26 +6055,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6831,10 +6785,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -6894,29 +6848,35 @@
     </row>
     <row r="7" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="142.19999999999999" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s" ph="1">
+        <v>4</v>
+      </c>
       <c r="B8" s="1" t="s">
-        <v>354</v>
+        <v>235</v>
       </c>
       <c r="C8" t="s" ph="1">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s" ph="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>235</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>84</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -6924,79 +6884,79 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>57</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s" ph="1">
-        <v>4</v>
-      </c>
       <c r="B11" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" t="s" ph="1">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s" ph="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
-      <c r="D11" t="s" ph="1">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D12" t="s" ph="1">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s" ph="1">
-        <v>4</v>
-      </c>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" t="s" ph="1">
+        <v>75</v>
+      </c>
+      <c r="D14" t="s" ph="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" t="s" ph="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
-      <c r="D14" t="s" ph="1">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" t="s" ph="1">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="D16" t="s" ph="1">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -7004,137 +6964,123 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s" ph="1">
-        <v>4</v>
-      </c>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" t="s" ph="1">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s" ph="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
-      <c r="D19" t="s" ph="1">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D20" t="s" ph="1">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s" ph="1">
-        <v>4</v>
-      </c>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C22" t="s" ph="1">
+        <v>141</v>
+      </c>
+      <c r="D22" t="s" ph="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
-      <c r="D22" t="s" ph="1">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="D23" t="s" ph="1">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>142</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s" ph="1">
-        <v>4</v>
-      </c>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s" ph="1">
+        <v>4</v>
+      </c>
       <c r="B26" s="1" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s" ph="1">
-        <v>4</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" t="s" ph="1">
-        <v>7</v>
-      </c>
-      <c r="D27" t="s" ph="1">
         <v>51</v>
       </c>
     </row>

</xml_diff>

<commit_message>
win10.xlsx: replace MFA info
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF6A61A-13C6-427E-AC35-BECD60CC8AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FD4325-235C-4F4D-980A-1D38609706E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="356">
   <si>
     <t>header1</t>
   </si>
@@ -4201,105 +4201,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>さらに下の方にある「IMCアカウントのMFA設定」をクリックしてIMCアカウントのMFA設定教材を表示しましょう。</t>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="44" eb="46">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="46" eb="48">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>moodle-dashboard-ja.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-mfa-top.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-mfaimc-below.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-mfahirodai-below.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-mfa-imc.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>広大moodleの「コースツリー」の中の「MFA設定ガイド」をクリックすると、コースのトップページが表示されます。まず「コメントシート」欄に表示される説明を読んでください。</t>
-    <rPh sb="0" eb="2">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="50" eb="52">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="68" eb="69">
-      <t>ラン</t>
-    </rPh>
-    <rPh sb="70" eb="72">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="75" eb="77">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="78" eb="79">
-      <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>moodle-mfa-hirodai.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>さらに下の方にある「広大IDのMFA設定」をクリックして広大IDのMFA設定教材を表示しましょう。</t>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>ヒョウジ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -5190,50 +5092,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">教材の下の方にある「広大IDのMFA利用設定実習」をクリックして、説明に従って広大IDの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check 10&lt;/span&gt;
-</t>
-    <rPh sb="0" eb="2">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="44" eb="49">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="54" eb="56">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="57" eb="58">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="64" eb="66">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="70" eb="73">
-      <t>カクコウモク</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>シリョウ</t>
-    </rPh>
-    <rPh sb="77" eb="78">
-      <t>ミ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check 13&lt;/span&gt;
 これを「Myもみじのトップページ」と呼ぶことにしましょう。
 履修登録をしたり、成績を確認することができます。
@@ -5791,46 +5649,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>教材の下の方にある「IMCアカウントのMFA利用設定実習」をクリックして、説明に従ってIMCアカウントの多要素認証（MFA）設定を進めましょう。詳細は教材の各項目の資料を見てください。&lt;span class="check"&gt;check 8&lt;/span&gt;</t>
-    <rPh sb="0" eb="2">
-      <t>キョウザイ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ホウ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="40" eb="41">
-      <t>シタガ</t>
-    </rPh>
-    <rPh sb="52" eb="57">
-      <t>タヨウソニンショウ</t>
-    </rPh>
-    <rPh sb="62" eb="64">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="65" eb="66">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>ショウサイ</t>
-    </rPh>
-    <rPh sb="78" eb="81">
-      <t>カクコウモク</t>
-    </rPh>
-    <rPh sb="82" eb="84">
-      <t>シリョウ</t>
-    </rPh>
-    <rPh sb="85" eb="86">
-      <t>ミ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">この画面になったら「接続」をクリックしてください。
 これで接続の設定が完了しました。
 接続が完了すると「接続済み」と表示されます。&lt;span class="check"&gt;check 13&lt;/span&gt;
@@ -5847,6 +5665,166 @@
     <rPh sb="36" eb="38">
       <t>セイキョウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Webマニュアルを参照しながら広大IDのMFA設定を開始してください。</t>
+    <rPh sb="9" eb="11">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4hirodaiid/#mfa-hu-webmanu"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次の設定手順書(1)を参照しながら広大IDのMFA設定を開始してください。</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="4" eb="7">
+      <t>テジュンショ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="image96/mfa-easymanual-20230327_HIRODAIID_p1.svg"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次の設定手順書(2)を参照しながら広大IDのMFA設定を完了してください。</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="4" eb="7">
+      <t>テジュンショ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>カンリョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="image96/mfa-easymanual-20230327_HIRODAIID_p2.svg"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4imcaccount/#mfa-imcaccount-setting-web"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次の設定手順書(1)を参照しながらIMCアカウントのMFA設定を開始してください。</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="4" eb="7">
+      <t>テジュンショ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="image96/mfa-easymanual-20250225_IMCaccount_p1.svg"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次の設定手順書(2)を参照しながらIMCアカウントのMFA設定を進めしてください。</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="4" eb="7">
+      <t>テジュンショ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>スス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="image96/mfa-easymanual-20250225_IMCaccount_p2.svg"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次の設定手順書(3)を参照しながらIMCアカウントのMFA設定を完了してください。</t>
+    <rPh sb="0" eb="1">
+      <t>ツギ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="4" eb="7">
+      <t>テジュンショ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>カンリョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="image96/mfa-easymanual-20250225_IMCaccount_p3.svg"&gt;&lt;/iframe&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6250,7 +6228,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6266,7 +6244,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6274,7 +6252,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6349,7 +6327,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6372,7 +6350,7 @@
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="D9" t="s">
         <v>147</v>
@@ -6383,7 +6361,7 @@
         <v>231</v>
       </c>
       <c r="D10" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6459,7 +6437,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6533,7 +6511,7 @@
         <v>232</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6787,7 +6765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
@@ -6829,7 +6807,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.8" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6848,7 +6826,7 @@
     </row>
     <row r="7" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -7136,7 +7114,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
@@ -7172,7 +7150,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -7307,7 +7285,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7315,7 +7293,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7331,7 +7309,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7339,7 +7317,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7410,7 +7388,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7471,7 +7449,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -7513,7 +7491,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -7524,7 +7502,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -7532,76 +7510,76 @@
     </row>
     <row r="25" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="D26" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="D27" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="D28" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D29" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="D30" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="D31" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="D32" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="D33" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
@@ -7609,7 +7587,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
@@ -7617,47 +7595,47 @@
     </row>
     <row r="38" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="D38" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="5" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="D40" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="D41" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="D42" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="5" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="D43" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -7712,7 +7690,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7786,7 +7764,7 @@
     </row>
     <row r="15" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7850,7 +7828,7 @@
     </row>
     <row r="23" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -7905,7 +7883,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7943,7 +7921,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -8011,7 +7989,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -8045,10 +8023,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475A5B02-452F-483B-8907-D83726E9A70E}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8088,7 +8066,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -8099,7 +8077,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8158,7 +8136,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -8169,13 +8147,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8213,13 +8191,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -8227,62 +8205,87 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>265</v>
+    <row r="20" spans="1:4" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="5" t="s">
+        <v>343</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="D20" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>259</v>
+        <v>344</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="C21" t="s">
+        <v>129</v>
       </c>
       <c r="D21" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C22" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="C25" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" t="s">
         <v>349</v>
       </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="D23" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" t="s">
-        <v>263</v>
+    </row>
+    <row r="26" spans="1:4" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="C26" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="C27" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="C28" t="s">
+        <v>129</v>
+      </c>
+      <c r="D28" t="s">
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -8296,7 +8299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="B15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B30" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -8313,7 +8316,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8337,7 +8340,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
@@ -8345,7 +8348,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8364,7 +8367,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -8426,7 +8429,7 @@
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="D15" t="s">
         <v>165</v>
@@ -8445,7 +8448,7 @@
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -8508,7 +8511,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -8522,7 +8525,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -8533,7 +8536,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8555,7 +8558,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
@@ -8589,7 +8592,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
@@ -8662,7 +8665,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8675,7 +8678,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -8692,7 +8695,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8714,13 +8717,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8734,7 +8737,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8742,13 +8745,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8756,13 +8759,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8792,7 +8795,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
add svgs to win10/image96/
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FD4325-235C-4F4D-980A-1D38609706E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99CC6EC-2EAD-44E7-968F-498CC7F9E356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="782" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="353">
   <si>
     <t>header1</t>
   </si>
@@ -5668,26 +5668,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Webマニュアルを参照しながら広大IDのMFA設定を開始してください。</t>
-    <rPh sb="9" eb="11">
-      <t>サンショウ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>カイシ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4hirodaiid/#mfa-hu-webmanu"&gt;&lt;/iframe&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>次の設定手順書(1)を参照しながら広大IDのMFA設定を開始してください。</t>
     <rPh sb="0" eb="1">
       <t>ツギ</t>
@@ -5743,10 +5723,6 @@
   </si>
   <si>
     <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="image96/mfa-easymanual-20230327_HIRODAIID_p2.svg"&gt;&lt;/iframe&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4imcaccount/#mfa-imcaccount-setting-web"&gt;&lt;/iframe&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -8023,10 +7999,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475A5B02-452F-483B-8907-D83726E9A70E}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8227,65 +8203,43 @@
         <v>346</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="C22" t="s">
-        <v>129</v>
-      </c>
-      <c r="D22" t="s">
-        <v>348</v>
-      </c>
+    <row r="22" spans="1:4" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:4" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:4" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="C25" t="s">
         <v>129</v>
       </c>
       <c r="D25" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C26" t="s">
         <v>129</v>
       </c>
       <c r="D26" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="5" t="s">
         <v>352</v>
-      </c>
-      <c r="C27" t="s">
-        <v>129</v>
-      </c>
-      <c r="D27" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="5" t="s">
-        <v>354</v>
-      </c>
-      <c r="C28" t="s">
-        <v>129</v>
-      </c>
-      <c r="D28" t="s">
-        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -8299,7 +8253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B24" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
win10.xlsx: update MFA setting instruction to be same with win11.xlsx
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99CC6EC-2EAD-44E7-968F-498CC7F9E356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7344559-96E9-4375-A9D9-DAF8F9C09DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="782" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-77" yWindow="-77" windowWidth="19903" windowHeight="12600" tabRatio="782" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="353">
   <si>
     <t>header1</t>
   </si>
@@ -5668,139 +5668,103 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>次の設定手順書(1)を参照しながら広大IDのMFA設定を開始してください。</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
+    <t>&lt;h2 id="mfa-hirodai-id"&gt;広大IDのMFA設定&lt;/h2&gt;</t>
+    <rPh sb="24" eb="26">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="4" eb="7">
-      <t>テジュンショ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4hirodaiid/#mfa-hu-webmanu"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="mfa-imc-account"&gt;IMCアカウントのMFA設定&lt;/h2&gt;</t>
+    <rPh sb="37" eb="39">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4imcaccount/#mfa-imcaccount-setting-web"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>このPDFは広大IDのMFA設定の全体の操作の流れを説明しています。</t>
+    <rPh sb="6" eb="8">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ゼンタイ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ナガ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>chartn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2023/03/mfa-easymanual-20230327_HIRODAIID.pdf"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PDFが見づらい場合は、Webマニュアルを参照しながら広大IDのMFA設定を開始してください。</t>
+    <rPh sb="4" eb="5">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
       <t>サンショウ</t>
     </rPh>
-    <rPh sb="17" eb="19">
+    <rPh sb="27" eb="29">
       <t>ヒロダイ</t>
     </rPh>
-    <rPh sb="25" eb="27">
+    <rPh sb="35" eb="37">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="28" eb="30">
+    <rPh sb="38" eb="40">
       <t>カイシ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="image96/mfa-easymanual-20230327_HIRODAIID_p1.svg"&gt;&lt;/iframe&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>次の設定手順書(2)を参照しながら広大IDのMFA設定を完了してください。</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
+    <t>このPDFはIMCアカウントのMFA設定の全体の操作の流れを説明しています。</t>
+    <rPh sb="18" eb="20">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="4" eb="7">
-      <t>テジュンショ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>サンショウ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="25" eb="27">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>カンリョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="image96/mfa-easymanual-20230327_HIRODAIID_p2.svg"&gt;&lt;/iframe&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>次の設定手順書(1)を参照しながらIMCアカウントのMFA設定を開始してください。</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="4" eb="7">
-      <t>テジュンショ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>サンショウ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>カイシ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="image96/mfa-easymanual-20250225_IMCaccount_p1.svg"&gt;&lt;/iframe&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>次の設定手順書(2)を参照しながらIMCアカウントのMFA設定を進めしてください。</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="4" eb="7">
-      <t>テジュンショ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>サンショウ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>スス</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="image96/mfa-easymanual-20250225_IMCaccount_p2.svg"&gt;&lt;/iframe&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>次の設定手順書(3)を参照しながらIMCアカウントのMFA設定を完了してください。</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="4" eb="7">
-      <t>テジュンショ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>サンショウ</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>カンリョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="image96/mfa-easymanual-20250225_IMCaccount_p3.svg"&gt;&lt;/iframe&gt;</t>
+    <rPh sb="21" eb="23">
+      <t>ゼンタイ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ナガ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2025/02/mfa-easymanual-20250225_IMCaccount.pdf"&gt;&lt;/iframe&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5863,7 +5827,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5880,6 +5844,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7999,10 +7966,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475A5B02-452F-483B-8907-D83726E9A70E}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+      <selection activeCell="A28" sqref="A28:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8181,66 +8148,91 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="21" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="7" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" s="7" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="5" t="s">
+    <row r="23" spans="1:4" s="7" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" s="7" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="C21" t="s">
-        <v>129</v>
-      </c>
-      <c r="D21" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="1:4" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:4" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="C24" t="s">
-        <v>129</v>
-      </c>
-      <c r="D24" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="C25" t="s">
-        <v>129</v>
-      </c>
-      <c r="D25" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="7" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="D26" t="s">
-        <v>352</v>
-      </c>
+      <c r="D27" s="7" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+    </row>
+    <row r="30" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B30"/>
+    </row>
+    <row r="31" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B31"/>
+    </row>
+    <row r="32" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+    </row>
+    <row r="35" spans="2:4" customFormat="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
win10.xlsx: add the note of EOL of win10
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7344559-96E9-4375-A9D9-DAF8F9C09DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F352584-6AFA-4D4F-8F99-6F321B4560BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-77" yWindow="-77" windowWidth="19903" windowHeight="12600" tabRatio="782" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-77" yWindow="-77" windowWidth="19903" windowHeight="12600" tabRatio="782" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -2446,23 +2446,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">必携PC初期実習では、みなさんのパソコンを広島大学のキャンパスで使用するための準備をおこないます。ここでおこなうことを以下にあげます。おおむね６０分程度かかると思います。頑張ってください。
-  </t>
-    <rPh sb="4" eb="6">
-      <t>ショキ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ジッシュウ</t>
-    </rPh>
-    <rPh sb="73" eb="74">
-      <t>フン</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>テイド</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>この章からはネットワーク環境と、学生番号・広大パスワードが必要です。大学から学生番号をもらってから、作業を進めてください。</t>
     <rPh sb="2" eb="3">
       <t>ショウ</t>
@@ -5765,6 +5748,54 @@
   </si>
   <si>
     <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2025/02/mfa-easymanual-20250225_IMCaccount.pdf"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">必携PC初期実習では、みなさんのパソコンを広島大学のキャンパスで使用するための準備をおこないます。ここでおこなうことを以下にあげます。おおむね６０分程度かかると思います。頑張ってください。
+&lt;strong&gt;Windows10のサポート期間は2025年10月14日とアナウンスされています。2025年4月の時点でWindows10で初期設定を実施しても構いませんが、できるだけ速やかにWindows11へ更新し、サポート終了後にWindows10を使い続けることがないようにしてください。&lt;/strong&gt;
+  </t>
+    <rPh sb="4" eb="6">
+      <t>ショキ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ジッシュウ</t>
+    </rPh>
+    <rPh sb="73" eb="74">
+      <t>フン</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>テイド</t>
+    </rPh>
+    <rPh sb="117" eb="119">
+      <t>キカン</t>
+    </rPh>
+    <rPh sb="124" eb="125">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="127" eb="128">
+      <t>ガツ</t>
+    </rPh>
+    <rPh sb="130" eb="131">
+      <t>ニチ</t>
+    </rPh>
+    <rPh sb="148" eb="149">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="150" eb="151">
+      <t>ガツ</t>
+    </rPh>
+    <rPh sb="152" eb="154">
+      <t>ジテン</t>
+    </rPh>
+    <rPh sb="209" eb="212">
+      <t>シュウリョウゴ</t>
+    </rPh>
+    <rPh sb="223" eb="224">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="225" eb="226">
+      <t>ツヅ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6154,8 +6185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6171,7 +6202,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6187,7 +6218,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -6195,7 +6226,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -6204,12 +6235,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>176</v>
+        <v>352</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6270,7 +6301,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -6288,12 +6319,12 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D9" t="s">
         <v>147</v>
@@ -6301,10 +6332,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -6356,7 +6387,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -6364,7 +6395,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -6380,12 +6411,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -6395,7 +6426,7 @@
     </row>
     <row r="9" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D9" t="s">
         <v>69</v>
@@ -6403,7 +6434,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -6411,7 +6442,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -6422,20 +6453,20 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D13" t="s">
         <v>188</v>
-      </c>
-      <c r="D13" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D14" t="s">
         <v>162</v>
@@ -6451,25 +6482,25 @@
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -6485,7 +6516,7 @@
     </row>
     <row r="24" spans="2:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
@@ -6708,8 +6739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -6726,7 +6757,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6750,7 +6781,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.8" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -6758,7 +6789,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -6769,7 +6800,7 @@
     </row>
     <row r="7" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
@@ -6777,7 +6808,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
@@ -7033,7 +7064,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7057,7 +7088,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
@@ -7065,7 +7096,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7093,7 +7124,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -7177,7 +7208,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7191,7 +7222,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -7228,7 +7259,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7236,7 +7267,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -7252,7 +7283,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -7260,7 +7291,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7331,7 +7362,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7345,7 +7376,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -7364,7 +7395,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -7378,7 +7409,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -7392,7 +7423,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -7434,7 +7465,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -7445,7 +7476,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -7453,76 +7484,76 @@
     </row>
     <row r="25" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D26" t="s">
         <v>267</v>
-      </c>
-      <c r="D26" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D29" t="s">
         <v>271</v>
-      </c>
-      <c r="D29" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B30" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D30" t="s">
         <v>273</v>
-      </c>
-      <c r="D30" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="D31" t="s">
         <v>275</v>
-      </c>
-      <c r="D31" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D32" t="s">
         <v>277</v>
-      </c>
-      <c r="D32" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
@@ -7530,7 +7561,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
@@ -7538,47 +7569,47 @@
     </row>
     <row r="38" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="D38" t="s">
         <v>282</v>
-      </c>
-      <c r="D38" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="D40" t="s">
         <v>284</v>
-      </c>
-      <c r="D40" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D41" t="s">
         <v>286</v>
-      </c>
-      <c r="D41" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="D42" t="s">
         <v>288</v>
-      </c>
-      <c r="D42" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D43" t="s">
         <v>290</v>
-      </c>
-      <c r="D43" t="s">
-        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -7633,7 +7664,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7641,7 +7672,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -7662,42 +7693,42 @@
     </row>
     <row r="9" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D10" t="s">
         <v>191</v>
-      </c>
-      <c r="D10" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D11" t="s">
         <v>193</v>
-      </c>
-      <c r="D11" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" t="s">
         <v>195</v>
-      </c>
-      <c r="D12" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -7707,12 +7738,12 @@
     </row>
     <row r="15" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D16" t="s">
         <v>71</v>
@@ -7723,42 +7754,42 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D18" t="s">
         <v>206</v>
-      </c>
-      <c r="D18" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D19" t="s">
         <v>208</v>
-      </c>
-      <c r="D19" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D20" t="s">
         <v>210</v>
-      </c>
-      <c r="D20" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D21" t="s">
         <v>212</v>
-      </c>
-      <c r="D21" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7766,12 +7797,12 @@
         <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -7826,7 +7857,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -7845,12 +7876,12 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="132" x14ac:dyDescent="0.2">
@@ -7864,12 +7895,12 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -7877,13 +7908,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -7910,7 +7941,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -7932,7 +7963,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -7968,7 +7999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475A5B02-452F-483B-8907-D83726E9A70E}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD34"/>
     </sheetView>
   </sheetViews>
@@ -7985,7 +8016,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -7993,7 +8024,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -8009,7 +8040,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -8020,7 +8051,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8036,7 +8067,7 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -8049,7 +8080,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -8060,7 +8091,7 @@
     </row>
     <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -8071,7 +8102,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8079,7 +8110,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -8090,26 +8121,26 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>317</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D16" t="s">
         <v>147</v>
@@ -8134,13 +8165,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -8150,29 +8181,29 @@
     </row>
     <row r="20" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>348</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="7" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>129</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="7" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -8183,29 +8214,29 @@
     </row>
     <row r="25" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>351</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="7" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>129</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="28" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8262,7 +8293,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8286,7 +8317,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
@@ -8294,7 +8325,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8313,7 +8344,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -8332,26 +8363,26 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>257</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D11" t="s">
         <v>188</v>
-      </c>
-      <c r="D11" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D12" t="s">
         <v>162</v>
@@ -8359,7 +8390,7 @@
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D13" t="s">
         <v>164</v>
@@ -8367,15 +8398,15 @@
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D15" t="s">
         <v>165</v>
@@ -8383,7 +8414,7 @@
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -8394,7 +8425,7 @@
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -8405,7 +8436,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -8427,7 +8458,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -8438,7 +8469,7 @@
     </row>
     <row r="22" spans="1:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D22" t="s">
         <v>149</v>
@@ -8446,10 +8477,10 @@
     </row>
     <row r="23" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D23" t="s">
         <v>184</v>
-      </c>
-      <c r="D23" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8457,13 +8488,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -8471,7 +8502,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -8482,7 +8513,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -8490,7 +8521,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -8504,7 +8535,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
@@ -8527,7 +8558,7 @@
     </row>
     <row r="30" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D30" t="s" ph="1">
         <v>47</v>
@@ -8538,7 +8569,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
@@ -8611,12 +8642,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8624,7 +8655,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -8635,13 +8666,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8663,13 +8694,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8683,7 +8714,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8691,13 +8722,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8705,13 +8736,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8741,7 +8772,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
win10.xlsx: HU-COOP no longer sells Win10 model.
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F352584-6AFA-4D4F-8F99-6F321B4560BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210C8F16-CD4A-493C-9866-C6BB8AD3A3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-77" yWindow="-77" windowWidth="19903" windowHeight="12600" tabRatio="782" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-77" yWindow="-77" windowWidth="19903" windowHeight="12600" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="352">
   <si>
     <t>header1</t>
   </si>
@@ -5641,13 +5641,6 @@
   <si>
     <t>ここには私物MSアカウントよりは多くのデータを置いておくことができます。
 スマホ用のOneDriveアプリもありますので、外出先でもデータを取り出すことがあれば、活用してください。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;strong&gt;※ 生協推奨PCを購入した方は、引き渡されたPCと一緒に生協から提供されたマニュアルおよび動画 に従って初期設定をを行い、このテキストは次の章（第１章）からはじめてください。(2025-01-10)&lt;/strong&gt;</t>
-    <rPh sb="36" eb="38">
-      <t>セイキョウ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -6185,8 +6178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -6240,7 +6233,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6737,10 +6730,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -6798,23 +6791,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="81" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s" ph="1">
+        <v>4</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+      <c r="C7" t="s" ph="1">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s" ph="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>234</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>84</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
@@ -6822,79 +6824,79 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>57</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s" ph="1">
-        <v>4</v>
-      </c>
       <c r="B10" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C10" t="s" ph="1">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s" ph="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s" ph="1">
         <v>7</v>
       </c>
-      <c r="D10" t="s" ph="1">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D11" t="s" ph="1">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s" ph="1">
-        <v>4</v>
-      </c>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" t="s" ph="1">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s" ph="1">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" t="s" ph="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s" ph="1">
         <v>7</v>
       </c>
-      <c r="D13" t="s" ph="1">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" t="s" ph="1">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="D15" t="s" ph="1">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
@@ -6902,137 +6904,123 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="52.8" ph="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s" ph="1">
-        <v>4</v>
-      </c>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" t="s" ph="1">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s" ph="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s" ph="1">
         <v>7</v>
       </c>
-      <c r="D18" t="s" ph="1">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D19" t="s" ph="1">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s" ph="1">
-        <v>4</v>
-      </c>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C21" t="s" ph="1">
+        <v>141</v>
+      </c>
+      <c r="D21" t="s" ph="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s" ph="1">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C22" t="s" ph="1">
         <v>7</v>
       </c>
-      <c r="D21" t="s" ph="1">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="D22" t="s" ph="1">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>142</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="92.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s" ph="1">
-        <v>4</v>
-      </c>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s" ph="1">
+        <v>4</v>
+      </c>
       <c r="B25" s="1" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>7</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s" ph="1">
-        <v>4</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" t="s" ph="1">
-        <v>7</v>
-      </c>
-      <c r="D26" t="s" ph="1">
         <v>51</v>
       </c>
     </row>
@@ -8181,29 +8169,29 @@
     </row>
     <row r="20" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>347</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="7" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>129</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="7" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -8214,29 +8202,29 @@
     </row>
     <row r="25" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>350</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="7" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>129</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="28" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win10.xlsx: fix a typo (hirodai-id -> imc-account)
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCD3F53-2786-41B8-A346-9E083653C955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94D9EBB-62EE-400E-BEE4-34F9A51026A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-77" yWindow="-77" windowWidth="19903" windowHeight="12600" tabRatio="782" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="782" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="354">
   <si>
     <t>header1</t>
   </si>
@@ -5653,10 +5653,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>chartn</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2023/03/mfa-easymanual-20230327_HIRODAIID.pdf"&gt;&lt;/iframe&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -5755,6 +5751,69 @@
   </si>
   <si>
     <t>&lt;p&gt;購入したばかりの Windows 10 の電源を入れて、使い始められるようになるまでに必要な設定作業を説明します。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MFA設定が完了したかは点検届で回答が求められます。&lt;span class="check"&gt;check 11&lt;/span&gt;</t>
+    <rPh sb="3" eb="5">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>カイトウ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>モト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PDFが見づらい場合は、Webマニュアルを参照しながらIMCアカウントのMFA設定を開始してください。</t>
+    <rPh sb="4" eb="5">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MFA設定が完了したかは点検届で回答が求められます。&lt;span class="check"&gt;check 12&lt;/span&gt;</t>
+    <rPh sb="3" eb="5">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>カイトウ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>モト</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6199,7 +6258,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6698,7 +6757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6716,7 +6775,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -6865,7 +6924,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="79.2" ph="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="66" ph="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s" ph="1">
         <v>4</v>
       </c>
@@ -7951,10 +8010,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475A5B02-452F-483B-8907-D83726E9A70E}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8143,15 +8202,15 @@
         <v>344</v>
       </c>
       <c r="C21" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>345</v>
       </c>
-      <c r="D21" s="7" t="s">
+    </row>
+    <row r="22" spans="1:4" s="7" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="5" t="s">
         <v>346</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="7" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="5" t="s">
-        <v>347</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>129</v>
@@ -8160,10 +8219,12 @@
         <v>341</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="7" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:4" s="7" customFormat="1" ht="13.05" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" s="7" customFormat="1" ht="13.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="5" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="7" customFormat="1" ht="13.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -8173,18 +8234,18 @@
     </row>
     <row r="26" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="7" customFormat="1" ht="13.05" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:4" s="7" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>129</v>
@@ -8193,31 +8254,50 @@
         <v>343</v>
       </c>
     </row>
-    <row r="28" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
-    </row>
-    <row r="30" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B30"/>
+    <row r="28" spans="1:4" s="7" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
     </row>
     <row r="31" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B31"/>
     </row>
     <row r="32" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
     </row>
     <row r="33" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
     </row>
-    <row r="35" spans="2:4" customFormat="1" ph="1" x14ac:dyDescent="0.2">
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
+    <row r="34" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+    </row>
+    <row r="36" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B37"/>
+    </row>
+    <row r="41" spans="2:4" customFormat="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+    </row>
+    <row r="43" spans="2:4" customFormat="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B43"/>
+    </row>
+    <row r="44" spans="2:4" customFormat="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B44"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -8230,7 +8310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="B24" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -8555,7 +8635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
win10.xlsx: update check list number
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94D9EBB-62EE-400E-BEE4-34F9A51026A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703135E9-43ED-48AF-A1B5-FC59A72A828E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="782" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="782" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -5037,44 +5037,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check 13&lt;/span&gt;
-これを「Myもみじのトップページ」と呼ぶことにしましょう。
-履修登録をしたり、成績を確認することができます。
-また「掲示」では、授業や学部からの連絡が表示されます。  </t>
-    <rPh sb="70" eb="71">
-      <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Outlook for Webのページが開き、新着メールを確認することができます。大学からのメール連絡は広大メールに来ますので、常にメールチェックするようにしてください。&lt;span class="check"&gt;check 11&lt;/span&gt;</t>
-    <rPh sb="20" eb="21">
-      <t>ヒラ</t>
-    </rPh>
-    <rPh sb="23" eb="25">
-      <t>シンチャク</t>
-    </rPh>
-    <rPh sb="29" eb="31">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="41" eb="43">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="49" eb="51">
-      <t>レンラク</t>
-    </rPh>
-    <rPh sb="52" eb="54">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="58" eb="59">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="64" eb="65">
-      <t>ツネ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">右側にある「広大moodle」のバナーをクリックして、広島大学オンライン学習支援システムのページに進みます。
   </t>
     <rPh sb="6" eb="8">
@@ -5263,97 +5225,325 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>デスクトップにPDFファイルのアイコンが現れたことを確認しておきます。</t>
+    <rPh sb="20" eb="21">
+      <t>アラワ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ここには私物MSアカウントよりは多くのデータを置いておくことができます。
+スマホ用のOneDriveアプリもありますので、外出先でもデータを取り出すことがあれば、活用してください。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="mfa-hirodai-id"&gt;広大IDのMFA設定&lt;/h2&gt;</t>
+    <rPh sb="24" eb="26">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4hirodaiid/#mfa-hu-webmanu"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="mfa-imc-account"&gt;IMCアカウントのMFA設定&lt;/h2&gt;</t>
+    <rPh sb="37" eb="39">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4imcaccount/#mfa-imcaccount-setting-web"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>このPDFは広大IDのMFA設定の全体の操作の流れを説明しています。</t>
+    <rPh sb="6" eb="8">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ゼンタイ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ナガ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2023/03/mfa-easymanual-20230327_HIRODAIID.pdf"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PDFが見づらい場合は、Webマニュアルを参照しながら広大IDのMFA設定を開始してください。</t>
+    <rPh sb="4" eb="5">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>このPDFはIMCアカウントのMFA設定の全体の操作の流れを説明しています。</t>
+    <rPh sb="18" eb="20">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ゼンタイ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ナガ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2025/02/mfa-easymanual-20250225_IMCaccount.pdf"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">必携PC初期実習では、みなさんのパソコンを広島大学のキャンパスで使用するための準備をおこないます。ここでおこなうことを以下にあげます。おおむね６０分程度かかると思います。頑張ってください。
+&lt;strong&gt;Windows10のサポート期間は2025年10月14日とアナウンスされています。2025年4月の時点でWindows10で初期設定を実施しても構いませんが、できるだけ速やかにWindows11へ更新し、サポート終了後にWindows10を使い続けることがないようにしてください。&lt;/strong&gt;
+  </t>
+    <rPh sb="4" eb="6">
+      <t>ショキ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>ジッシュウ</t>
+    </rPh>
+    <rPh sb="73" eb="74">
+      <t>フン</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>テイド</t>
+    </rPh>
+    <rPh sb="117" eb="119">
+      <t>キカン</t>
+    </rPh>
+    <rPh sb="124" eb="125">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="127" eb="128">
+      <t>ガツ</t>
+    </rPh>
+    <rPh sb="130" eb="131">
+      <t>ニチ</t>
+    </rPh>
+    <rPh sb="148" eb="149">
+      <t>ネン</t>
+    </rPh>
+    <rPh sb="150" eb="151">
+      <t>ガツ</t>
+    </rPh>
+    <rPh sb="152" eb="154">
+      <t>ジテン</t>
+    </rPh>
+    <rPh sb="209" eb="212">
+      <t>シュウリョウゴ</t>
+    </rPh>
+    <rPh sb="223" eb="224">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="225" eb="226">
+      <t>ツヅ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;p&gt;購入したばかりの Windows 10 の電源を入れて、使い始められるようになるまでに必要な設定作業を説明します。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MFA設定が完了したかは点検届で回答が求められます。&lt;span class="check"&gt;check 11&lt;/span&gt;</t>
+    <rPh sb="3" eb="5">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>カイトウ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>モト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PDFが見づらい場合は、Webマニュアルを参照しながらIMCアカウントのMFA設定を開始してください。</t>
+    <rPh sb="4" eb="5">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MFA設定が完了したかは点検届で回答が求められます。&lt;span class="check"&gt;check 12&lt;/span&gt;</t>
+    <rPh sb="3" eb="5">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>テンケン</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>トドケ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>カイトウ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>モト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t xml:space="preserve">ウィルス対策ソフトのDefenderを含めて、Windows基本システムは定期的に自動更新されます。
-このウィンドウの上の方で更新状況が確認できます。&lt;span class="check"&gt;check 2&lt;/span&gt;&lt;span class="check"&gt;check 4&lt;/span&gt;
+このウィンドウの上の方で更新状況が確認できます。
+&lt;span class="check"&gt;check 4&lt;/span&gt;
+&lt;span class="check"&gt;check 5&lt;/span&gt;
 さらに、Officeも自動更新するように設定しましょう。「詳細オプション」をクリックしてください。
   </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t xml:space="preserve">Defenderでは、ウイルスやスパイウェアその他の悪意を持つプログラム全般を「脅威」とし、それらを判別するルールを保存したファイルを「脅威の定義」と呼んでいます。
-「ウイルスと脅威の防止の更新」の下に、前回いつ「脅威の定義」が更新されたかが書かれています。&lt;span class="check"&gt;check 3&lt;/span&gt;&lt;span class="check"&gt;check 4&lt;/span&gt;
+「ウイルスと脅威の防止の更新」の下に、前回いつ「脅威の定義」が更新されたかが書かれています。
 &lt;p class="spl"&gt;※ここで「他のプログラム（ウィルスバスター、マカフィーリブセーフなど）が有効になっている」という旨の表示がされた場合、ウィルス対策はその表示されたプログラムが行っています。その場合はこの下の項目は飛ばして、別途そのプログラムの「利用期限」と「更新方法」「フルスキャンの実施方法」を確認してください。とくに「利用期限」が切れてウィルス対策に穴ができることがないよう注意してください。あとで Defender の利用に戻すこともできます。&lt;/p&gt;
 脅威の定義を新しくするには「ウイルスと脅威の防止の更新」をクリックします。
   </t>
-    <rPh sb="248" eb="250">
+    <rPh sb="180" eb="182">
       <t>ユウコウ</t>
     </rPh>
-    <rPh sb="260" eb="261">
+    <rPh sb="192" eb="193">
       <t>ムネ</t>
     </rPh>
-    <rPh sb="275" eb="277">
+    <rPh sb="207" eb="209">
       <t>タイサク</t>
     </rPh>
+    <rPh sb="212" eb="214">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="223" eb="224">
+      <t>オコナ</t>
+    </rPh>
+    <rPh sb="232" eb="234">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="237" eb="238">
+      <t>シタ</t>
+    </rPh>
+    <rPh sb="239" eb="241">
+      <t>コウモク</t>
+    </rPh>
+    <rPh sb="242" eb="243">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="247" eb="249">
+      <t>ベット</t>
+    </rPh>
+    <rPh sb="258" eb="260">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="260" eb="262">
+      <t>キゲン</t>
+    </rPh>
+    <rPh sb="265" eb="267">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="267" eb="269">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="278" eb="280">
+      <t>ジッシ</t>
+    </rPh>
     <rPh sb="280" eb="282">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="291" eb="292">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="300" eb="302">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="305" eb="306">
-      <t>シタ</t>
-    </rPh>
-    <rPh sb="307" eb="309">
-      <t>コウモク</t>
-    </rPh>
-    <rPh sb="310" eb="311">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="315" eb="317">
-      <t>ベット</t>
-    </rPh>
-    <rPh sb="326" eb="328">
+      <t>ホウホウ</t>
+    </rPh>
+    <rPh sb="284" eb="286">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="297" eb="299">
       <t>リヨウ</t>
     </rPh>
-    <rPh sb="328" eb="330">
+    <rPh sb="299" eb="301">
       <t>キゲン</t>
     </rPh>
-    <rPh sb="333" eb="335">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="335" eb="337">
-      <t>ホウホウ</t>
-    </rPh>
-    <rPh sb="346" eb="348">
-      <t>ジッシ</t>
+    <rPh sb="303" eb="304">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="310" eb="312">
+      <t>タイサク</t>
+    </rPh>
+    <rPh sb="313" eb="314">
+      <t>アナ</t>
+    </rPh>
+    <rPh sb="325" eb="327">
+      <t>チュウイ</t>
     </rPh>
     <rPh sb="348" eb="350">
-      <t>ホウホウ</t>
-    </rPh>
-    <rPh sb="352" eb="354">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="365" eb="367">
       <t>リヨウ</t>
     </rPh>
-    <rPh sb="367" eb="369">
-      <t>キゲン</t>
-    </rPh>
-    <rPh sb="371" eb="372">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="378" eb="380">
-      <t>タイサク</t>
-    </rPh>
-    <rPh sb="381" eb="382">
-      <t>アナ</t>
-    </rPh>
-    <rPh sb="393" eb="395">
-      <t>チュウイ</t>
-    </rPh>
-    <rPh sb="416" eb="418">
-      <t>リヨウ</t>
-    </rPh>
-    <rPh sb="419" eb="420">
+    <rPh sb="351" eb="352">
       <t>モド</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">三種類の高度なスキャンがありますね。「フルスキャン」を選んで下の「今すぐスキャン」ボタンを押すと、フルスキャンが実施されます。&lt;span class="check"&gt;check 5&lt;/span&gt;
+    <t xml:space="preserve">三種類の高度なスキャンがありますね。「フルスキャン」を選んで下の「今すぐスキャン」ボタンを押すと、フルスキャンが実施されます。&lt;span class="check"&gt;check 6&lt;/span&gt;
 フルスキャンの実施には数時間（新品のPCでも３０分程度）かかります。時間の余裕のあるときにできるだけ早く実施してください。
 右上の×をクリックして、ウィンドウを閉じましょう。
   </t>
@@ -5378,19 +5568,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>デスクトップにPDFファイルのアイコンが現れたことを確認しておきます。</t>
-    <rPh sb="20" eb="21">
-      <t>アラワ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>カクニン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>BitLocker鍵を出力したPDFをダブルクリックしてその内容を表示します。
 この内容の、「ID」と「回復キー」の両方が途切れずちゃんと読めるようにスマートフォンや携帯電話などで写真を撮っておきます。
-数日の間に必要になることはないでしょうが4年間の間、あるいは卒業後にPCが故障したりするとこのキーが必要になる場合があります。紛失した場合はこの手順を再度実施してキーを確保してください。&lt;span class="check"&gt;check 6&lt;/span&gt;</t>
+数日の間に必要になることはないでしょうが4年間の間、あるいは卒業後にPCが故障したりするとこのキーが必要になる場合があります。紛失した場合はこの手順を再度実施してキーを確保してください。
+&lt;span class="check"&gt;check 3&lt;/span&gt;</t>
     <rPh sb="9" eb="10">
       <t>カギ</t>
     </rPh>
@@ -5402,7 +5583,7 @@
   <si>
     <t>「ライセンス契約に同意します」で「同意する」をクリックします。
 &lt;p class="spl"&gt;※本来は「利用許諾契約書を読む」で契約事項を読んでから同意するものです。「ファイル」→「アカウント」→「Excelのバージョン情報」と辿ればいつでも読めるので、時間のある時に読んでおいてください。&lt;/p&gt;
-これでOfficeを使用するための準備が完了しました。&lt;span class="check"&gt;check 11&lt;/span&gt;
+これでOfficeを使用するための準備が完了しました。&lt;span class="check"&gt;check 9&lt;/span&gt;
 &lt;strong&gt;広島大学のOffice365アカウントは卒業などで学籍を失うと無くなってしまうので、Office365がインストールされたままでも卒業後は使えなくなります。&lt;/strong&gt;
 以上でこの章の作業は終了です。</t>
     <rPh sb="6" eb="8">
@@ -5462,7 +5643,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">ログインしたら、この画面（ダッシュボード）が出ます。&lt;span class="check"&gt;check 7&lt;/span&gt;
+    <t xml:space="preserve">ログインしたら、この画面（ダッシュボード）が出ます。
 真ん中に見える「コースツリー」に、あなたがアクセスできるコースが表示されています。これらは、あなたの履修課目に関する授業支援や、広島大学において自習すべき教材などのコースです。（この図は在学生向けの一例で、新入生に表示されるものとは異なります）
 新入生向けに共通で表示されるものを簡単に説明すると：
 &lt;dl&gt;
@@ -5471,349 +5652,171 @@
 &lt;dt&gt;MFA設定ガイド&lt;/dt&gt;
 &lt;dd&gt;広島大学ではパスワード窃取によるアカウント乗っ取りの防止策として、広大IDを持つ全ての構成員に対しIMCアカウントおよび広大IDの多要素認証（MFA）設定を義務付けています。この「MFA設定ガイド」で、広島大学でMFA設定を行うための手順を説明しています&lt;/dd&gt; &lt;/dl&gt;
 </t>
-    <rPh sb="65" eb="66">
+    <rPh sb="31" eb="32">
       <t>ミ</t>
     </rPh>
-    <rPh sb="111" eb="113">
+    <rPh sb="77" eb="79">
       <t>リシュウ</t>
     </rPh>
-    <rPh sb="113" eb="115">
+    <rPh sb="79" eb="81">
       <t>カモク</t>
     </rPh>
-    <rPh sb="116" eb="117">
+    <rPh sb="82" eb="83">
       <t>カン</t>
     </rPh>
-    <rPh sb="119" eb="121">
+    <rPh sb="85" eb="87">
       <t>ジュギョウ</t>
     </rPh>
-    <rPh sb="121" eb="123">
+    <rPh sb="87" eb="89">
       <t>シエン</t>
     </rPh>
-    <rPh sb="125" eb="127">
+    <rPh sb="91" eb="93">
       <t>ヒロシマ</t>
     </rPh>
-    <rPh sb="127" eb="129">
+    <rPh sb="93" eb="95">
       <t>ダイガク</t>
     </rPh>
-    <rPh sb="133" eb="135">
+    <rPh sb="99" eb="101">
       <t>ジシュウ</t>
     </rPh>
-    <rPh sb="138" eb="140">
+    <rPh sb="104" eb="106">
       <t>キョウザイ</t>
     </rPh>
-    <rPh sb="157" eb="158">
+    <rPh sb="123" eb="124">
       <t>ム</t>
     </rPh>
-    <rPh sb="184" eb="187">
+    <rPh sb="150" eb="153">
       <t>シンニュウセイ</t>
     </rPh>
-    <rPh sb="187" eb="188">
+    <rPh sb="153" eb="154">
       <t>ム</t>
     </rPh>
-    <rPh sb="190" eb="192">
+    <rPh sb="156" eb="158">
       <t>キョウツウ</t>
     </rPh>
-    <rPh sb="193" eb="195">
+    <rPh sb="159" eb="161">
       <t>ヒョウジ</t>
     </rPh>
-    <rPh sb="340" eb="342">
+    <rPh sb="306" eb="308">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="343" eb="345">
+    <rPh sb="309" eb="311">
       <t>テンケン</t>
     </rPh>
-    <rPh sb="346" eb="347">
+    <rPh sb="312" eb="313">
       <t>ス</t>
     </rPh>
-    <rPh sb="358" eb="359">
+    <rPh sb="324" eb="325">
       <t>ハヤ</t>
     </rPh>
-    <rPh sb="367" eb="368">
+    <rPh sb="333" eb="334">
       <t>ヒラ</t>
     </rPh>
-    <rPh sb="405" eb="407">
+    <rPh sb="371" eb="373">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="420" eb="424">
+    <rPh sb="386" eb="390">
       <t>ヒロシマダイガク</t>
     </rPh>
-    <rPh sb="431" eb="433">
+    <rPh sb="397" eb="399">
       <t>セッシュ</t>
     </rPh>
-    <rPh sb="441" eb="442">
+    <rPh sb="407" eb="408">
       <t>ノ</t>
     </rPh>
-    <rPh sb="443" eb="444">
+    <rPh sb="409" eb="410">
       <t>ト</t>
     </rPh>
-    <rPh sb="453" eb="455">
+    <rPh sb="419" eb="421">
       <t>ヒロダイ</t>
     </rPh>
-    <rPh sb="458" eb="459">
+    <rPh sb="424" eb="425">
       <t>モ</t>
     </rPh>
-    <rPh sb="460" eb="461">
+    <rPh sb="426" eb="427">
       <t>スベ</t>
     </rPh>
-    <rPh sb="463" eb="466">
+    <rPh sb="429" eb="432">
       <t>コウセイイン</t>
     </rPh>
-    <rPh sb="467" eb="468">
+    <rPh sb="433" eb="434">
       <t>タイ</t>
     </rPh>
-    <rPh sb="480" eb="482">
+    <rPh sb="446" eb="448">
       <t>ヒロダイ</t>
     </rPh>
-    <rPh sb="485" eb="490">
+    <rPh sb="451" eb="456">
       <t>タヨウソニンショウ</t>
+    </rPh>
+    <rPh sb="461" eb="463">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="464" eb="467">
+      <t>ギムヅ</t>
+    </rPh>
+    <rPh sb="479" eb="481">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="487" eb="491">
+      <t>ヒロシマダイガク</t>
     </rPh>
     <rPh sb="495" eb="497">
       <t>セッテイ</t>
     </rPh>
-    <rPh sb="498" eb="501">
-      <t>ギムヅ</t>
-    </rPh>
-    <rPh sb="513" eb="515">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="521" eb="525">
-      <t>ヒロシマダイガク</t>
-    </rPh>
-    <rPh sb="529" eb="531">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="532" eb="533">
+    <rPh sb="498" eb="499">
       <t>オコナ</t>
     </rPh>
-    <rPh sb="537" eb="539">
+    <rPh sb="503" eb="505">
       <t>テジュン</t>
     </rPh>
-    <rPh sb="540" eb="542">
+    <rPh sb="506" eb="508">
       <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Outlook for Webのページが開き、新着メールを確認することができます。大学からのメール連絡は広大メールに来ますので、常にメールチェックするようにしてください。&lt;span class="check"&gt;check 8&lt;/span&gt;</t>
+    <rPh sb="20" eb="21">
+      <t>ヒラ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>シンチャク</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ダイガク</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>レンラク</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>ヒロダイ</t>
+    </rPh>
+    <rPh sb="58" eb="59">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>ツネ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">するとこのような画面になります。&lt;span class="check"&gt;check 7&lt;/span&gt;
+これを「Myもみじのトップページ」と呼ぶことにしましょう。
+履修登録をしたり、成績を確認することができます。
+また「掲示」では、授業や学部からの連絡が表示されます。  </t>
+    <rPh sb="69" eb="70">
+      <t>ヨ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t xml:space="preserve">この画面になったら「接続」をクリックしてください。
 これで接続の設定が完了しました。
-接続が完了すると「接続済み」と表示されます。&lt;span class="check"&gt;check 13&lt;/span&gt;
+接続が完了すると「接続済み」と表示されます。&lt;span class="check"&gt;check 10&lt;/span&gt;
    </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ここには私物MSアカウントよりは多くのデータを置いておくことができます。
-スマホ用のOneDriveアプリもありますので、外出先でもデータを取り出すことがあれば、活用してください。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h2 id="mfa-hirodai-id"&gt;広大IDのMFA設定&lt;/h2&gt;</t>
-    <rPh sb="24" eb="26">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4hirodaiid/#mfa-hu-webmanu"&gt;&lt;/iframe&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;h2 id="mfa-imc-account"&gt;IMCアカウントのMFA設定&lt;/h2&gt;</t>
-    <rPh sb="37" eb="39">
-      <t>セッテイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="400px" src="https://www.media.hiroshima-u.ac.jp/services/mfa/mfa4imcaccount/#mfa-imcaccount-setting-web"&gt;&lt;/iframe&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>このPDFは広大IDのMFA設定の全体の操作の流れを説明しています。</t>
-    <rPh sb="6" eb="8">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>ゼンタイ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ソウサ</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>ナガ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>セツメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2023/03/mfa-easymanual-20230327_HIRODAIID.pdf"&gt;&lt;/iframe&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PDFが見づらい場合は、Webマニュアルを参照しながら広大IDのMFA設定を開始してください。</t>
-    <rPh sb="4" eb="5">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>サンショウ</t>
-    </rPh>
-    <rPh sb="27" eb="29">
-      <t>ヒロダイ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>カイシ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>このPDFはIMCアカウントのMFA設定の全体の操作の流れを説明しています。</t>
-    <rPh sb="18" eb="20">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ゼンタイ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>ソウサ</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>ナガ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>セツメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2025/02/mfa-easymanual-20250225_IMCaccount.pdf"&gt;&lt;/iframe&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">必携PC初期実習では、みなさんのパソコンを広島大学のキャンパスで使用するための準備をおこないます。ここでおこなうことを以下にあげます。おおむね６０分程度かかると思います。頑張ってください。
-&lt;strong&gt;Windows10のサポート期間は2025年10月14日とアナウンスされています。2025年4月の時点でWindows10で初期設定を実施しても構いませんが、できるだけ速やかにWindows11へ更新し、サポート終了後にWindows10を使い続けることがないようにしてください。&lt;/strong&gt;
-  </t>
-    <rPh sb="4" eb="6">
-      <t>ショキ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ジッシュウ</t>
-    </rPh>
-    <rPh sb="73" eb="74">
-      <t>フン</t>
-    </rPh>
-    <rPh sb="74" eb="76">
-      <t>テイド</t>
-    </rPh>
-    <rPh sb="117" eb="119">
-      <t>キカン</t>
-    </rPh>
-    <rPh sb="124" eb="125">
-      <t>ネン</t>
-    </rPh>
-    <rPh sb="127" eb="128">
-      <t>ガツ</t>
-    </rPh>
-    <rPh sb="130" eb="131">
-      <t>ニチ</t>
-    </rPh>
-    <rPh sb="148" eb="149">
-      <t>ネン</t>
-    </rPh>
-    <rPh sb="150" eb="151">
-      <t>ガツ</t>
-    </rPh>
-    <rPh sb="152" eb="154">
-      <t>ジテン</t>
-    </rPh>
-    <rPh sb="209" eb="212">
-      <t>シュウリョウゴ</t>
-    </rPh>
-    <rPh sb="223" eb="224">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="225" eb="226">
-      <t>ツヅ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>&lt;p&gt;購入したばかりの Windows 10 の電源を入れて、使い始められるようになるまでに必要な設定作業を説明します。</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>MFA設定が完了したかは点検届で回答が求められます。&lt;span class="check"&gt;check 11&lt;/span&gt;</t>
-    <rPh sb="3" eb="5">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>カンリョウ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>テンケン</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>トドケ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>カイトウ</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>モト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PDFが見づらい場合は、Webマニュアルを参照しながらIMCアカウントのMFA設定を開始してください。</t>
-    <rPh sb="4" eb="5">
-      <t>ミ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>バアイ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>サンショウ</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="42" eb="44">
-      <t>カイシ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>MFA設定が完了したかは点検届で回答が求められます。&lt;span class="check"&gt;check 12&lt;/span&gt;</t>
-    <rPh sb="3" eb="5">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>カンリョウ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>テンケン</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>トドケ</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>カイトウ</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>モト</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6258,7 +6261,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -6342,7 +6345,7 @@
     </row>
     <row r="9" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D9" t="s">
         <v>147</v>
@@ -6775,7 +6778,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -7060,7 +7063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -7137,7 +7140,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -7255,8 +7258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7370,12 +7373,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>331</v>
+        <v>345</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -7431,12 +7434,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="132" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>332</v>
+        <v>346</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -7478,7 +7481,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>333</v>
+        <v>347</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -7558,7 +7561,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D33" t="s">
         <v>277</v>
@@ -7636,7 +7639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43F54BA-B356-43A4-B76F-707ED0C70724}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="118" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="118" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -7815,7 +7818,7 @@
     </row>
     <row r="23" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>335</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -7829,8 +7832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DD8924-3FAE-44AB-A508-09E9136389D4}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7908,7 +7911,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -7976,7 +7979,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
@@ -8012,8 +8015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475A5B02-452F-483B-8907-D83726E9A70E}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A18" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8134,13 +8137,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -8178,7 +8181,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>337</v>
+        <v>350</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -8194,34 +8197,34 @@
     </row>
     <row r="20" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>129</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="7" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="5" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>129</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="7" customFormat="1" ht="13.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="7" customFormat="1" ht="13.2" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -8229,34 +8232,34 @@
     </row>
     <row r="25" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>129</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="7" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>129</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="7" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="5" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
     </row>
     <row r="29" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
@@ -8310,8 +8313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="B18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8327,7 +8330,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -8359,7 +8362,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -8378,7 +8381,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -8440,7 +8443,7 @@
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>314</v>
+        <v>351</v>
       </c>
       <c r="D15" t="s">
         <v>165</v>
@@ -8459,7 +8462,7 @@
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -8522,7 +8525,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>313</v>
+        <v>352</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -8569,7 +8572,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
@@ -8635,8 +8638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="B15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8706,7 +8709,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8728,13 +8731,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8748,7 +8751,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -8756,13 +8759,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>323</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -8770,13 +8773,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>338</v>
+        <v>353</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -8806,7 +8809,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
win10.xlsx: fix for printer
</commit_message>
<xml_diff>
--- a/win10.xlsx
+++ b/win10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7FC93B-08C8-4A54-9CA7-B0AF94355C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DA341F-97BA-4D77-AEC2-C31B82686CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="782" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15576" windowHeight="11784" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -6281,8 +6281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02489F37-694A-4583-9CE4-9D6A1DDB1F5F}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -7258,8 +7258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8313,8 +8313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638EE2BE-B56D-442A-95BC-70A644A8F67B}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="B18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -8638,8 +8638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="B15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>

</xml_diff>